<commit_message>
Add: RS for Info Messafge
#1

+ 공지 메세지 관련 RS 작성
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B8E8BA-8415-40B3-B045-62E4FF168D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4ED294-97FC-47EB-ABB5-CFF382F5EC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10185" yWindow="0" windowWidth="17850" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10185" yWindow="1545" windowWidth="17850" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,23 +139,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>에러 텍스트 출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FR-U-A-02</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>화면 비례 길이 최소 단위 계산</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FR-U-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게임 오브젝트 화면 비례 사이즈 반응형</t>
+    <t>공지 메시지 = 시스템 메시지 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임 오브젝트 수직/수평 으로 입력한 거리만큼 일정/가속 속도로 이동</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -211,10 +203,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -495,34 +488,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q28"/>
+  <dimension ref="B2:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="P3" t="s">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="S3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" t="s">
+      <c r="S4" s="1"/>
+      <c r="T4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -541,12 +534,12 @@
       <c r="I5" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" t="s">
+      <c r="S5" s="2"/>
+      <c r="T5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -566,12 +559,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -587,11 +580,11 @@
       <c r="J12" t="s">
         <v>15</v>
       </c>
-      <c r="P12" t="s">
+      <c r="S12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -604,21 +597,15 @@
       <c r="J13" t="s">
         <v>17</v>
       </c>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="S13" s="2"/>
+    </row>
+    <row r="22" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="H22" t="s">
-        <v>31</v>
-      </c>
-      <c r="J22" t="s">
-        <v>30</v>
-      </c>
-      <c r="P22" s="2"/>
-    </row>
-    <row r="25" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="S22" s="3"/>
+    </row>
+    <row r="25" spans="4:19" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
         <v>18</v>
       </c>
@@ -628,27 +615,28 @@
       <c r="J25" t="s">
         <v>21</v>
       </c>
-      <c r="P25" s="2"/>
-    </row>
-    <row r="26" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H26" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" t="s">
+        <v>30</v>
+      </c>
+      <c r="S26" s="2"/>
+    </row>
+    <row r="30" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30" t="s">
         <v>29</v>
       </c>
-      <c r="J26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="F28" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" t="s">
-        <v>27</v>
-      </c>
-      <c r="J28" t="s">
-        <v>28</v>
-      </c>
-      <c r="P28" s="2"/>
+      <c r="S30" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Docs: Modification for Object Animation
#1

+ 오브젝트 Fade in/out을 static 함수로 변경
+ 공지 메세지 관련 기능
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4ED294-97FC-47EB-ABB5-CFF382F5EC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBE8D5F-CF2C-4595-9F21-F3574FE9F58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10185" yWindow="1545" windowWidth="17850" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10395" yWindow="1290" windowWidth="17850" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -111,10 +111,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>로딩을 위한 화면 Fade In/out</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Implementation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -148,6 +144,18 @@
   </si>
   <si>
     <t>게임 오브젝트 수직/수평 으로 입력한 거리만큼 일정/가속 속도로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-T-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지 메시지 출력 사이클</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임 오브젝트 Fade in/out</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -203,11 +211,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -488,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:T30"/>
+  <dimension ref="B2:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -503,7 +510,7 @@
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
@@ -512,7 +519,7 @@
       </c>
       <c r="S4" s="1"/>
       <c r="T4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
@@ -536,7 +543,7 @@
       </c>
       <c r="S5" s="2"/>
       <c r="T5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
@@ -553,10 +560,10 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
         <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
@@ -581,7 +588,7 @@
         <v>15</v>
       </c>
       <c r="S12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
@@ -603,7 +610,6 @@
       <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="S22" s="3"/>
     </row>
     <row r="25" spans="4:19" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
@@ -613,30 +619,39 @@
         <v>20</v>
       </c>
       <c r="J25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S25" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="S25" s="2"/>
     </row>
     <row r="26" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S26" s="2"/>
     </row>
     <row r="30" spans="4:19" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S30" s="2"/>
+    </row>
+    <row r="31" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>30</v>
+      </c>
+      <c r="J31" t="s">
+        <v>31</v>
+      </c>
+      <c r="S31" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Docs: Synchronizing RS with Actual
#1

~ 변경된 내용에 맞춰 FR 수정
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBE8D5F-CF2C-4595-9F21-F3574FE9F58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992F0432-7108-4781-9BAA-766A4294B717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10395" yWindow="1290" windowWidth="17850" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,10 +103,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>애니메이션</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FR-U-A-01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -127,10 +123,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>텍스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FR-U-T-01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -156,6 +148,38 @@
   </si>
   <si>
     <t>게임 오브젝트 Fade in/out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Animation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>애니메이션 관련</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -179,7 +203,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,8 +222,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -207,14 +237,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -495,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:T31"/>
+  <dimension ref="B2:T65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -510,7 +599,7 @@
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
@@ -519,7 +608,7 @@
       </c>
       <c r="S4" s="1"/>
       <c r="T4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
@@ -533,17 +622,23 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
@@ -557,101 +652,1203 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
         <v>10</v>
       </c>
       <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T12" s="7"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="4"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B21" s="4"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B23" s="4"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="4"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B24" s="4"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="4"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B25" s="4"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B26" s="4"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B27" s="4"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B28" s="4"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B29" s="4"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B30" s="4"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B31" s="4"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B32" s="4"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B33" s="4"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B34" s="4"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B35" s="4"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B37" s="4"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" t="s">
-        <v>15</v>
-      </c>
-      <c r="S12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" t="s">
-        <v>17</v>
-      </c>
-      <c r="S13" s="2"/>
-    </row>
-    <row r="22" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="F25" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" t="s">
-        <v>32</v>
-      </c>
-      <c r="S25" s="2"/>
-    </row>
-    <row r="26" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="H26" t="s">
-        <v>27</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="I37" s="3"/>
+      <c r="J37" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="4"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B38" s="4"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S26" s="2"/>
-    </row>
-    <row r="30" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="F30" t="s">
-        <v>24</v>
-      </c>
-      <c r="H30" t="s">
-        <v>26</v>
-      </c>
-      <c r="J30" t="s">
-        <v>28</v>
-      </c>
-      <c r="S30" s="2"/>
-    </row>
-    <row r="31" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="H31" t="s">
-        <v>30</v>
-      </c>
-      <c r="J31" t="s">
-        <v>31</v>
-      </c>
-      <c r="S31" s="2"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="4"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B39" s="4"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B40" s="4"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B41" s="4"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B42" s="4"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B43" s="4"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B44" s="4"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B45" s="4"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B46" s="4"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B47" s="4"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B48" s="4"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+    </row>
+    <row r="49" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B49" s="4"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B50" s="4"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+    </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B51" s="4"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B52" s="4"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+    </row>
+    <row r="53" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B53" s="4"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="4"/>
+    </row>
+    <row r="54" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B54" s="4"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+    </row>
+    <row r="55" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B55" s="4"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B56" s="4"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+    </row>
+    <row r="57" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B57" s="4"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+    </row>
+    <row r="58" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B58" s="4"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+    </row>
+    <row r="59" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B59" s="4"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="4"/>
+    </row>
+    <row r="60" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B60" s="4"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+    </row>
+    <row r="61" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B61" s="4"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="4"/>
+    </row>
+    <row r="62" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B62" s="4"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+    </row>
+    <row r="63" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B63" s="4"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="4"/>
+      <c r="M63" s="4"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="4"/>
+      <c r="P63" s="4"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="4"/>
+    </row>
+    <row r="64" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B64" s="4"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="4"/>
+      <c r="T64" s="4"/>
+    </row>
+    <row r="65" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B65" s="4"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4"/>
+      <c r="P65" s="4"/>
+      <c r="Q65" s="4"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="4"/>
+      <c r="T65" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Docs: #5 Update RS for Mouse Event Manager
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992F0432-7108-4781-9BAA-766A4294B717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6A4DB5-00B3-4E3B-8EDE-EF996CAE1B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10395" yWindow="1290" windowWidth="17850" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6615" yWindow="0" windowWidth="20445" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,14 +63,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>U</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI 관련</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Category 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -103,10 +95,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FR-U-A-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Implementation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -123,14 +111,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FR-U-T-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FR-U-A-02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공지 메시지 = 시스템 메시지 출력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -139,10 +119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FR-U-T-02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공지 메시지 출력 사이클</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -155,10 +131,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>N</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -180,6 +152,42 @@
   </si>
   <si>
     <t>애니메이션 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>광역 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-A-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-A-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-T-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-T-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마우스 이벤트 메니저</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -299,7 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -587,7 +595,7 @@
   <dimension ref="B2:T65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -599,7 +607,7 @@
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
@@ -608,7 +616,7 @@
       </c>
       <c r="S4" s="1"/>
       <c r="T4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
@@ -622,23 +630,23 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
@@ -649,22 +657,22 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="J6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
@@ -674,23 +682,23 @@
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -701,7 +709,7 @@
       <c r="Q12" s="7"/>
       <c r="R12" s="8"/>
       <c r="S12" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="T12" s="7"/>
     </row>
@@ -717,11 +725,11 @@
       <c r="F13" s="4"/>
       <c r="G13" s="3"/>
       <c r="H13" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -731,7 +739,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="2"/>
+      <c r="S13" s="1"/>
       <c r="T13" s="4"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.3">
@@ -927,19 +935,17 @@
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="F23" s="4"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -949,7 +955,7 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="3"/>
-      <c r="S23" s="1"/>
+      <c r="S23" s="2"/>
       <c r="T23" s="4"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.3">
@@ -959,13 +965,9 @@
       <c r="E24" s="3"/>
       <c r="F24" s="4"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="H24" s="4"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -974,7 +976,7 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="3"/>
-      <c r="S24" s="1"/>
+      <c r="S24" s="4"/>
       <c r="T24" s="4"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.3">
@@ -1045,11 +1047,17 @@
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="G28" s="3"/>
-      <c r="H28" s="4"/>
+      <c r="H28" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="I28" s="3"/>
-      <c r="J28" s="4"/>
+      <c r="J28" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -1058,7 +1066,7 @@
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="3"/>
-      <c r="S28" s="4"/>
+      <c r="S28" s="1"/>
       <c r="T28" s="4"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.3">
@@ -1068,9 +1076,13 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="4"/>
+      <c r="H29" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="I29" s="3"/>
-      <c r="J29" s="4"/>
+      <c r="J29" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
@@ -1079,7 +1091,7 @@
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="3"/>
-      <c r="S29" s="4"/>
+      <c r="S29" s="1"/>
       <c r="T29" s="4"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.3">
@@ -1182,7 +1194,7 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="Q34" s="4"/>
       <c r="R34" s="3"/>
@@ -1237,15 +1249,15 @@
       <c r="D37" s="4"/>
       <c r="E37" s="3"/>
       <c r="F37" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="4" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -1266,11 +1278,11 @@
       <c r="F38" s="4"/>
       <c r="G38" s="3"/>
       <c r="H38" s="4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>

</xml_diff>

<commit_message>
Docs: #5 Update RS for Controlling Event for Mouse Event Manager
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6A4DB5-00B3-4E3B-8EDE-EF996CAE1B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCEBB73-4B11-4188-8C58-23ECF942686E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6615" yWindow="0" windowWidth="20445" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -188,6 +188,14 @@
   </si>
   <si>
     <t>마우스 이벤트 메니저</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마우스 이벤트 메니저에 이벤트 전달</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -595,7 +603,7 @@
   <dimension ref="B2:T65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -955,7 +963,7 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="3"/>
-      <c r="S23" s="2"/>
+      <c r="S23" s="1"/>
       <c r="T23" s="4"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.3">
@@ -965,9 +973,13 @@
       <c r="E24" s="3"/>
       <c r="F24" s="4"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="4"/>
+      <c r="H24" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="I24" s="3"/>
-      <c r="J24" s="4"/>
+      <c r="J24" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -976,7 +988,7 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="3"/>
-      <c r="S24" s="4"/>
+      <c r="S24" s="1"/>
       <c r="T24" s="4"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Docs/2 basic section map composition (#8)
* Docs: #2 Add FlowChart for Map Editor

* Docs: #2 Add FlowChart For Basic Mouse Event

* Docs: #5 Flow chart for basic Mouse Event Manager

* Docs: #2 Update FlowChart for Map Editor <- Mouse Event

* Docs: #1 Update FlowChart-Info-Message

* Docs: #5 Update RS for Mouse Event Manager

* Docs: #5 Update RS for Controlling Event for Mouse Event Manager

---------

Co-authored-by: MJ <75807617+kang123077@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992F0432-7108-4781-9BAA-766A4294B717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCEBB73-4B11-4188-8C58-23ECF942686E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10395" yWindow="1290" windowWidth="17850" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6615" yWindow="0" windowWidth="20445" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,14 +63,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>U</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI 관련</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Category 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -103,10 +95,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FR-U-A-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Implementation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -123,14 +111,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FR-U-T-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FR-U-A-02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공지 메시지 = 시스템 메시지 출력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -139,10 +119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FR-U-T-02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공지 메시지 출력 사이클</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -155,10 +131,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>N</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -180,6 +152,50 @@
   </si>
   <si>
     <t>애니메이션 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>광역 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-A-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-A-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-T-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-T-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마우스 이벤트 메니저</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마우스 이벤트 메니저에 이벤트 전달</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -299,7 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -587,7 +603,7 @@
   <dimension ref="B2:T65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -599,7 +615,7 @@
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
@@ -608,7 +624,7 @@
       </c>
       <c r="S4" s="1"/>
       <c r="T4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
@@ -622,23 +638,23 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
@@ -649,22 +665,22 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="J6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
@@ -674,23 +690,23 @@
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -701,7 +717,7 @@
       <c r="Q12" s="7"/>
       <c r="R12" s="8"/>
       <c r="S12" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="T12" s="7"/>
     </row>
@@ -717,11 +733,11 @@
       <c r="F13" s="4"/>
       <c r="G13" s="3"/>
       <c r="H13" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -731,7 +747,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="2"/>
+      <c r="S13" s="1"/>
       <c r="T13" s="4"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.3">
@@ -927,19 +943,17 @@
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="F23" s="4"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -960,11 +974,11 @@
       <c r="F24" s="4"/>
       <c r="G24" s="3"/>
       <c r="H24" s="4" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="4" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -1045,11 +1059,17 @@
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="G28" s="3"/>
-      <c r="H28" s="4"/>
+      <c r="H28" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="I28" s="3"/>
-      <c r="J28" s="4"/>
+      <c r="J28" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -1058,7 +1078,7 @@
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="3"/>
-      <c r="S28" s="4"/>
+      <c r="S28" s="1"/>
       <c r="T28" s="4"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.3">
@@ -1068,9 +1088,13 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="4"/>
+      <c r="H29" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="I29" s="3"/>
-      <c r="J29" s="4"/>
+      <c r="J29" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
@@ -1079,7 +1103,7 @@
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="3"/>
-      <c r="S29" s="4"/>
+      <c r="S29" s="1"/>
       <c r="T29" s="4"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.3">
@@ -1182,7 +1206,7 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="Q34" s="4"/>
       <c r="R34" s="3"/>
@@ -1237,15 +1261,15 @@
       <c r="D37" s="4"/>
       <c r="E37" s="3"/>
       <c r="F37" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="4" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -1266,11 +1290,11 @@
       <c r="F38" s="4"/>
       <c r="G38" s="3"/>
       <c r="H38" s="4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>

</xml_diff>

<commit_message>
Docs: #9 Add Functions for Basic Editor to RS
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCEBB73-4B11-4188-8C58-23ECF942686E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE8671E-293D-4D7C-AF0A-7B02D8814E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="0" windowWidth="20445" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16320" yWindow="0" windowWidth="12585" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,10 +143,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>`</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Animation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -196,6 +192,123 @@
   </si>
   <si>
     <t>마우스 이벤트 메니저에 이벤트 전달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Editor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에디터 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 에디터 기능등</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>불러오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01.03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01.04</t>
+  </si>
+  <si>
+    <t>FR-C-E-01.06</t>
+  </si>
+  <si>
+    <t>추상 함수 실행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01.04.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01.04.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01.04.03</t>
+  </si>
+  <si>
+    <t>FR-C-E-01.04.04</t>
+  </si>
+  <si>
+    <t>FR-C-E-01.04.05</t>
+  </si>
+  <si>
+    <t>FR-C-E-01.04.06</t>
+  </si>
+  <si>
+    <t>에디터 켜기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에디터 초기화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마우스 이벤트 할당</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커스텀 버튼들 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 불러오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에디터 끄기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01.04.07</t>
+  </si>
+  <si>
+    <t>다른 이름으로 저장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01.05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마우스 이벤트 초기화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 메뉴로 돌아가기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -245,7 +358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -275,26 +388,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -316,10 +409,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -602,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:T65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -665,22 +758,33 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
       </c>
       <c r="H6" t="s">
         <v>16</v>
       </c>
       <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
         <v>30</v>
       </c>
-      <c r="J6" t="s">
-        <v>31</v>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
@@ -689,37 +793,37 @@
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="7" t="s">
+      <c r="I12" s="6"/>
+      <c r="J12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="7" t="s">
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T12" s="7"/>
+      <c r="T12" s="5"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
@@ -919,41 +1023,41 @@
       <c r="T21" s="4"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -974,11 +1078,11 @@
       <c r="F24" s="4"/>
       <c r="G24" s="3"/>
       <c r="H24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -1038,11 +1142,17 @@
       <c r="C27" s="3"/>
       <c r="D27" s="4"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="4"/>
+      <c r="H27" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="I27" s="3"/>
-      <c r="J27" s="4"/>
+      <c r="J27" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -1051,7 +1161,7 @@
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="3"/>
-      <c r="S27" s="4"/>
+      <c r="S27" s="2"/>
       <c r="T27" s="4"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.3">
@@ -1059,16 +1169,14 @@
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="F28" s="4"/>
       <c r="G28" s="3"/>
       <c r="H28" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="4" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -1078,7 +1186,7 @@
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="3"/>
-      <c r="S28" s="1"/>
+      <c r="S28" s="2"/>
       <c r="T28" s="4"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.3">
@@ -1089,11 +1197,11 @@
       <c r="F29" s="4"/>
       <c r="G29" s="3"/>
       <c r="H29" s="4" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="4" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -1103,7 +1211,7 @@
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="3"/>
-      <c r="S29" s="1"/>
+      <c r="S29" s="2"/>
       <c r="T29" s="4"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.3">
@@ -1113,9 +1221,13 @@
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="4"/>
+      <c r="H30" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
@@ -1124,7 +1236,7 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="3"/>
-      <c r="S30" s="4"/>
+      <c r="S30" s="2"/>
       <c r="T30" s="4"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.3">
@@ -1134,9 +1246,13 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="4"/>
+      <c r="H31" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="I31" s="3"/>
-      <c r="J31" s="4"/>
+      <c r="J31" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
@@ -1145,7 +1261,7 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="4"/>
+      <c r="S31" s="2"/>
       <c r="T31" s="4"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
@@ -1155,9 +1271,13 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="4"/>
+      <c r="H32" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="I32" s="3"/>
-      <c r="J32" s="4"/>
+      <c r="J32" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
@@ -1166,7 +1286,7 @@
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="3"/>
-      <c r="S32" s="4"/>
+      <c r="S32" s="2"/>
       <c r="T32" s="4"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.3">
@@ -1176,9 +1296,13 @@
       <c r="E33" s="3"/>
       <c r="F33" s="4"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="4"/>
+      <c r="H33" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="I33" s="3"/>
-      <c r="J33" s="4"/>
+      <c r="J33" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -1187,7 +1311,7 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="3"/>
-      <c r="S33" s="4"/>
+      <c r="S33" s="2"/>
       <c r="T33" s="4"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.3">
@@ -1197,20 +1321,22 @@
       <c r="E34" s="3"/>
       <c r="F34" s="4"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="4"/>
+      <c r="H34" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="I34" s="3"/>
-      <c r="J34" s="4"/>
+      <c r="J34" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
-      <c r="P34" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="3"/>
-      <c r="S34" s="4"/>
+      <c r="S34" s="2"/>
       <c r="T34" s="4"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.3">
@@ -1220,9 +1346,13 @@
       <c r="E35" s="3"/>
       <c r="F35" s="4"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="4"/>
+      <c r="H35" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="I35" s="3"/>
-      <c r="J35" s="4"/>
+      <c r="J35" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -1231,45 +1361,47 @@
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="3"/>
-      <c r="S35" s="4"/>
+      <c r="S35" s="2"/>
       <c r="T35" s="4"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B36" s="5"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="7"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="F37" s="4"/>
       <c r="G37" s="3"/>
       <c r="H37" s="4" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="4" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -1279,7 +1411,7 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="3"/>
-      <c r="S37" s="1"/>
+      <c r="S37" s="2"/>
       <c r="T37" s="4"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.3">
@@ -1290,11 +1422,11 @@
       <c r="F38" s="4"/>
       <c r="G38" s="3"/>
       <c r="H38" s="4" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="4" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
@@ -1304,7 +1436,7 @@
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
       <c r="R38" s="3"/>
-      <c r="S38" s="1"/>
+      <c r="S38" s="2"/>
       <c r="T38" s="4"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.3">
@@ -1314,9 +1446,13 @@
       <c r="E39" s="3"/>
       <c r="F39" s="4"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="4"/>
+      <c r="H39" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="I39" s="3"/>
-      <c r="J39" s="4"/>
+      <c r="J39" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -1325,7 +1461,7 @@
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
       <c r="R39" s="3"/>
-      <c r="S39" s="4"/>
+      <c r="S39" s="2"/>
       <c r="T39" s="4"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.3">
@@ -1335,9 +1471,13 @@
       <c r="E40" s="3"/>
       <c r="F40" s="4"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="4"/>
+      <c r="H40" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="I40" s="3"/>
-      <c r="J40" s="4"/>
+      <c r="J40" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -1346,7 +1486,7 @@
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
       <c r="R40" s="3"/>
-      <c r="S40" s="4"/>
+      <c r="S40" s="2"/>
       <c r="T40" s="4"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.3">
@@ -1564,11 +1704,17 @@
       <c r="C51" s="3"/>
       <c r="D51" s="4"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="4"/>
+      <c r="F51" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="G51" s="3"/>
-      <c r="H51" s="4"/>
+      <c r="H51" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="I51" s="3"/>
-      <c r="J51" s="4"/>
+      <c r="J51" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
@@ -1577,7 +1723,7 @@
       <c r="P51" s="4"/>
       <c r="Q51" s="4"/>
       <c r="R51" s="3"/>
-      <c r="S51" s="4"/>
+      <c r="S51" s="1"/>
       <c r="T51" s="4"/>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.3">
@@ -1587,9 +1733,13 @@
       <c r="E52" s="3"/>
       <c r="F52" s="4"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="4"/>
+      <c r="H52" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="I52" s="3"/>
-      <c r="J52" s="4"/>
+      <c r="J52" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
@@ -1598,7 +1748,7 @@
       <c r="P52" s="4"/>
       <c r="Q52" s="4"/>
       <c r="R52" s="3"/>
-      <c r="S52" s="4"/>
+      <c r="S52" s="1"/>
       <c r="T52" s="4"/>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.3">
@@ -1690,11 +1840,17 @@
       <c r="C57" s="3"/>
       <c r="D57" s="4"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="4"/>
+      <c r="F57" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G57" s="3"/>
-      <c r="H57" s="4"/>
+      <c r="H57" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="I57" s="3"/>
-      <c r="J57" s="4"/>
+      <c r="J57" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
@@ -1703,7 +1859,7 @@
       <c r="P57" s="4"/>
       <c r="Q57" s="4"/>
       <c r="R57" s="3"/>
-      <c r="S57" s="4"/>
+      <c r="S57" s="1"/>
       <c r="T57" s="4"/>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.3">
@@ -1713,9 +1869,13 @@
       <c r="E58" s="3"/>
       <c r="F58" s="4"/>
       <c r="G58" s="3"/>
-      <c r="H58" s="4"/>
+      <c r="H58" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="I58" s="3"/>
-      <c r="J58" s="4"/>
+      <c r="J58" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
@@ -1724,7 +1884,7 @@
       <c r="P58" s="4"/>
       <c r="Q58" s="4"/>
       <c r="R58" s="3"/>
-      <c r="S58" s="4"/>
+      <c r="S58" s="1"/>
       <c r="T58" s="4"/>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Docs: #10 Update RS for Modal Module
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE8671E-293D-4D7C-AF0A-7B02D8814E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E77F48-49CD-4B50-A588-9B26865DB0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16320" yWindow="0" windowWidth="12585" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="92">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,10 +107,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공지 메시지 = 시스템 메시지 출력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -171,14 +167,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FR-C-T-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FR-C-T-02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FR-C-01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -242,13 +230,6 @@
     <t>FR-C-E-01.04</t>
   </si>
   <si>
-    <t>FR-C-E-01.06</t>
-  </si>
-  <si>
-    <t>추상 함수 실행</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FR-C-E-01.04.01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -293,22 +274,112 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FR-C-E-01.04.07</t>
-  </si>
-  <si>
-    <t>다른 이름으로 저장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FR-C-E-01.05</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>마우스 이벤트 초기화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인 메뉴로 돌아가기</t>
+    <t>에디터용 인터페이스: 맵 에디터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 메뉴 UI 토글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-N-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-N-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-01.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 컨텐츠 프리펩 광역 컨포넌트에 전달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-01.02</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.03</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.04</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.05</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.06</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.07</t>
+  </si>
+  <si>
+    <t>모달 초기화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 초기값 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 타입 관련 컴포넌트 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 컨텐츠 적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 취소 / 확인 버튼 이벤트 적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 텍스트 모달 인터페이스 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-03</t>
+  </si>
+  <si>
+    <t>일반 텍스트 인풋 모달 인터페이스 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -403,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -411,8 +482,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -693,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:T65"/>
+  <dimension ref="B2:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="U72" sqref="U72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -731,19 +800,19 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
       </c>
       <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
         <v>26</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>27</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" t="s">
@@ -758,33 +827,53 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>32</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
       </c>
       <c r="H6" t="s">
         <v>16</v>
       </c>
       <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
         <v>29</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>73</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
@@ -1023,41 +1112,41 @@
       <c r="T21" s="4"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="7"/>
+      <c r="D22" s="4"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="7"/>
+      <c r="H22" s="4"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
       <c r="R22" s="3"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -1078,11 +1167,11 @@
       <c r="F24" s="4"/>
       <c r="G24" s="3"/>
       <c r="H24" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -1143,15 +1232,15 @@
       <c r="D27" s="4"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -1172,11 +1261,11 @@
       <c r="F28" s="4"/>
       <c r="G28" s="3"/>
       <c r="H28" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -1197,11 +1286,11 @@
       <c r="F29" s="4"/>
       <c r="G29" s="3"/>
       <c r="H29" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -1222,11 +1311,11 @@
       <c r="F30" s="4"/>
       <c r="G30" s="3"/>
       <c r="H30" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -1247,11 +1336,11 @@
       <c r="F31" s="4"/>
       <c r="G31" s="3"/>
       <c r="H31" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
@@ -1272,11 +1361,11 @@
       <c r="F32" s="4"/>
       <c r="G32" s="3"/>
       <c r="H32" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -1297,11 +1386,11 @@
       <c r="F33" s="4"/>
       <c r="G33" s="3"/>
       <c r="H33" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -1322,11 +1411,11 @@
       <c r="F34" s="4"/>
       <c r="G34" s="3"/>
       <c r="H34" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -1347,11 +1436,11 @@
       <c r="F35" s="4"/>
       <c r="G35" s="3"/>
       <c r="H35" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -1365,29 +1454,29 @@
       <c r="T35" s="4"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B36" s="7"/>
+      <c r="B36" s="4"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="7"/>
+      <c r="D36" s="4"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="7"/>
+      <c r="F36" s="4"/>
       <c r="G36" s="3"/>
       <c r="H36" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I36" s="3"/>
-      <c r="J36" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
+      <c r="J36" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
       <c r="R36" s="3"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="7"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="4"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
@@ -1397,11 +1486,11 @@
       <c r="F37" s="4"/>
       <c r="G37" s="3"/>
       <c r="H37" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -1422,11 +1511,11 @@
       <c r="F38" s="4"/>
       <c r="G38" s="3"/>
       <c r="H38" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
@@ -1446,13 +1535,9 @@
       <c r="E39" s="3"/>
       <c r="F39" s="4"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="H39" s="4"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -1461,7 +1546,7 @@
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
       <c r="R39" s="3"/>
-      <c r="S39" s="2"/>
+      <c r="S39" s="4"/>
       <c r="T39" s="4"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.3">
@@ -1471,13 +1556,9 @@
       <c r="E40" s="3"/>
       <c r="F40" s="4"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="H40" s="4"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -1486,7 +1567,7 @@
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
       <c r="R40" s="3"/>
-      <c r="S40" s="2"/>
+      <c r="S40" s="4"/>
       <c r="T40" s="4"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.3">
@@ -1709,11 +1790,11 @@
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
@@ -1734,11 +1815,11 @@
       <c r="F52" s="4"/>
       <c r="G52" s="3"/>
       <c r="H52" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I52" s="3"/>
       <c r="J52" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -1841,15 +1922,15 @@
       <c r="D57" s="4"/>
       <c r="E57" s="3"/>
       <c r="F57" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="4" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
@@ -1870,11 +1951,11 @@
       <c r="F58" s="4"/>
       <c r="G58" s="3"/>
       <c r="H58" s="4" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
@@ -2034,6 +2115,3431 @@
       <c r="S65" s="4"/>
       <c r="T65" s="4"/>
     </row>
+    <row r="66" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B66" s="4"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="4"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="4"/>
+      <c r="Q66" s="4"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="4"/>
+      <c r="T66" s="4"/>
+    </row>
+    <row r="67" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B67" s="4"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
+      <c r="P67" s="4"/>
+      <c r="Q67" s="4"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="4"/>
+    </row>
+    <row r="68" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B68" s="4"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="4"/>
+      <c r="Q68" s="4"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="4"/>
+      <c r="T68" s="4"/>
+    </row>
+    <row r="69" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B69" s="4"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
+      <c r="P69" s="4"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="4"/>
+      <c r="T69" s="4"/>
+    </row>
+    <row r="70" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B70" s="4"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="4"/>
+      <c r="Q70" s="4"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="4"/>
+      <c r="T70" s="4"/>
+    </row>
+    <row r="71" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B71" s="4"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
+      <c r="P71" s="4"/>
+      <c r="Q71" s="4"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="4"/>
+      <c r="T71" s="4"/>
+    </row>
+    <row r="72" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B72" s="4"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
+      <c r="P72" s="4"/>
+      <c r="Q72" s="4"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="4"/>
+      <c r="T72" s="4"/>
+    </row>
+    <row r="73" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B73" s="4"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4"/>
+      <c r="P73" s="4"/>
+      <c r="Q73" s="4"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="4"/>
+      <c r="T73" s="4"/>
+    </row>
+    <row r="74" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B74" s="4"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E74" s="3"/>
+      <c r="F74" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G74" s="3"/>
+      <c r="H74" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I74" s="3"/>
+      <c r="J74" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
+      <c r="P74" s="4"/>
+      <c r="Q74" s="4"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="4"/>
+    </row>
+    <row r="75" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B75" s="4"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I75" s="3"/>
+      <c r="J75" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
+      <c r="P75" s="4"/>
+      <c r="Q75" s="4"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="4"/>
+    </row>
+    <row r="76" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B76" s="4"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I76" s="3"/>
+      <c r="J76" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K76" s="4"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="4"/>
+      <c r="O76" s="4"/>
+      <c r="P76" s="4"/>
+      <c r="Q76" s="4"/>
+      <c r="R76" s="3"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="4"/>
+    </row>
+    <row r="77" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B77" s="4"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I77" s="3"/>
+      <c r="J77" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="3"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="4"/>
+    </row>
+    <row r="78" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B78" s="4"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="J78" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K78" s="4"/>
+      <c r="L78" s="4"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="4"/>
+      <c r="Q78" s="4"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="4"/>
+    </row>
+    <row r="79" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B79" s="4"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I79" s="3"/>
+      <c r="J79" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="4"/>
+      <c r="N79" s="4"/>
+      <c r="O79" s="4"/>
+      <c r="P79" s="4"/>
+      <c r="Q79" s="4"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="4"/>
+    </row>
+    <row r="80" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B80" s="4"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I80" s="3"/>
+      <c r="J80" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="3"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="4"/>
+    </row>
+    <row r="81" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B81" s="4"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I81" s="3"/>
+      <c r="J81" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="4"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="4"/>
+    </row>
+    <row r="82" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B82" s="4"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I82" s="3"/>
+      <c r="J82" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K82" s="4"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="4"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="4"/>
+      <c r="Q82" s="4"/>
+      <c r="R82" s="3"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="4"/>
+    </row>
+    <row r="83" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B83" s="4"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I83" s="3"/>
+      <c r="J83" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K83" s="4"/>
+      <c r="L83" s="4"/>
+      <c r="M83" s="4"/>
+      <c r="N83" s="4"/>
+      <c r="O83" s="4"/>
+      <c r="P83" s="4"/>
+      <c r="Q83" s="4"/>
+      <c r="R83" s="3"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="4"/>
+    </row>
+    <row r="84" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B84" s="4"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="3"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="4"/>
+      <c r="Q84" s="4"/>
+      <c r="R84" s="3"/>
+      <c r="S84" s="4"/>
+      <c r="T84" s="4"/>
+    </row>
+    <row r="85" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B85" s="4"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="4"/>
+      <c r="L85" s="4"/>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="4"/>
+      <c r="P85" s="4"/>
+      <c r="Q85" s="4"/>
+      <c r="R85" s="3"/>
+      <c r="S85" s="4"/>
+      <c r="T85" s="4"/>
+    </row>
+    <row r="86" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B86" s="4"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="4"/>
+      <c r="Q86" s="4"/>
+      <c r="R86" s="3"/>
+      <c r="S86" s="4"/>
+      <c r="T86" s="4"/>
+    </row>
+    <row r="87" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B87" s="4"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="3"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
+      <c r="L87" s="4"/>
+      <c r="M87" s="4"/>
+      <c r="N87" s="4"/>
+      <c r="O87" s="4"/>
+      <c r="P87" s="4"/>
+      <c r="Q87" s="4"/>
+      <c r="R87" s="3"/>
+      <c r="S87" s="4"/>
+      <c r="T87" s="4"/>
+    </row>
+    <row r="88" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B88" s="4"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="4"/>
+      <c r="Q88" s="4"/>
+      <c r="R88" s="3"/>
+      <c r="S88" s="4"/>
+      <c r="T88" s="4"/>
+    </row>
+    <row r="89" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B89" s="4"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="4"/>
+      <c r="O89" s="4"/>
+      <c r="P89" s="4"/>
+      <c r="Q89" s="4"/>
+      <c r="R89" s="3"/>
+      <c r="S89" s="4"/>
+      <c r="T89" s="4"/>
+    </row>
+    <row r="90" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B90" s="4"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+      <c r="M90" s="4"/>
+      <c r="N90" s="4"/>
+      <c r="O90" s="4"/>
+      <c r="P90" s="4"/>
+      <c r="Q90" s="4"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="4"/>
+      <c r="T90" s="4"/>
+    </row>
+    <row r="91" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B91" s="4"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
+      <c r="L91" s="4"/>
+      <c r="M91" s="4"/>
+      <c r="N91" s="4"/>
+      <c r="O91" s="4"/>
+      <c r="P91" s="4"/>
+      <c r="Q91" s="4"/>
+      <c r="R91" s="3"/>
+      <c r="S91" s="4"/>
+      <c r="T91" s="4"/>
+    </row>
+    <row r="92" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B92" s="4"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="4"/>
+      <c r="O92" s="4"/>
+      <c r="P92" s="4"/>
+      <c r="Q92" s="4"/>
+      <c r="R92" s="3"/>
+      <c r="S92" s="4"/>
+      <c r="T92" s="4"/>
+    </row>
+    <row r="93" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B93" s="4"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
+      <c r="L93" s="4"/>
+      <c r="M93" s="4"/>
+      <c r="N93" s="4"/>
+      <c r="O93" s="4"/>
+      <c r="P93" s="4"/>
+      <c r="Q93" s="4"/>
+      <c r="R93" s="3"/>
+      <c r="S93" s="4"/>
+      <c r="T93" s="4"/>
+    </row>
+    <row r="94" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B94" s="4"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="3"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
+      <c r="L94" s="4"/>
+      <c r="M94" s="4"/>
+      <c r="N94" s="4"/>
+      <c r="O94" s="4"/>
+      <c r="P94" s="4"/>
+      <c r="Q94" s="4"/>
+      <c r="R94" s="3"/>
+      <c r="S94" s="4"/>
+      <c r="T94" s="4"/>
+    </row>
+    <row r="95" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B95" s="4"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="4"/>
+      <c r="M95" s="4"/>
+      <c r="N95" s="4"/>
+      <c r="O95" s="4"/>
+      <c r="P95" s="4"/>
+      <c r="Q95" s="4"/>
+      <c r="R95" s="3"/>
+      <c r="S95" s="4"/>
+      <c r="T95" s="4"/>
+    </row>
+    <row r="96" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B96" s="4"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="3"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="4"/>
+      <c r="L96" s="4"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="4"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="4"/>
+      <c r="Q96" s="4"/>
+      <c r="R96" s="3"/>
+      <c r="S96" s="4"/>
+      <c r="T96" s="4"/>
+    </row>
+    <row r="97" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B97" s="4"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="3"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="4"/>
+      <c r="L97" s="4"/>
+      <c r="M97" s="4"/>
+      <c r="N97" s="4"/>
+      <c r="O97" s="4"/>
+      <c r="P97" s="4"/>
+      <c r="Q97" s="4"/>
+      <c r="R97" s="3"/>
+      <c r="S97" s="4"/>
+      <c r="T97" s="4"/>
+    </row>
+    <row r="98" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B98" s="4"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="3"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
+      <c r="L98" s="4"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="4"/>
+      <c r="O98" s="4"/>
+      <c r="P98" s="4"/>
+      <c r="Q98" s="4"/>
+      <c r="R98" s="3"/>
+      <c r="S98" s="4"/>
+      <c r="T98" s="4"/>
+    </row>
+    <row r="99" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B99" s="4"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="3"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="4"/>
+      <c r="L99" s="4"/>
+      <c r="M99" s="4"/>
+      <c r="N99" s="4"/>
+      <c r="O99" s="4"/>
+      <c r="P99" s="4"/>
+      <c r="Q99" s="4"/>
+      <c r="R99" s="3"/>
+      <c r="S99" s="4"/>
+      <c r="T99" s="4"/>
+    </row>
+    <row r="100" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B100" s="4"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="3"/>
+      <c r="J100" s="4"/>
+      <c r="K100" s="4"/>
+      <c r="L100" s="4"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="4"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="4"/>
+      <c r="Q100" s="4"/>
+      <c r="R100" s="3"/>
+      <c r="S100" s="4"/>
+      <c r="T100" s="4"/>
+    </row>
+    <row r="101" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B101" s="4"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="4"/>
+      <c r="K101" s="4"/>
+      <c r="L101" s="4"/>
+      <c r="M101" s="4"/>
+      <c r="N101" s="4"/>
+      <c r="O101" s="4"/>
+      <c r="P101" s="4"/>
+      <c r="Q101" s="4"/>
+      <c r="R101" s="3"/>
+      <c r="S101" s="4"/>
+      <c r="T101" s="4"/>
+    </row>
+    <row r="102" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B102" s="4"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="3"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="4"/>
+      <c r="L102" s="4"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="4"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="4"/>
+      <c r="Q102" s="4"/>
+      <c r="R102" s="3"/>
+      <c r="S102" s="4"/>
+      <c r="T102" s="4"/>
+    </row>
+    <row r="103" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B103" s="4"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="3"/>
+      <c r="J103" s="4"/>
+      <c r="K103" s="4"/>
+      <c r="L103" s="4"/>
+      <c r="M103" s="4"/>
+      <c r="N103" s="4"/>
+      <c r="O103" s="4"/>
+      <c r="P103" s="4"/>
+      <c r="Q103" s="4"/>
+      <c r="R103" s="3"/>
+      <c r="S103" s="4"/>
+      <c r="T103" s="4"/>
+    </row>
+    <row r="104" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B104" s="4"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="3"/>
+      <c r="J104" s="4"/>
+      <c r="K104" s="4"/>
+      <c r="L104" s="4"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="4"/>
+      <c r="O104" s="4"/>
+      <c r="P104" s="4"/>
+      <c r="Q104" s="4"/>
+      <c r="R104" s="3"/>
+      <c r="S104" s="4"/>
+      <c r="T104" s="4"/>
+    </row>
+    <row r="105" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B105" s="4"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="3"/>
+      <c r="J105" s="4"/>
+      <c r="K105" s="4"/>
+      <c r="L105" s="4"/>
+      <c r="M105" s="4"/>
+      <c r="N105" s="4"/>
+      <c r="O105" s="4"/>
+      <c r="P105" s="4"/>
+      <c r="Q105" s="4"/>
+      <c r="R105" s="3"/>
+      <c r="S105" s="4"/>
+      <c r="T105" s="4"/>
+    </row>
+    <row r="106" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B106" s="4"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="3"/>
+      <c r="J106" s="4"/>
+      <c r="K106" s="4"/>
+      <c r="L106" s="4"/>
+      <c r="M106" s="4"/>
+      <c r="N106" s="4"/>
+      <c r="O106" s="4"/>
+      <c r="P106" s="4"/>
+      <c r="Q106" s="4"/>
+      <c r="R106" s="3"/>
+      <c r="S106" s="4"/>
+      <c r="T106" s="4"/>
+    </row>
+    <row r="107" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B107" s="4"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="3"/>
+      <c r="J107" s="4"/>
+      <c r="K107" s="4"/>
+      <c r="L107" s="4"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="O107" s="4"/>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="4"/>
+      <c r="R107" s="3"/>
+      <c r="S107" s="4"/>
+      <c r="T107" s="4"/>
+    </row>
+    <row r="108" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B108" s="4"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="4"/>
+      <c r="K108" s="4"/>
+      <c r="L108" s="4"/>
+      <c r="M108" s="4"/>
+      <c r="N108" s="4"/>
+      <c r="O108" s="4"/>
+      <c r="P108" s="4"/>
+      <c r="Q108" s="4"/>
+      <c r="R108" s="3"/>
+      <c r="S108" s="4"/>
+      <c r="T108" s="4"/>
+    </row>
+    <row r="109" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B109" s="4"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="3"/>
+      <c r="J109" s="4"/>
+      <c r="K109" s="4"/>
+      <c r="L109" s="4"/>
+      <c r="M109" s="4"/>
+      <c r="N109" s="4"/>
+      <c r="O109" s="4"/>
+      <c r="P109" s="4"/>
+      <c r="Q109" s="4"/>
+      <c r="R109" s="3"/>
+      <c r="S109" s="4"/>
+      <c r="T109" s="4"/>
+    </row>
+    <row r="110" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B110" s="4"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="3"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="3"/>
+      <c r="J110" s="4"/>
+      <c r="K110" s="4"/>
+      <c r="L110" s="4"/>
+      <c r="M110" s="4"/>
+      <c r="N110" s="4"/>
+      <c r="O110" s="4"/>
+      <c r="P110" s="4"/>
+      <c r="Q110" s="4"/>
+      <c r="R110" s="3"/>
+      <c r="S110" s="4"/>
+      <c r="T110" s="4"/>
+    </row>
+    <row r="111" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B111" s="4"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="3"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="3"/>
+      <c r="J111" s="4"/>
+      <c r="K111" s="4"/>
+      <c r="L111" s="4"/>
+      <c r="M111" s="4"/>
+      <c r="N111" s="4"/>
+      <c r="O111" s="4"/>
+      <c r="P111" s="4"/>
+      <c r="Q111" s="4"/>
+      <c r="R111" s="3"/>
+      <c r="S111" s="4"/>
+      <c r="T111" s="4"/>
+    </row>
+    <row r="112" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B112" s="4"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="3"/>
+      <c r="J112" s="4"/>
+      <c r="K112" s="4"/>
+      <c r="L112" s="4"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="4"/>
+      <c r="O112" s="4"/>
+      <c r="P112" s="4"/>
+      <c r="Q112" s="4"/>
+      <c r="R112" s="3"/>
+      <c r="S112" s="4"/>
+      <c r="T112" s="4"/>
+    </row>
+    <row r="113" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B113" s="4"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="4"/>
+      <c r="I113" s="3"/>
+      <c r="J113" s="4"/>
+      <c r="K113" s="4"/>
+      <c r="L113" s="4"/>
+      <c r="M113" s="4"/>
+      <c r="N113" s="4"/>
+      <c r="O113" s="4"/>
+      <c r="P113" s="4"/>
+      <c r="Q113" s="4"/>
+      <c r="R113" s="3"/>
+      <c r="S113" s="4"/>
+      <c r="T113" s="4"/>
+    </row>
+    <row r="114" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B114" s="4"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="3"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="3"/>
+      <c r="J114" s="4"/>
+      <c r="K114" s="4"/>
+      <c r="L114" s="4"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="4"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="4"/>
+      <c r="Q114" s="4"/>
+      <c r="R114" s="3"/>
+      <c r="S114" s="4"/>
+      <c r="T114" s="4"/>
+    </row>
+    <row r="115" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B115" s="4"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="3"/>
+      <c r="H115" s="4"/>
+      <c r="I115" s="3"/>
+      <c r="J115" s="4"/>
+      <c r="K115" s="4"/>
+      <c r="L115" s="4"/>
+      <c r="M115" s="4"/>
+      <c r="N115" s="4"/>
+      <c r="O115" s="4"/>
+      <c r="P115" s="4"/>
+      <c r="Q115" s="4"/>
+      <c r="R115" s="3"/>
+      <c r="S115" s="4"/>
+      <c r="T115" s="4"/>
+    </row>
+    <row r="116" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B116" s="4"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="3"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="3"/>
+      <c r="J116" s="4"/>
+      <c r="K116" s="4"/>
+      <c r="L116" s="4"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="4"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="4"/>
+      <c r="Q116" s="4"/>
+      <c r="R116" s="3"/>
+      <c r="S116" s="4"/>
+      <c r="T116" s="4"/>
+    </row>
+    <row r="117" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B117" s="4"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="3"/>
+      <c r="H117" s="4"/>
+      <c r="I117" s="3"/>
+      <c r="J117" s="4"/>
+      <c r="K117" s="4"/>
+      <c r="L117" s="4"/>
+      <c r="M117" s="4"/>
+      <c r="N117" s="4"/>
+      <c r="O117" s="4"/>
+      <c r="P117" s="4"/>
+      <c r="Q117" s="4"/>
+      <c r="R117" s="3"/>
+      <c r="S117" s="4"/>
+      <c r="T117" s="4"/>
+    </row>
+    <row r="118" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B118" s="4"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="3"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="3"/>
+      <c r="J118" s="4"/>
+      <c r="K118" s="4"/>
+      <c r="L118" s="4"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="4"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="4"/>
+      <c r="Q118" s="4"/>
+      <c r="R118" s="3"/>
+      <c r="S118" s="4"/>
+      <c r="T118" s="4"/>
+    </row>
+    <row r="119" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B119" s="4"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="3"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="3"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="3"/>
+      <c r="J119" s="4"/>
+      <c r="K119" s="4"/>
+      <c r="L119" s="4"/>
+      <c r="M119" s="4"/>
+      <c r="N119" s="4"/>
+      <c r="O119" s="4"/>
+      <c r="P119" s="4"/>
+      <c r="Q119" s="4"/>
+      <c r="R119" s="3"/>
+      <c r="S119" s="4"/>
+      <c r="T119" s="4"/>
+    </row>
+    <row r="120" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B120" s="4"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="3"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="3"/>
+      <c r="J120" s="4"/>
+      <c r="K120" s="4"/>
+      <c r="L120" s="4"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="4"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="4"/>
+      <c r="Q120" s="4"/>
+      <c r="R120" s="3"/>
+      <c r="S120" s="4"/>
+      <c r="T120" s="4"/>
+    </row>
+    <row r="121" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B121" s="4"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="3"/>
+      <c r="H121" s="4"/>
+      <c r="I121" s="3"/>
+      <c r="J121" s="4"/>
+      <c r="K121" s="4"/>
+      <c r="L121" s="4"/>
+      <c r="M121" s="4"/>
+      <c r="N121" s="4"/>
+      <c r="O121" s="4"/>
+      <c r="P121" s="4"/>
+      <c r="Q121" s="4"/>
+      <c r="R121" s="3"/>
+      <c r="S121" s="4"/>
+      <c r="T121" s="4"/>
+    </row>
+    <row r="122" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B122" s="4"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="3"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="3"/>
+      <c r="J122" s="4"/>
+      <c r="K122" s="4"/>
+      <c r="L122" s="4"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="4"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="4"/>
+      <c r="Q122" s="4"/>
+      <c r="R122" s="3"/>
+      <c r="S122" s="4"/>
+      <c r="T122" s="4"/>
+    </row>
+    <row r="123" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B123" s="4"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="3"/>
+      <c r="H123" s="4"/>
+      <c r="I123" s="3"/>
+      <c r="J123" s="4"/>
+      <c r="K123" s="4"/>
+      <c r="L123" s="4"/>
+      <c r="M123" s="4"/>
+      <c r="N123" s="4"/>
+      <c r="O123" s="4"/>
+      <c r="P123" s="4"/>
+      <c r="Q123" s="4"/>
+      <c r="R123" s="3"/>
+      <c r="S123" s="4"/>
+      <c r="T123" s="4"/>
+    </row>
+    <row r="124" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B124" s="4"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="3"/>
+      <c r="H124" s="4"/>
+      <c r="I124" s="3"/>
+      <c r="J124" s="4"/>
+      <c r="K124" s="4"/>
+      <c r="L124" s="4"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="4"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="4"/>
+      <c r="Q124" s="4"/>
+      <c r="R124" s="3"/>
+      <c r="S124" s="4"/>
+      <c r="T124" s="4"/>
+    </row>
+    <row r="125" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B125" s="4"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="3"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="3"/>
+      <c r="H125" s="4"/>
+      <c r="I125" s="3"/>
+      <c r="J125" s="4"/>
+      <c r="K125" s="4"/>
+      <c r="L125" s="4"/>
+      <c r="M125" s="4"/>
+      <c r="N125" s="4"/>
+      <c r="O125" s="4"/>
+      <c r="P125" s="4"/>
+      <c r="Q125" s="4"/>
+      <c r="R125" s="3"/>
+      <c r="S125" s="4"/>
+      <c r="T125" s="4"/>
+    </row>
+    <row r="126" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B126" s="4"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="3"/>
+      <c r="H126" s="4"/>
+      <c r="I126" s="3"/>
+      <c r="J126" s="4"/>
+      <c r="K126" s="4"/>
+      <c r="L126" s="4"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="4"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="4"/>
+      <c r="Q126" s="4"/>
+      <c r="R126" s="3"/>
+      <c r="S126" s="4"/>
+      <c r="T126" s="4"/>
+    </row>
+    <row r="127" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B127" s="4"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="3"/>
+      <c r="F127" s="4"/>
+      <c r="G127" s="3"/>
+      <c r="H127" s="4"/>
+      <c r="I127" s="3"/>
+      <c r="J127" s="4"/>
+      <c r="K127" s="4"/>
+      <c r="L127" s="4"/>
+      <c r="M127" s="4"/>
+      <c r="N127" s="4"/>
+      <c r="O127" s="4"/>
+      <c r="P127" s="4"/>
+      <c r="Q127" s="4"/>
+      <c r="R127" s="3"/>
+      <c r="S127" s="4"/>
+      <c r="T127" s="4"/>
+    </row>
+    <row r="128" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B128" s="4"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="3"/>
+      <c r="H128" s="4"/>
+      <c r="I128" s="3"/>
+      <c r="J128" s="4"/>
+      <c r="K128" s="4"/>
+      <c r="L128" s="4"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="4"/>
+      <c r="O128" s="4"/>
+      <c r="P128" s="4"/>
+      <c r="Q128" s="4"/>
+      <c r="R128" s="3"/>
+      <c r="S128" s="4"/>
+      <c r="T128" s="4"/>
+    </row>
+    <row r="129" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B129" s="4"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="4"/>
+      <c r="G129" s="3"/>
+      <c r="H129" s="4"/>
+      <c r="I129" s="3"/>
+      <c r="J129" s="4"/>
+      <c r="K129" s="4"/>
+      <c r="L129" s="4"/>
+      <c r="M129" s="4"/>
+      <c r="N129" s="4"/>
+      <c r="O129" s="4"/>
+      <c r="P129" s="4"/>
+      <c r="Q129" s="4"/>
+      <c r="R129" s="3"/>
+      <c r="S129" s="4"/>
+      <c r="T129" s="4"/>
+    </row>
+    <row r="130" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B130" s="4"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="4"/>
+      <c r="G130" s="3"/>
+      <c r="H130" s="4"/>
+      <c r="I130" s="3"/>
+      <c r="J130" s="4"/>
+      <c r="K130" s="4"/>
+      <c r="L130" s="4"/>
+      <c r="M130" s="4"/>
+      <c r="N130" s="4"/>
+      <c r="O130" s="4"/>
+      <c r="P130" s="4"/>
+      <c r="Q130" s="4"/>
+      <c r="R130" s="3"/>
+      <c r="S130" s="4"/>
+      <c r="T130" s="4"/>
+    </row>
+    <row r="131" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B131" s="4"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="4"/>
+      <c r="G131" s="3"/>
+      <c r="H131" s="4"/>
+      <c r="I131" s="3"/>
+      <c r="J131" s="4"/>
+      <c r="K131" s="4"/>
+      <c r="L131" s="4"/>
+      <c r="M131" s="4"/>
+      <c r="N131" s="4"/>
+      <c r="O131" s="4"/>
+      <c r="P131" s="4"/>
+      <c r="Q131" s="4"/>
+      <c r="R131" s="3"/>
+      <c r="S131" s="4"/>
+      <c r="T131" s="4"/>
+    </row>
+    <row r="132" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B132" s="4"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="3"/>
+      <c r="H132" s="4"/>
+      <c r="I132" s="3"/>
+      <c r="J132" s="4"/>
+      <c r="K132" s="4"/>
+      <c r="L132" s="4"/>
+      <c r="M132" s="4"/>
+      <c r="N132" s="4"/>
+      <c r="O132" s="4"/>
+      <c r="P132" s="4"/>
+      <c r="Q132" s="4"/>
+      <c r="R132" s="3"/>
+      <c r="S132" s="4"/>
+      <c r="T132" s="4"/>
+    </row>
+    <row r="133" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B133" s="4"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="4"/>
+      <c r="E133" s="3"/>
+      <c r="F133" s="4"/>
+      <c r="G133" s="3"/>
+      <c r="H133" s="4"/>
+      <c r="I133" s="3"/>
+      <c r="J133" s="4"/>
+      <c r="K133" s="4"/>
+      <c r="L133" s="4"/>
+      <c r="M133" s="4"/>
+      <c r="N133" s="4"/>
+      <c r="O133" s="4"/>
+      <c r="P133" s="4"/>
+      <c r="Q133" s="4"/>
+      <c r="R133" s="3"/>
+      <c r="S133" s="4"/>
+      <c r="T133" s="4"/>
+    </row>
+    <row r="134" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B134" s="4"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="4"/>
+      <c r="G134" s="3"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="3"/>
+      <c r="J134" s="4"/>
+      <c r="K134" s="4"/>
+      <c r="L134" s="4"/>
+      <c r="M134" s="4"/>
+      <c r="N134" s="4"/>
+      <c r="O134" s="4"/>
+      <c r="P134" s="4"/>
+      <c r="Q134" s="4"/>
+      <c r="R134" s="3"/>
+      <c r="S134" s="4"/>
+      <c r="T134" s="4"/>
+    </row>
+    <row r="135" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B135" s="4"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="3"/>
+      <c r="H135" s="4"/>
+      <c r="I135" s="3"/>
+      <c r="J135" s="4"/>
+      <c r="K135" s="4"/>
+      <c r="L135" s="4"/>
+      <c r="M135" s="4"/>
+      <c r="N135" s="4"/>
+      <c r="O135" s="4"/>
+      <c r="P135" s="4"/>
+      <c r="Q135" s="4"/>
+      <c r="R135" s="3"/>
+      <c r="S135" s="4"/>
+      <c r="T135" s="4"/>
+    </row>
+    <row r="136" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B136" s="4"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="3"/>
+      <c r="H136" s="4"/>
+      <c r="I136" s="3"/>
+      <c r="J136" s="4"/>
+      <c r="K136" s="4"/>
+      <c r="L136" s="4"/>
+      <c r="M136" s="4"/>
+      <c r="N136" s="4"/>
+      <c r="O136" s="4"/>
+      <c r="P136" s="4"/>
+      <c r="Q136" s="4"/>
+      <c r="R136" s="3"/>
+      <c r="S136" s="4"/>
+      <c r="T136" s="4"/>
+    </row>
+    <row r="137" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B137" s="4"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="3"/>
+      <c r="H137" s="4"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="4"/>
+      <c r="K137" s="4"/>
+      <c r="L137" s="4"/>
+      <c r="M137" s="4"/>
+      <c r="N137" s="4"/>
+      <c r="O137" s="4"/>
+      <c r="P137" s="4"/>
+      <c r="Q137" s="4"/>
+      <c r="R137" s="3"/>
+      <c r="S137" s="4"/>
+      <c r="T137" s="4"/>
+    </row>
+    <row r="138" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B138" s="4"/>
+      <c r="C138" s="3"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="4"/>
+      <c r="G138" s="3"/>
+      <c r="H138" s="4"/>
+      <c r="I138" s="3"/>
+      <c r="J138" s="4"/>
+      <c r="K138" s="4"/>
+      <c r="L138" s="4"/>
+      <c r="M138" s="4"/>
+      <c r="N138" s="4"/>
+      <c r="O138" s="4"/>
+      <c r="P138" s="4"/>
+      <c r="Q138" s="4"/>
+      <c r="R138" s="3"/>
+      <c r="S138" s="4"/>
+      <c r="T138" s="4"/>
+    </row>
+    <row r="139" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B139" s="4"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="4"/>
+      <c r="E139" s="3"/>
+      <c r="F139" s="4"/>
+      <c r="G139" s="3"/>
+      <c r="H139" s="4"/>
+      <c r="I139" s="3"/>
+      <c r="J139" s="4"/>
+      <c r="K139" s="4"/>
+      <c r="L139" s="4"/>
+      <c r="M139" s="4"/>
+      <c r="N139" s="4"/>
+      <c r="O139" s="4"/>
+      <c r="P139" s="4"/>
+      <c r="Q139" s="4"/>
+      <c r="R139" s="3"/>
+      <c r="S139" s="4"/>
+      <c r="T139" s="4"/>
+    </row>
+    <row r="140" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B140" s="4"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="4"/>
+      <c r="G140" s="3"/>
+      <c r="H140" s="4"/>
+      <c r="I140" s="3"/>
+      <c r="J140" s="4"/>
+      <c r="K140" s="4"/>
+      <c r="L140" s="4"/>
+      <c r="M140" s="4"/>
+      <c r="N140" s="4"/>
+      <c r="O140" s="4"/>
+      <c r="P140" s="4"/>
+      <c r="Q140" s="4"/>
+      <c r="R140" s="3"/>
+      <c r="S140" s="4"/>
+      <c r="T140" s="4"/>
+    </row>
+    <row r="141" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B141" s="4"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="4"/>
+      <c r="E141" s="3"/>
+      <c r="F141" s="4"/>
+      <c r="G141" s="3"/>
+      <c r="H141" s="4"/>
+      <c r="I141" s="3"/>
+      <c r="J141" s="4"/>
+      <c r="K141" s="4"/>
+      <c r="L141" s="4"/>
+      <c r="M141" s="4"/>
+      <c r="N141" s="4"/>
+      <c r="O141" s="4"/>
+      <c r="P141" s="4"/>
+      <c r="Q141" s="4"/>
+      <c r="R141" s="3"/>
+      <c r="S141" s="4"/>
+      <c r="T141" s="4"/>
+    </row>
+    <row r="142" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B142" s="4"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="4"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="3"/>
+      <c r="H142" s="4"/>
+      <c r="I142" s="3"/>
+      <c r="J142" s="4"/>
+      <c r="K142" s="4"/>
+      <c r="L142" s="4"/>
+      <c r="M142" s="4"/>
+      <c r="N142" s="4"/>
+      <c r="O142" s="4"/>
+      <c r="P142" s="4"/>
+      <c r="Q142" s="4"/>
+      <c r="R142" s="3"/>
+      <c r="S142" s="4"/>
+      <c r="T142" s="4"/>
+    </row>
+    <row r="143" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B143" s="4"/>
+      <c r="C143" s="3"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="3"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="3"/>
+      <c r="H143" s="4"/>
+      <c r="I143" s="3"/>
+      <c r="J143" s="4"/>
+      <c r="K143" s="4"/>
+      <c r="L143" s="4"/>
+      <c r="M143" s="4"/>
+      <c r="N143" s="4"/>
+      <c r="O143" s="4"/>
+      <c r="P143" s="4"/>
+      <c r="Q143" s="4"/>
+      <c r="R143" s="3"/>
+      <c r="S143" s="4"/>
+      <c r="T143" s="4"/>
+    </row>
+    <row r="144" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B144" s="4"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="3"/>
+      <c r="H144" s="4"/>
+      <c r="I144" s="3"/>
+      <c r="J144" s="4"/>
+      <c r="K144" s="4"/>
+      <c r="L144" s="4"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="4"/>
+      <c r="O144" s="4"/>
+      <c r="P144" s="4"/>
+      <c r="Q144" s="4"/>
+      <c r="R144" s="3"/>
+      <c r="S144" s="4"/>
+      <c r="T144" s="4"/>
+    </row>
+    <row r="145" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B145" s="4"/>
+      <c r="C145" s="3"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="3"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="3"/>
+      <c r="H145" s="4"/>
+      <c r="I145" s="3"/>
+      <c r="J145" s="4"/>
+      <c r="K145" s="4"/>
+      <c r="L145" s="4"/>
+      <c r="M145" s="4"/>
+      <c r="N145" s="4"/>
+      <c r="O145" s="4"/>
+      <c r="P145" s="4"/>
+      <c r="Q145" s="4"/>
+      <c r="R145" s="3"/>
+      <c r="S145" s="4"/>
+      <c r="T145" s="4"/>
+    </row>
+    <row r="146" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B146" s="4"/>
+      <c r="C146" s="3"/>
+      <c r="D146" s="4"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="3"/>
+      <c r="H146" s="4"/>
+      <c r="I146" s="3"/>
+      <c r="J146" s="4"/>
+      <c r="K146" s="4"/>
+      <c r="L146" s="4"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="4"/>
+      <c r="O146" s="4"/>
+      <c r="P146" s="4"/>
+      <c r="Q146" s="4"/>
+      <c r="R146" s="3"/>
+      <c r="S146" s="4"/>
+      <c r="T146" s="4"/>
+    </row>
+    <row r="147" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B147" s="4"/>
+      <c r="C147" s="3"/>
+      <c r="D147" s="4"/>
+      <c r="E147" s="3"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="3"/>
+      <c r="H147" s="4"/>
+      <c r="I147" s="3"/>
+      <c r="J147" s="4"/>
+      <c r="K147" s="4"/>
+      <c r="L147" s="4"/>
+      <c r="M147" s="4"/>
+      <c r="N147" s="4"/>
+      <c r="O147" s="4"/>
+      <c r="P147" s="4"/>
+      <c r="Q147" s="4"/>
+      <c r="R147" s="3"/>
+      <c r="S147" s="4"/>
+      <c r="T147" s="4"/>
+    </row>
+    <row r="148" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B148" s="4"/>
+      <c r="C148" s="3"/>
+      <c r="D148" s="4"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="3"/>
+      <c r="H148" s="4"/>
+      <c r="I148" s="3"/>
+      <c r="J148" s="4"/>
+      <c r="K148" s="4"/>
+      <c r="L148" s="4"/>
+      <c r="M148" s="4"/>
+      <c r="N148" s="4"/>
+      <c r="O148" s="4"/>
+      <c r="P148" s="4"/>
+      <c r="Q148" s="4"/>
+      <c r="R148" s="3"/>
+      <c r="S148" s="4"/>
+      <c r="T148" s="4"/>
+    </row>
+    <row r="149" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B149" s="4"/>
+      <c r="C149" s="3"/>
+      <c r="D149" s="4"/>
+      <c r="E149" s="3"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="3"/>
+      <c r="H149" s="4"/>
+      <c r="I149" s="3"/>
+      <c r="J149" s="4"/>
+      <c r="K149" s="4"/>
+      <c r="L149" s="4"/>
+      <c r="M149" s="4"/>
+      <c r="N149" s="4"/>
+      <c r="O149" s="4"/>
+      <c r="P149" s="4"/>
+      <c r="Q149" s="4"/>
+      <c r="R149" s="3"/>
+      <c r="S149" s="4"/>
+      <c r="T149" s="4"/>
+    </row>
+    <row r="150" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B150" s="4"/>
+      <c r="C150" s="3"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="3"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="3"/>
+      <c r="H150" s="4"/>
+      <c r="I150" s="3"/>
+      <c r="J150" s="4"/>
+      <c r="K150" s="4"/>
+      <c r="L150" s="4"/>
+      <c r="M150" s="4"/>
+      <c r="N150" s="4"/>
+      <c r="O150" s="4"/>
+      <c r="P150" s="4"/>
+      <c r="Q150" s="4"/>
+      <c r="R150" s="3"/>
+      <c r="S150" s="4"/>
+      <c r="T150" s="4"/>
+    </row>
+    <row r="151" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B151" s="4"/>
+      <c r="C151" s="3"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="3"/>
+      <c r="F151" s="4"/>
+      <c r="G151" s="3"/>
+      <c r="H151" s="4"/>
+      <c r="I151" s="3"/>
+      <c r="J151" s="4"/>
+      <c r="K151" s="4"/>
+      <c r="L151" s="4"/>
+      <c r="M151" s="4"/>
+      <c r="N151" s="4"/>
+      <c r="O151" s="4"/>
+      <c r="P151" s="4"/>
+      <c r="Q151" s="4"/>
+      <c r="R151" s="3"/>
+      <c r="S151" s="4"/>
+      <c r="T151" s="4"/>
+    </row>
+    <row r="152" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B152" s="4"/>
+      <c r="C152" s="3"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="3"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="3"/>
+      <c r="H152" s="4"/>
+      <c r="I152" s="3"/>
+      <c r="J152" s="4"/>
+      <c r="K152" s="4"/>
+      <c r="L152" s="4"/>
+      <c r="M152" s="4"/>
+      <c r="N152" s="4"/>
+      <c r="O152" s="4"/>
+      <c r="P152" s="4"/>
+      <c r="Q152" s="4"/>
+      <c r="R152" s="3"/>
+      <c r="S152" s="4"/>
+      <c r="T152" s="4"/>
+    </row>
+    <row r="153" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B153" s="4"/>
+      <c r="C153" s="3"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="3"/>
+      <c r="F153" s="4"/>
+      <c r="G153" s="3"/>
+      <c r="H153" s="4"/>
+      <c r="I153" s="3"/>
+      <c r="J153" s="4"/>
+      <c r="K153" s="4"/>
+      <c r="L153" s="4"/>
+      <c r="M153" s="4"/>
+      <c r="N153" s="4"/>
+      <c r="O153" s="4"/>
+      <c r="P153" s="4"/>
+      <c r="Q153" s="4"/>
+      <c r="R153" s="3"/>
+      <c r="S153" s="4"/>
+      <c r="T153" s="4"/>
+    </row>
+    <row r="154" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B154" s="4"/>
+      <c r="C154" s="3"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="3"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="3"/>
+      <c r="H154" s="4"/>
+      <c r="I154" s="3"/>
+      <c r="J154" s="4"/>
+      <c r="K154" s="4"/>
+      <c r="L154" s="4"/>
+      <c r="M154" s="4"/>
+      <c r="N154" s="4"/>
+      <c r="O154" s="4"/>
+      <c r="P154" s="4"/>
+      <c r="Q154" s="4"/>
+      <c r="R154" s="3"/>
+      <c r="S154" s="4"/>
+      <c r="T154" s="4"/>
+    </row>
+    <row r="155" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B155" s="4"/>
+      <c r="C155" s="3"/>
+      <c r="D155" s="4"/>
+      <c r="E155" s="3"/>
+      <c r="F155" s="4"/>
+      <c r="G155" s="3"/>
+      <c r="H155" s="4"/>
+      <c r="I155" s="3"/>
+      <c r="J155" s="4"/>
+      <c r="K155" s="4"/>
+      <c r="L155" s="4"/>
+      <c r="M155" s="4"/>
+      <c r="N155" s="4"/>
+      <c r="O155" s="4"/>
+      <c r="P155" s="4"/>
+      <c r="Q155" s="4"/>
+      <c r="R155" s="3"/>
+      <c r="S155" s="4"/>
+      <c r="T155" s="4"/>
+    </row>
+    <row r="156" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B156" s="4"/>
+      <c r="C156" s="3"/>
+      <c r="D156" s="4"/>
+      <c r="E156" s="3"/>
+      <c r="F156" s="4"/>
+      <c r="G156" s="3"/>
+      <c r="H156" s="4"/>
+      <c r="I156" s="3"/>
+      <c r="J156" s="4"/>
+      <c r="K156" s="4"/>
+      <c r="L156" s="4"/>
+      <c r="M156" s="4"/>
+      <c r="N156" s="4"/>
+      <c r="O156" s="4"/>
+      <c r="P156" s="4"/>
+      <c r="Q156" s="4"/>
+      <c r="R156" s="3"/>
+      <c r="S156" s="4"/>
+      <c r="T156" s="4"/>
+    </row>
+    <row r="157" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B157" s="4"/>
+      <c r="C157" s="3"/>
+      <c r="D157" s="4"/>
+      <c r="E157" s="3"/>
+      <c r="F157" s="4"/>
+      <c r="G157" s="3"/>
+      <c r="H157" s="4"/>
+      <c r="I157" s="3"/>
+      <c r="J157" s="4"/>
+      <c r="K157" s="4"/>
+      <c r="L157" s="4"/>
+      <c r="M157" s="4"/>
+      <c r="N157" s="4"/>
+      <c r="O157" s="4"/>
+      <c r="P157" s="4"/>
+      <c r="Q157" s="4"/>
+      <c r="R157" s="3"/>
+      <c r="S157" s="4"/>
+      <c r="T157" s="4"/>
+    </row>
+    <row r="158" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B158" s="4"/>
+      <c r="C158" s="3"/>
+      <c r="D158" s="4"/>
+      <c r="E158" s="3"/>
+      <c r="F158" s="4"/>
+      <c r="G158" s="3"/>
+      <c r="H158" s="4"/>
+      <c r="I158" s="3"/>
+      <c r="J158" s="4"/>
+      <c r="K158" s="4"/>
+      <c r="L158" s="4"/>
+      <c r="M158" s="4"/>
+      <c r="N158" s="4"/>
+      <c r="O158" s="4"/>
+      <c r="P158" s="4"/>
+      <c r="Q158" s="4"/>
+      <c r="R158" s="3"/>
+      <c r="S158" s="4"/>
+      <c r="T158" s="4"/>
+    </row>
+    <row r="159" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B159" s="4"/>
+      <c r="C159" s="3"/>
+      <c r="D159" s="4"/>
+      <c r="E159" s="3"/>
+      <c r="F159" s="4"/>
+      <c r="G159" s="3"/>
+      <c r="H159" s="4"/>
+      <c r="I159" s="3"/>
+      <c r="J159" s="4"/>
+      <c r="K159" s="4"/>
+      <c r="L159" s="4"/>
+      <c r="M159" s="4"/>
+      <c r="N159" s="4"/>
+      <c r="O159" s="4"/>
+      <c r="P159" s="4"/>
+      <c r="Q159" s="4"/>
+      <c r="R159" s="3"/>
+      <c r="S159" s="4"/>
+      <c r="T159" s="4"/>
+    </row>
+    <row r="160" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B160" s="4"/>
+      <c r="C160" s="3"/>
+      <c r="D160" s="4"/>
+      <c r="E160" s="3"/>
+      <c r="F160" s="4"/>
+      <c r="G160" s="3"/>
+      <c r="H160" s="4"/>
+      <c r="I160" s="3"/>
+      <c r="J160" s="4"/>
+      <c r="K160" s="4"/>
+      <c r="L160" s="4"/>
+      <c r="M160" s="4"/>
+      <c r="N160" s="4"/>
+      <c r="O160" s="4"/>
+      <c r="P160" s="4"/>
+      <c r="Q160" s="4"/>
+      <c r="R160" s="3"/>
+      <c r="S160" s="4"/>
+      <c r="T160" s="4"/>
+    </row>
+    <row r="161" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B161" s="4"/>
+      <c r="C161" s="3"/>
+      <c r="D161" s="4"/>
+      <c r="E161" s="3"/>
+      <c r="F161" s="4"/>
+      <c r="G161" s="3"/>
+      <c r="H161" s="4"/>
+      <c r="I161" s="3"/>
+      <c r="J161" s="4"/>
+      <c r="K161" s="4"/>
+      <c r="L161" s="4"/>
+      <c r="M161" s="4"/>
+      <c r="N161" s="4"/>
+      <c r="O161" s="4"/>
+      <c r="P161" s="4"/>
+      <c r="Q161" s="4"/>
+      <c r="R161" s="3"/>
+      <c r="S161" s="4"/>
+      <c r="T161" s="4"/>
+    </row>
+    <row r="162" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B162" s="4"/>
+      <c r="C162" s="3"/>
+      <c r="D162" s="4"/>
+      <c r="E162" s="3"/>
+      <c r="F162" s="4"/>
+      <c r="G162" s="3"/>
+      <c r="H162" s="4"/>
+      <c r="I162" s="3"/>
+      <c r="J162" s="4"/>
+      <c r="K162" s="4"/>
+      <c r="L162" s="4"/>
+      <c r="M162" s="4"/>
+      <c r="N162" s="4"/>
+      <c r="O162" s="4"/>
+      <c r="P162" s="4"/>
+      <c r="Q162" s="4"/>
+      <c r="R162" s="3"/>
+      <c r="S162" s="4"/>
+      <c r="T162" s="4"/>
+    </row>
+    <row r="163" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B163" s="4"/>
+      <c r="C163" s="3"/>
+      <c r="D163" s="4"/>
+      <c r="E163" s="3"/>
+      <c r="F163" s="4"/>
+      <c r="G163" s="3"/>
+      <c r="H163" s="4"/>
+      <c r="I163" s="3"/>
+      <c r="J163" s="4"/>
+      <c r="K163" s="4"/>
+      <c r="L163" s="4"/>
+      <c r="M163" s="4"/>
+      <c r="N163" s="4"/>
+      <c r="O163" s="4"/>
+      <c r="P163" s="4"/>
+      <c r="Q163" s="4"/>
+      <c r="R163" s="3"/>
+      <c r="S163" s="4"/>
+      <c r="T163" s="4"/>
+    </row>
+    <row r="164" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B164" s="4"/>
+      <c r="C164" s="3"/>
+      <c r="D164" s="4"/>
+      <c r="E164" s="3"/>
+      <c r="F164" s="4"/>
+      <c r="G164" s="3"/>
+      <c r="H164" s="4"/>
+      <c r="I164" s="3"/>
+      <c r="J164" s="4"/>
+      <c r="K164" s="4"/>
+      <c r="L164" s="4"/>
+      <c r="M164" s="4"/>
+      <c r="N164" s="4"/>
+      <c r="O164" s="4"/>
+      <c r="P164" s="4"/>
+      <c r="Q164" s="4"/>
+      <c r="R164" s="3"/>
+      <c r="S164" s="4"/>
+      <c r="T164" s="4"/>
+    </row>
+    <row r="165" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B165" s="4"/>
+      <c r="C165" s="3"/>
+      <c r="D165" s="4"/>
+      <c r="E165" s="3"/>
+      <c r="F165" s="4"/>
+      <c r="G165" s="3"/>
+      <c r="H165" s="4"/>
+      <c r="I165" s="3"/>
+      <c r="J165" s="4"/>
+      <c r="K165" s="4"/>
+      <c r="L165" s="4"/>
+      <c r="M165" s="4"/>
+      <c r="N165" s="4"/>
+      <c r="O165" s="4"/>
+      <c r="P165" s="4"/>
+      <c r="Q165" s="4"/>
+      <c r="R165" s="3"/>
+      <c r="S165" s="4"/>
+      <c r="T165" s="4"/>
+    </row>
+    <row r="166" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B166" s="4"/>
+      <c r="C166" s="3"/>
+      <c r="D166" s="4"/>
+      <c r="E166" s="3"/>
+      <c r="F166" s="4"/>
+      <c r="G166" s="3"/>
+      <c r="H166" s="4"/>
+      <c r="I166" s="3"/>
+      <c r="J166" s="4"/>
+      <c r="K166" s="4"/>
+      <c r="L166" s="4"/>
+      <c r="M166" s="4"/>
+      <c r="N166" s="4"/>
+      <c r="O166" s="4"/>
+      <c r="P166" s="4"/>
+      <c r="Q166" s="4"/>
+      <c r="R166" s="3"/>
+      <c r="S166" s="4"/>
+      <c r="T166" s="4"/>
+    </row>
+    <row r="167" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B167" s="4"/>
+      <c r="C167" s="3"/>
+      <c r="D167" s="4"/>
+      <c r="E167" s="3"/>
+      <c r="F167" s="4"/>
+      <c r="G167" s="3"/>
+      <c r="H167" s="4"/>
+      <c r="I167" s="3"/>
+      <c r="J167" s="4"/>
+      <c r="K167" s="4"/>
+      <c r="L167" s="4"/>
+      <c r="M167" s="4"/>
+      <c r="N167" s="4"/>
+      <c r="O167" s="4"/>
+      <c r="P167" s="4"/>
+      <c r="Q167" s="4"/>
+      <c r="R167" s="3"/>
+      <c r="S167" s="4"/>
+      <c r="T167" s="4"/>
+    </row>
+    <row r="168" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B168" s="4"/>
+      <c r="C168" s="3"/>
+      <c r="D168" s="4"/>
+      <c r="E168" s="3"/>
+      <c r="F168" s="4"/>
+      <c r="G168" s="3"/>
+      <c r="H168" s="4"/>
+      <c r="I168" s="3"/>
+      <c r="J168" s="4"/>
+      <c r="K168" s="4"/>
+      <c r="L168" s="4"/>
+      <c r="M168" s="4"/>
+      <c r="N168" s="4"/>
+      <c r="O168" s="4"/>
+      <c r="P168" s="4"/>
+      <c r="Q168" s="4"/>
+      <c r="R168" s="3"/>
+      <c r="S168" s="4"/>
+      <c r="T168" s="4"/>
+    </row>
+    <row r="169" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B169" s="4"/>
+      <c r="C169" s="3"/>
+      <c r="D169" s="4"/>
+      <c r="E169" s="3"/>
+      <c r="F169" s="4"/>
+      <c r="G169" s="3"/>
+      <c r="H169" s="4"/>
+      <c r="I169" s="3"/>
+      <c r="J169" s="4"/>
+      <c r="K169" s="4"/>
+      <c r="L169" s="4"/>
+      <c r="M169" s="4"/>
+      <c r="N169" s="4"/>
+      <c r="O169" s="4"/>
+      <c r="P169" s="4"/>
+      <c r="Q169" s="4"/>
+      <c r="R169" s="3"/>
+      <c r="S169" s="4"/>
+      <c r="T169" s="4"/>
+    </row>
+    <row r="170" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B170" s="4"/>
+      <c r="C170" s="3"/>
+      <c r="D170" s="4"/>
+      <c r="E170" s="3"/>
+      <c r="F170" s="4"/>
+      <c r="G170" s="3"/>
+      <c r="H170" s="4"/>
+      <c r="I170" s="3"/>
+      <c r="J170" s="4"/>
+      <c r="K170" s="4"/>
+      <c r="L170" s="4"/>
+      <c r="M170" s="4"/>
+      <c r="N170" s="4"/>
+      <c r="O170" s="4"/>
+      <c r="P170" s="4"/>
+      <c r="Q170" s="4"/>
+      <c r="R170" s="3"/>
+      <c r="S170" s="4"/>
+      <c r="T170" s="4"/>
+    </row>
+    <row r="171" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B171" s="4"/>
+      <c r="C171" s="3"/>
+      <c r="D171" s="4"/>
+      <c r="E171" s="3"/>
+      <c r="F171" s="4"/>
+      <c r="G171" s="3"/>
+      <c r="H171" s="4"/>
+      <c r="I171" s="3"/>
+      <c r="J171" s="4"/>
+      <c r="K171" s="4"/>
+      <c r="L171" s="4"/>
+      <c r="M171" s="4"/>
+      <c r="N171" s="4"/>
+      <c r="O171" s="4"/>
+      <c r="P171" s="4"/>
+      <c r="Q171" s="4"/>
+      <c r="R171" s="3"/>
+      <c r="S171" s="4"/>
+      <c r="T171" s="4"/>
+    </row>
+    <row r="172" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B172" s="4"/>
+      <c r="C172" s="3"/>
+      <c r="D172" s="4"/>
+      <c r="E172" s="3"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="3"/>
+      <c r="H172" s="4"/>
+      <c r="I172" s="3"/>
+      <c r="J172" s="4"/>
+      <c r="K172" s="4"/>
+      <c r="L172" s="4"/>
+      <c r="M172" s="4"/>
+      <c r="N172" s="4"/>
+      <c r="O172" s="4"/>
+      <c r="P172" s="4"/>
+      <c r="Q172" s="4"/>
+      <c r="R172" s="3"/>
+      <c r="S172" s="4"/>
+      <c r="T172" s="4"/>
+    </row>
+    <row r="173" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B173" s="4"/>
+      <c r="C173" s="3"/>
+      <c r="D173" s="4"/>
+      <c r="E173" s="3"/>
+      <c r="F173" s="4"/>
+      <c r="G173" s="3"/>
+      <c r="H173" s="4"/>
+      <c r="I173" s="3"/>
+      <c r="J173" s="4"/>
+      <c r="K173" s="4"/>
+      <c r="L173" s="4"/>
+      <c r="M173" s="4"/>
+      <c r="N173" s="4"/>
+      <c r="O173" s="4"/>
+      <c r="P173" s="4"/>
+      <c r="Q173" s="4"/>
+      <c r="R173" s="3"/>
+      <c r="S173" s="4"/>
+      <c r="T173" s="4"/>
+    </row>
+    <row r="174" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B174" s="4"/>
+      <c r="C174" s="3"/>
+      <c r="D174" s="4"/>
+      <c r="E174" s="3"/>
+      <c r="F174" s="4"/>
+      <c r="G174" s="3"/>
+      <c r="H174" s="4"/>
+      <c r="I174" s="3"/>
+      <c r="J174" s="4"/>
+      <c r="K174" s="4"/>
+      <c r="L174" s="4"/>
+      <c r="M174" s="4"/>
+      <c r="N174" s="4"/>
+      <c r="O174" s="4"/>
+      <c r="P174" s="4"/>
+      <c r="Q174" s="4"/>
+      <c r="R174" s="3"/>
+      <c r="S174" s="4"/>
+      <c r="T174" s="4"/>
+    </row>
+    <row r="175" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B175" s="4"/>
+      <c r="C175" s="3"/>
+      <c r="D175" s="4"/>
+      <c r="E175" s="3"/>
+      <c r="F175" s="4"/>
+      <c r="G175" s="3"/>
+      <c r="H175" s="4"/>
+      <c r="I175" s="3"/>
+      <c r="J175" s="4"/>
+      <c r="K175" s="4"/>
+      <c r="L175" s="4"/>
+      <c r="M175" s="4"/>
+      <c r="N175" s="4"/>
+      <c r="O175" s="4"/>
+      <c r="P175" s="4"/>
+      <c r="Q175" s="4"/>
+      <c r="R175" s="3"/>
+      <c r="S175" s="4"/>
+      <c r="T175" s="4"/>
+    </row>
+    <row r="176" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B176" s="4"/>
+      <c r="C176" s="3"/>
+      <c r="D176" s="4"/>
+      <c r="E176" s="3"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="3"/>
+      <c r="H176" s="4"/>
+      <c r="I176" s="3"/>
+      <c r="J176" s="4"/>
+      <c r="K176" s="4"/>
+      <c r="L176" s="4"/>
+      <c r="M176" s="4"/>
+      <c r="N176" s="4"/>
+      <c r="O176" s="4"/>
+      <c r="P176" s="4"/>
+      <c r="Q176" s="4"/>
+      <c r="R176" s="3"/>
+      <c r="S176" s="4"/>
+      <c r="T176" s="4"/>
+    </row>
+    <row r="177" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B177" s="4"/>
+      <c r="C177" s="3"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="3"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="3"/>
+      <c r="H177" s="4"/>
+      <c r="I177" s="3"/>
+      <c r="J177" s="4"/>
+      <c r="K177" s="4"/>
+      <c r="L177" s="4"/>
+      <c r="M177" s="4"/>
+      <c r="N177" s="4"/>
+      <c r="O177" s="4"/>
+      <c r="P177" s="4"/>
+      <c r="Q177" s="4"/>
+      <c r="R177" s="3"/>
+      <c r="S177" s="4"/>
+      <c r="T177" s="4"/>
+    </row>
+    <row r="178" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B178" s="4"/>
+      <c r="C178" s="3"/>
+      <c r="D178" s="4"/>
+      <c r="E178" s="3"/>
+      <c r="F178" s="4"/>
+      <c r="G178" s="3"/>
+      <c r="H178" s="4"/>
+      <c r="I178" s="3"/>
+      <c r="J178" s="4"/>
+      <c r="K178" s="4"/>
+      <c r="L178" s="4"/>
+      <c r="M178" s="4"/>
+      <c r="N178" s="4"/>
+      <c r="O178" s="4"/>
+      <c r="P178" s="4"/>
+      <c r="Q178" s="4"/>
+      <c r="R178" s="3"/>
+      <c r="S178" s="4"/>
+      <c r="T178" s="4"/>
+    </row>
+    <row r="179" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B179" s="4"/>
+      <c r="C179" s="3"/>
+      <c r="D179" s="4"/>
+      <c r="E179" s="3"/>
+      <c r="F179" s="4"/>
+      <c r="G179" s="3"/>
+      <c r="H179" s="4"/>
+      <c r="I179" s="3"/>
+      <c r="J179" s="4"/>
+      <c r="K179" s="4"/>
+      <c r="L179" s="4"/>
+      <c r="M179" s="4"/>
+      <c r="N179" s="4"/>
+      <c r="O179" s="4"/>
+      <c r="P179" s="4"/>
+      <c r="Q179" s="4"/>
+      <c r="R179" s="3"/>
+      <c r="S179" s="4"/>
+      <c r="T179" s="4"/>
+    </row>
+    <row r="180" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B180" s="4"/>
+      <c r="C180" s="3"/>
+      <c r="D180" s="4"/>
+      <c r="E180" s="3"/>
+      <c r="F180" s="4"/>
+      <c r="G180" s="3"/>
+      <c r="H180" s="4"/>
+      <c r="I180" s="3"/>
+      <c r="J180" s="4"/>
+      <c r="K180" s="4"/>
+      <c r="L180" s="4"/>
+      <c r="M180" s="4"/>
+      <c r="N180" s="4"/>
+      <c r="O180" s="4"/>
+      <c r="P180" s="4"/>
+      <c r="Q180" s="4"/>
+      <c r="R180" s="3"/>
+      <c r="S180" s="4"/>
+      <c r="T180" s="4"/>
+    </row>
+    <row r="181" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B181" s="4"/>
+      <c r="C181" s="3"/>
+      <c r="D181" s="4"/>
+      <c r="E181" s="3"/>
+      <c r="F181" s="4"/>
+      <c r="G181" s="3"/>
+      <c r="H181" s="4"/>
+      <c r="I181" s="3"/>
+      <c r="J181" s="4"/>
+      <c r="K181" s="4"/>
+      <c r="L181" s="4"/>
+      <c r="M181" s="4"/>
+      <c r="N181" s="4"/>
+      <c r="O181" s="4"/>
+      <c r="P181" s="4"/>
+      <c r="Q181" s="4"/>
+      <c r="R181" s="3"/>
+      <c r="S181" s="4"/>
+      <c r="T181" s="4"/>
+    </row>
+    <row r="182" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B182" s="4"/>
+      <c r="C182" s="3"/>
+      <c r="D182" s="4"/>
+      <c r="E182" s="3"/>
+      <c r="F182" s="4"/>
+      <c r="G182" s="3"/>
+      <c r="H182" s="4"/>
+      <c r="I182" s="3"/>
+      <c r="J182" s="4"/>
+      <c r="K182" s="4"/>
+      <c r="L182" s="4"/>
+      <c r="M182" s="4"/>
+      <c r="N182" s="4"/>
+      <c r="O182" s="4"/>
+      <c r="P182" s="4"/>
+      <c r="Q182" s="4"/>
+      <c r="R182" s="3"/>
+      <c r="S182" s="4"/>
+      <c r="T182" s="4"/>
+    </row>
+    <row r="183" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B183" s="4"/>
+      <c r="C183" s="3"/>
+      <c r="D183" s="4"/>
+      <c r="E183" s="3"/>
+      <c r="F183" s="4"/>
+      <c r="G183" s="3"/>
+      <c r="H183" s="4"/>
+      <c r="I183" s="3"/>
+      <c r="J183" s="4"/>
+      <c r="K183" s="4"/>
+      <c r="L183" s="4"/>
+      <c r="M183" s="4"/>
+      <c r="N183" s="4"/>
+      <c r="O183" s="4"/>
+      <c r="P183" s="4"/>
+      <c r="Q183" s="4"/>
+      <c r="R183" s="3"/>
+      <c r="S183" s="4"/>
+      <c r="T183" s="4"/>
+    </row>
+    <row r="184" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B184" s="4"/>
+      <c r="C184" s="3"/>
+      <c r="D184" s="4"/>
+      <c r="E184" s="3"/>
+      <c r="F184" s="4"/>
+      <c r="G184" s="3"/>
+      <c r="H184" s="4"/>
+      <c r="I184" s="3"/>
+      <c r="J184" s="4"/>
+      <c r="K184" s="4"/>
+      <c r="L184" s="4"/>
+      <c r="M184" s="4"/>
+      <c r="N184" s="4"/>
+      <c r="O184" s="4"/>
+      <c r="P184" s="4"/>
+      <c r="Q184" s="4"/>
+      <c r="R184" s="3"/>
+      <c r="S184" s="4"/>
+      <c r="T184" s="4"/>
+    </row>
+    <row r="185" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B185" s="4"/>
+      <c r="C185" s="3"/>
+      <c r="D185" s="4"/>
+      <c r="E185" s="3"/>
+      <c r="F185" s="4"/>
+      <c r="G185" s="3"/>
+      <c r="H185" s="4"/>
+      <c r="I185" s="3"/>
+      <c r="J185" s="4"/>
+      <c r="K185" s="4"/>
+      <c r="L185" s="4"/>
+      <c r="M185" s="4"/>
+      <c r="N185" s="4"/>
+      <c r="O185" s="4"/>
+      <c r="P185" s="4"/>
+      <c r="Q185" s="4"/>
+      <c r="R185" s="3"/>
+      <c r="S185" s="4"/>
+      <c r="T185" s="4"/>
+    </row>
+    <row r="186" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B186" s="4"/>
+      <c r="C186" s="3"/>
+      <c r="D186" s="4"/>
+      <c r="E186" s="3"/>
+      <c r="F186" s="4"/>
+      <c r="G186" s="3"/>
+      <c r="H186" s="4"/>
+      <c r="I186" s="3"/>
+      <c r="J186" s="4"/>
+      <c r="K186" s="4"/>
+      <c r="L186" s="4"/>
+      <c r="M186" s="4"/>
+      <c r="N186" s="4"/>
+      <c r="O186" s="4"/>
+      <c r="P186" s="4"/>
+      <c r="Q186" s="4"/>
+      <c r="R186" s="3"/>
+      <c r="S186" s="4"/>
+      <c r="T186" s="4"/>
+    </row>
+    <row r="187" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B187" s="4"/>
+      <c r="C187" s="3"/>
+      <c r="D187" s="4"/>
+      <c r="E187" s="3"/>
+      <c r="F187" s="4"/>
+      <c r="G187" s="3"/>
+      <c r="H187" s="4"/>
+      <c r="I187" s="3"/>
+      <c r="J187" s="4"/>
+      <c r="K187" s="4"/>
+      <c r="L187" s="4"/>
+      <c r="M187" s="4"/>
+      <c r="N187" s="4"/>
+      <c r="O187" s="4"/>
+      <c r="P187" s="4"/>
+      <c r="Q187" s="4"/>
+      <c r="R187" s="3"/>
+      <c r="S187" s="4"/>
+      <c r="T187" s="4"/>
+    </row>
+    <row r="188" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B188" s="4"/>
+      <c r="C188" s="3"/>
+      <c r="D188" s="4"/>
+      <c r="E188" s="3"/>
+      <c r="F188" s="4"/>
+      <c r="G188" s="3"/>
+      <c r="H188" s="4"/>
+      <c r="I188" s="3"/>
+      <c r="J188" s="4"/>
+      <c r="K188" s="4"/>
+      <c r="L188" s="4"/>
+      <c r="M188" s="4"/>
+      <c r="N188" s="4"/>
+      <c r="O188" s="4"/>
+      <c r="P188" s="4"/>
+      <c r="Q188" s="4"/>
+      <c r="R188" s="3"/>
+      <c r="S188" s="4"/>
+      <c r="T188" s="4"/>
+    </row>
+    <row r="189" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B189" s="4"/>
+      <c r="C189" s="3"/>
+      <c r="D189" s="4"/>
+      <c r="E189" s="3"/>
+      <c r="F189" s="4"/>
+      <c r="G189" s="3"/>
+      <c r="H189" s="4"/>
+      <c r="I189" s="3"/>
+      <c r="J189" s="4"/>
+      <c r="K189" s="4"/>
+      <c r="L189" s="4"/>
+      <c r="M189" s="4"/>
+      <c r="N189" s="4"/>
+      <c r="O189" s="4"/>
+      <c r="P189" s="4"/>
+      <c r="Q189" s="4"/>
+      <c r="R189" s="3"/>
+      <c r="S189" s="4"/>
+      <c r="T189" s="4"/>
+    </row>
+    <row r="190" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B190" s="4"/>
+      <c r="C190" s="3"/>
+      <c r="D190" s="4"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="4"/>
+      <c r="G190" s="3"/>
+      <c r="H190" s="4"/>
+      <c r="I190" s="3"/>
+      <c r="J190" s="4"/>
+      <c r="K190" s="4"/>
+      <c r="L190" s="4"/>
+      <c r="M190" s="4"/>
+      <c r="N190" s="4"/>
+      <c r="O190" s="4"/>
+      <c r="P190" s="4"/>
+      <c r="Q190" s="4"/>
+      <c r="R190" s="3"/>
+      <c r="S190" s="4"/>
+      <c r="T190" s="4"/>
+    </row>
+    <row r="191" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B191" s="4"/>
+      <c r="C191" s="3"/>
+      <c r="D191" s="4"/>
+      <c r="E191" s="3"/>
+      <c r="F191" s="4"/>
+      <c r="G191" s="3"/>
+      <c r="H191" s="4"/>
+      <c r="I191" s="3"/>
+      <c r="J191" s="4"/>
+      <c r="K191" s="4"/>
+      <c r="L191" s="4"/>
+      <c r="M191" s="4"/>
+      <c r="N191" s="4"/>
+      <c r="O191" s="4"/>
+      <c r="P191" s="4"/>
+      <c r="Q191" s="4"/>
+      <c r="R191" s="3"/>
+      <c r="S191" s="4"/>
+      <c r="T191" s="4"/>
+    </row>
+    <row r="192" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B192" s="4"/>
+      <c r="C192" s="3"/>
+      <c r="D192" s="4"/>
+      <c r="E192" s="3"/>
+      <c r="F192" s="4"/>
+      <c r="G192" s="3"/>
+      <c r="H192" s="4"/>
+      <c r="I192" s="3"/>
+      <c r="J192" s="4"/>
+      <c r="K192" s="4"/>
+      <c r="L192" s="4"/>
+      <c r="M192" s="4"/>
+      <c r="N192" s="4"/>
+      <c r="O192" s="4"/>
+      <c r="P192" s="4"/>
+      <c r="Q192" s="4"/>
+      <c r="R192" s="3"/>
+      <c r="S192" s="4"/>
+      <c r="T192" s="4"/>
+    </row>
+    <row r="193" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B193" s="4"/>
+      <c r="C193" s="3"/>
+      <c r="D193" s="4"/>
+      <c r="E193" s="3"/>
+      <c r="F193" s="4"/>
+      <c r="G193" s="3"/>
+      <c r="H193" s="4"/>
+      <c r="I193" s="3"/>
+      <c r="J193" s="4"/>
+      <c r="K193" s="4"/>
+      <c r="L193" s="4"/>
+      <c r="M193" s="4"/>
+      <c r="N193" s="4"/>
+      <c r="O193" s="4"/>
+      <c r="P193" s="4"/>
+      <c r="Q193" s="4"/>
+      <c r="R193" s="3"/>
+      <c r="S193" s="4"/>
+      <c r="T193" s="4"/>
+    </row>
+    <row r="194" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B194" s="4"/>
+      <c r="C194" s="3"/>
+      <c r="D194" s="4"/>
+      <c r="E194" s="3"/>
+      <c r="F194" s="4"/>
+      <c r="G194" s="3"/>
+      <c r="H194" s="4"/>
+      <c r="I194" s="3"/>
+      <c r="J194" s="4"/>
+      <c r="K194" s="4"/>
+      <c r="L194" s="4"/>
+      <c r="M194" s="4"/>
+      <c r="N194" s="4"/>
+      <c r="O194" s="4"/>
+      <c r="P194" s="4"/>
+      <c r="Q194" s="4"/>
+      <c r="R194" s="3"/>
+      <c r="S194" s="4"/>
+      <c r="T194" s="4"/>
+    </row>
+    <row r="195" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B195" s="4"/>
+      <c r="C195" s="3"/>
+      <c r="D195" s="4"/>
+      <c r="E195" s="3"/>
+      <c r="F195" s="4"/>
+      <c r="G195" s="3"/>
+      <c r="H195" s="4"/>
+      <c r="I195" s="3"/>
+      <c r="J195" s="4"/>
+      <c r="K195" s="4"/>
+      <c r="L195" s="4"/>
+      <c r="M195" s="4"/>
+      <c r="N195" s="4"/>
+      <c r="O195" s="4"/>
+      <c r="P195" s="4"/>
+      <c r="Q195" s="4"/>
+      <c r="R195" s="3"/>
+      <c r="S195" s="4"/>
+      <c r="T195" s="4"/>
+    </row>
+    <row r="196" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B196" s="4"/>
+      <c r="C196" s="3"/>
+      <c r="D196" s="4"/>
+      <c r="E196" s="3"/>
+      <c r="F196" s="4"/>
+      <c r="G196" s="3"/>
+      <c r="H196" s="4"/>
+      <c r="I196" s="3"/>
+      <c r="J196" s="4"/>
+      <c r="K196" s="4"/>
+      <c r="L196" s="4"/>
+      <c r="M196" s="4"/>
+      <c r="N196" s="4"/>
+      <c r="O196" s="4"/>
+      <c r="P196" s="4"/>
+      <c r="Q196" s="4"/>
+      <c r="R196" s="3"/>
+      <c r="S196" s="4"/>
+      <c r="T196" s="4"/>
+    </row>
+    <row r="197" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B197" s="4"/>
+      <c r="C197" s="3"/>
+      <c r="D197" s="4"/>
+      <c r="E197" s="3"/>
+      <c r="F197" s="4"/>
+      <c r="G197" s="3"/>
+      <c r="H197" s="4"/>
+      <c r="I197" s="3"/>
+      <c r="J197" s="4"/>
+      <c r="K197" s="4"/>
+      <c r="L197" s="4"/>
+      <c r="M197" s="4"/>
+      <c r="N197" s="4"/>
+      <c r="O197" s="4"/>
+      <c r="P197" s="4"/>
+      <c r="Q197" s="4"/>
+      <c r="R197" s="3"/>
+      <c r="S197" s="4"/>
+      <c r="T197" s="4"/>
+    </row>
+    <row r="198" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B198" s="4"/>
+      <c r="C198" s="3"/>
+      <c r="D198" s="4"/>
+      <c r="E198" s="3"/>
+      <c r="F198" s="4"/>
+      <c r="G198" s="3"/>
+      <c r="H198" s="4"/>
+      <c r="I198" s="3"/>
+      <c r="J198" s="4"/>
+      <c r="K198" s="4"/>
+      <c r="L198" s="4"/>
+      <c r="M198" s="4"/>
+      <c r="N198" s="4"/>
+      <c r="O198" s="4"/>
+      <c r="P198" s="4"/>
+      <c r="Q198" s="4"/>
+      <c r="R198" s="3"/>
+      <c r="S198" s="4"/>
+      <c r="T198" s="4"/>
+    </row>
+    <row r="199" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B199" s="4"/>
+      <c r="C199" s="3"/>
+      <c r="D199" s="4"/>
+      <c r="E199" s="3"/>
+      <c r="F199" s="4"/>
+      <c r="G199" s="3"/>
+      <c r="H199" s="4"/>
+      <c r="I199" s="3"/>
+      <c r="J199" s="4"/>
+      <c r="K199" s="4"/>
+      <c r="L199" s="4"/>
+      <c r="M199" s="4"/>
+      <c r="N199" s="4"/>
+      <c r="O199" s="4"/>
+      <c r="P199" s="4"/>
+      <c r="Q199" s="4"/>
+      <c r="R199" s="3"/>
+      <c r="S199" s="4"/>
+      <c r="T199" s="4"/>
+    </row>
+    <row r="200" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B200" s="4"/>
+      <c r="C200" s="3"/>
+      <c r="D200" s="4"/>
+      <c r="E200" s="3"/>
+      <c r="F200" s="4"/>
+      <c r="G200" s="3"/>
+      <c r="H200" s="4"/>
+      <c r="I200" s="3"/>
+      <c r="J200" s="4"/>
+      <c r="K200" s="4"/>
+      <c r="L200" s="4"/>
+      <c r="M200" s="4"/>
+      <c r="N200" s="4"/>
+      <c r="O200" s="4"/>
+      <c r="P200" s="4"/>
+      <c r="Q200" s="4"/>
+      <c r="R200" s="3"/>
+      <c r="S200" s="4"/>
+      <c r="T200" s="4"/>
+    </row>
+    <row r="201" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B201" s="4"/>
+      <c r="C201" s="3"/>
+      <c r="D201" s="4"/>
+      <c r="E201" s="3"/>
+      <c r="F201" s="4"/>
+      <c r="G201" s="3"/>
+      <c r="H201" s="4"/>
+      <c r="I201" s="3"/>
+      <c r="J201" s="4"/>
+      <c r="K201" s="4"/>
+      <c r="L201" s="4"/>
+      <c r="M201" s="4"/>
+      <c r="N201" s="4"/>
+      <c r="O201" s="4"/>
+      <c r="P201" s="4"/>
+      <c r="Q201" s="4"/>
+      <c r="R201" s="3"/>
+      <c r="S201" s="4"/>
+      <c r="T201" s="4"/>
+    </row>
+    <row r="202" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B202" s="4"/>
+      <c r="C202" s="3"/>
+      <c r="D202" s="4"/>
+      <c r="E202" s="3"/>
+      <c r="F202" s="4"/>
+      <c r="G202" s="3"/>
+      <c r="H202" s="4"/>
+      <c r="I202" s="3"/>
+      <c r="J202" s="4"/>
+      <c r="K202" s="4"/>
+      <c r="L202" s="4"/>
+      <c r="M202" s="4"/>
+      <c r="N202" s="4"/>
+      <c r="O202" s="4"/>
+      <c r="P202" s="4"/>
+      <c r="Q202" s="4"/>
+      <c r="R202" s="3"/>
+      <c r="S202" s="4"/>
+      <c r="T202" s="4"/>
+    </row>
+    <row r="203" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B203" s="4"/>
+      <c r="C203" s="3"/>
+      <c r="D203" s="4"/>
+      <c r="E203" s="3"/>
+      <c r="F203" s="4"/>
+      <c r="G203" s="3"/>
+      <c r="H203" s="4"/>
+      <c r="I203" s="3"/>
+      <c r="J203" s="4"/>
+      <c r="K203" s="4"/>
+      <c r="L203" s="4"/>
+      <c r="M203" s="4"/>
+      <c r="N203" s="4"/>
+      <c r="O203" s="4"/>
+      <c r="P203" s="4"/>
+      <c r="Q203" s="4"/>
+      <c r="R203" s="3"/>
+      <c r="S203" s="4"/>
+      <c r="T203" s="4"/>
+    </row>
+    <row r="204" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B204" s="4"/>
+      <c r="C204" s="3"/>
+      <c r="D204" s="4"/>
+      <c r="E204" s="3"/>
+      <c r="F204" s="4"/>
+      <c r="G204" s="3"/>
+      <c r="H204" s="4"/>
+      <c r="I204" s="3"/>
+      <c r="J204" s="4"/>
+      <c r="K204" s="4"/>
+      <c r="L204" s="4"/>
+      <c r="M204" s="4"/>
+      <c r="N204" s="4"/>
+      <c r="O204" s="4"/>
+      <c r="P204" s="4"/>
+      <c r="Q204" s="4"/>
+      <c r="R204" s="3"/>
+      <c r="S204" s="4"/>
+      <c r="T204" s="4"/>
+    </row>
+    <row r="205" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B205" s="4"/>
+      <c r="C205" s="3"/>
+      <c r="D205" s="4"/>
+      <c r="E205" s="3"/>
+      <c r="F205" s="4"/>
+      <c r="G205" s="3"/>
+      <c r="H205" s="4"/>
+      <c r="I205" s="3"/>
+      <c r="J205" s="4"/>
+      <c r="K205" s="4"/>
+      <c r="L205" s="4"/>
+      <c r="M205" s="4"/>
+      <c r="N205" s="4"/>
+      <c r="O205" s="4"/>
+      <c r="P205" s="4"/>
+      <c r="Q205" s="4"/>
+      <c r="R205" s="3"/>
+      <c r="S205" s="4"/>
+      <c r="T205" s="4"/>
+    </row>
+    <row r="206" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B206" s="4"/>
+      <c r="C206" s="3"/>
+      <c r="D206" s="4"/>
+      <c r="E206" s="3"/>
+      <c r="F206" s="4"/>
+      <c r="G206" s="3"/>
+      <c r="H206" s="4"/>
+      <c r="I206" s="3"/>
+      <c r="J206" s="4"/>
+      <c r="K206" s="4"/>
+      <c r="L206" s="4"/>
+      <c r="M206" s="4"/>
+      <c r="N206" s="4"/>
+      <c r="O206" s="4"/>
+      <c r="P206" s="4"/>
+      <c r="Q206" s="4"/>
+      <c r="R206" s="3"/>
+      <c r="S206" s="4"/>
+      <c r="T206" s="4"/>
+    </row>
+    <row r="207" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B207" s="4"/>
+      <c r="C207" s="3"/>
+      <c r="D207" s="4"/>
+      <c r="E207" s="3"/>
+      <c r="F207" s="4"/>
+      <c r="G207" s="3"/>
+      <c r="H207" s="4"/>
+      <c r="I207" s="3"/>
+      <c r="J207" s="4"/>
+      <c r="K207" s="4"/>
+      <c r="L207" s="4"/>
+      <c r="M207" s="4"/>
+      <c r="N207" s="4"/>
+      <c r="O207" s="4"/>
+      <c r="P207" s="4"/>
+      <c r="Q207" s="4"/>
+      <c r="R207" s="3"/>
+      <c r="S207" s="4"/>
+      <c r="T207" s="4"/>
+    </row>
+    <row r="208" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B208" s="4"/>
+      <c r="C208" s="3"/>
+      <c r="D208" s="4"/>
+      <c r="E208" s="3"/>
+      <c r="F208" s="4"/>
+      <c r="G208" s="3"/>
+      <c r="H208" s="4"/>
+      <c r="I208" s="3"/>
+      <c r="J208" s="4"/>
+      <c r="K208" s="4"/>
+      <c r="L208" s="4"/>
+      <c r="M208" s="4"/>
+      <c r="N208" s="4"/>
+      <c r="O208" s="4"/>
+      <c r="P208" s="4"/>
+      <c r="Q208" s="4"/>
+      <c r="R208" s="3"/>
+      <c r="S208" s="4"/>
+      <c r="T208" s="4"/>
+    </row>
+    <row r="209" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B209" s="4"/>
+      <c r="C209" s="3"/>
+      <c r="D209" s="4"/>
+      <c r="E209" s="3"/>
+      <c r="F209" s="4"/>
+      <c r="G209" s="3"/>
+      <c r="H209" s="4"/>
+      <c r="I209" s="3"/>
+      <c r="J209" s="4"/>
+      <c r="K209" s="4"/>
+      <c r="L209" s="4"/>
+      <c r="M209" s="4"/>
+      <c r="N209" s="4"/>
+      <c r="O209" s="4"/>
+      <c r="P209" s="4"/>
+      <c r="Q209" s="4"/>
+      <c r="R209" s="3"/>
+      <c r="S209" s="4"/>
+      <c r="T209" s="4"/>
+    </row>
+    <row r="210" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B210" s="4"/>
+      <c r="C210" s="3"/>
+      <c r="D210" s="4"/>
+      <c r="E210" s="3"/>
+      <c r="F210" s="4"/>
+      <c r="G210" s="3"/>
+      <c r="H210" s="4"/>
+      <c r="I210" s="3"/>
+      <c r="J210" s="4"/>
+      <c r="K210" s="4"/>
+      <c r="L210" s="4"/>
+      <c r="M210" s="4"/>
+      <c r="N210" s="4"/>
+      <c r="O210" s="4"/>
+      <c r="P210" s="4"/>
+      <c r="Q210" s="4"/>
+      <c r="R210" s="3"/>
+      <c r="S210" s="4"/>
+      <c r="T210" s="4"/>
+    </row>
+    <row r="211" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B211" s="4"/>
+      <c r="C211" s="3"/>
+      <c r="D211" s="4"/>
+      <c r="E211" s="3"/>
+      <c r="F211" s="4"/>
+      <c r="G211" s="3"/>
+      <c r="H211" s="4"/>
+      <c r="I211" s="3"/>
+      <c r="J211" s="4"/>
+      <c r="K211" s="4"/>
+      <c r="L211" s="4"/>
+      <c r="M211" s="4"/>
+      <c r="N211" s="4"/>
+      <c r="O211" s="4"/>
+      <c r="P211" s="4"/>
+      <c r="Q211" s="4"/>
+      <c r="R211" s="3"/>
+      <c r="S211" s="4"/>
+      <c r="T211" s="4"/>
+    </row>
+    <row r="212" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B212" s="4"/>
+      <c r="C212" s="3"/>
+      <c r="D212" s="4"/>
+      <c r="E212" s="3"/>
+      <c r="F212" s="4"/>
+      <c r="G212" s="3"/>
+      <c r="H212" s="4"/>
+      <c r="I212" s="3"/>
+      <c r="J212" s="4"/>
+      <c r="K212" s="4"/>
+      <c r="L212" s="4"/>
+      <c r="M212" s="4"/>
+      <c r="N212" s="4"/>
+      <c r="O212" s="4"/>
+      <c r="P212" s="4"/>
+      <c r="Q212" s="4"/>
+      <c r="R212" s="3"/>
+      <c r="S212" s="4"/>
+      <c r="T212" s="4"/>
+    </row>
+    <row r="213" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B213" s="4"/>
+      <c r="C213" s="3"/>
+      <c r="D213" s="4"/>
+      <c r="E213" s="3"/>
+      <c r="F213" s="4"/>
+      <c r="G213" s="3"/>
+      <c r="H213" s="4"/>
+      <c r="I213" s="3"/>
+      <c r="J213" s="4"/>
+      <c r="K213" s="4"/>
+      <c r="L213" s="4"/>
+      <c r="M213" s="4"/>
+      <c r="N213" s="4"/>
+      <c r="O213" s="4"/>
+      <c r="P213" s="4"/>
+      <c r="Q213" s="4"/>
+      <c r="R213" s="3"/>
+      <c r="S213" s="4"/>
+      <c r="T213" s="4"/>
+    </row>
+    <row r="214" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B214" s="4"/>
+      <c r="C214" s="3"/>
+      <c r="D214" s="4"/>
+      <c r="E214" s="3"/>
+      <c r="F214" s="4"/>
+      <c r="G214" s="3"/>
+      <c r="H214" s="4"/>
+      <c r="I214" s="3"/>
+      <c r="J214" s="4"/>
+      <c r="K214" s="4"/>
+      <c r="L214" s="4"/>
+      <c r="M214" s="4"/>
+      <c r="N214" s="4"/>
+      <c r="O214" s="4"/>
+      <c r="P214" s="4"/>
+      <c r="Q214" s="4"/>
+      <c r="R214" s="3"/>
+      <c r="S214" s="4"/>
+      <c r="T214" s="4"/>
+    </row>
+    <row r="215" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B215" s="4"/>
+      <c r="C215" s="3"/>
+      <c r="D215" s="4"/>
+      <c r="E215" s="3"/>
+      <c r="F215" s="4"/>
+      <c r="G215" s="3"/>
+      <c r="H215" s="4"/>
+      <c r="I215" s="3"/>
+      <c r="J215" s="4"/>
+      <c r="K215" s="4"/>
+      <c r="L215" s="4"/>
+      <c r="M215" s="4"/>
+      <c r="N215" s="4"/>
+      <c r="O215" s="4"/>
+      <c r="P215" s="4"/>
+      <c r="Q215" s="4"/>
+      <c r="R215" s="3"/>
+      <c r="S215" s="4"/>
+      <c r="T215" s="4"/>
+    </row>
+    <row r="216" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B216" s="4"/>
+      <c r="C216" s="3"/>
+      <c r="D216" s="4"/>
+      <c r="E216" s="3"/>
+      <c r="F216" s="4"/>
+      <c r="G216" s="3"/>
+      <c r="H216" s="4"/>
+      <c r="I216" s="3"/>
+      <c r="J216" s="4"/>
+      <c r="K216" s="4"/>
+      <c r="L216" s="4"/>
+      <c r="M216" s="4"/>
+      <c r="N216" s="4"/>
+      <c r="O216" s="4"/>
+      <c r="P216" s="4"/>
+      <c r="Q216" s="4"/>
+      <c r="R216" s="3"/>
+      <c r="S216" s="4"/>
+      <c r="T216" s="4"/>
+    </row>
+    <row r="217" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B217" s="4"/>
+      <c r="C217" s="3"/>
+      <c r="D217" s="4"/>
+      <c r="E217" s="3"/>
+      <c r="F217" s="4"/>
+      <c r="G217" s="3"/>
+      <c r="H217" s="4"/>
+      <c r="I217" s="3"/>
+      <c r="J217" s="4"/>
+      <c r="K217" s="4"/>
+      <c r="L217" s="4"/>
+      <c r="M217" s="4"/>
+      <c r="N217" s="4"/>
+      <c r="O217" s="4"/>
+      <c r="P217" s="4"/>
+      <c r="Q217" s="4"/>
+      <c r="R217" s="3"/>
+      <c r="S217" s="4"/>
+      <c r="T217" s="4"/>
+    </row>
+    <row r="218" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B218" s="4"/>
+      <c r="C218" s="3"/>
+      <c r="D218" s="4"/>
+      <c r="E218" s="3"/>
+      <c r="F218" s="4"/>
+      <c r="G218" s="3"/>
+      <c r="H218" s="4"/>
+      <c r="I218" s="3"/>
+      <c r="J218" s="4"/>
+      <c r="K218" s="4"/>
+      <c r="L218" s="4"/>
+      <c r="M218" s="4"/>
+      <c r="N218" s="4"/>
+      <c r="O218" s="4"/>
+      <c r="P218" s="4"/>
+      <c r="Q218" s="4"/>
+      <c r="R218" s="3"/>
+      <c r="S218" s="4"/>
+      <c r="T218" s="4"/>
+    </row>
+    <row r="219" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B219" s="4"/>
+      <c r="C219" s="3"/>
+      <c r="D219" s="4"/>
+      <c r="E219" s="3"/>
+      <c r="F219" s="4"/>
+      <c r="G219" s="3"/>
+      <c r="H219" s="4"/>
+      <c r="I219" s="3"/>
+      <c r="J219" s="4"/>
+      <c r="K219" s="4"/>
+      <c r="L219" s="4"/>
+      <c r="M219" s="4"/>
+      <c r="N219" s="4"/>
+      <c r="O219" s="4"/>
+      <c r="P219" s="4"/>
+      <c r="Q219" s="4"/>
+      <c r="R219" s="3"/>
+      <c r="S219" s="4"/>
+      <c r="T219" s="4"/>
+    </row>
+    <row r="220" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B220" s="4"/>
+      <c r="C220" s="3"/>
+      <c r="D220" s="4"/>
+      <c r="E220" s="3"/>
+      <c r="F220" s="4"/>
+      <c r="G220" s="3"/>
+      <c r="H220" s="4"/>
+      <c r="I220" s="3"/>
+      <c r="J220" s="4"/>
+      <c r="K220" s="4"/>
+      <c r="L220" s="4"/>
+      <c r="M220" s="4"/>
+      <c r="N220" s="4"/>
+      <c r="O220" s="4"/>
+      <c r="P220" s="4"/>
+      <c r="Q220" s="4"/>
+      <c r="R220" s="3"/>
+      <c r="S220" s="4"/>
+      <c r="T220" s="4"/>
+    </row>
+    <row r="221" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B221" s="4"/>
+      <c r="C221" s="3"/>
+      <c r="D221" s="4"/>
+      <c r="E221" s="3"/>
+      <c r="F221" s="4"/>
+      <c r="G221" s="3"/>
+      <c r="H221" s="4"/>
+      <c r="I221" s="3"/>
+      <c r="J221" s="4"/>
+      <c r="K221" s="4"/>
+      <c r="L221" s="4"/>
+      <c r="M221" s="4"/>
+      <c r="N221" s="4"/>
+      <c r="O221" s="4"/>
+      <c r="P221" s="4"/>
+      <c r="Q221" s="4"/>
+      <c r="R221" s="3"/>
+      <c r="S221" s="4"/>
+      <c r="T221" s="4"/>
+    </row>
+    <row r="222" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B222" s="4"/>
+      <c r="C222" s="3"/>
+      <c r="D222" s="4"/>
+      <c r="E222" s="3"/>
+      <c r="F222" s="4"/>
+      <c r="G222" s="3"/>
+      <c r="H222" s="4"/>
+      <c r="I222" s="3"/>
+      <c r="J222" s="4"/>
+      <c r="K222" s="4"/>
+      <c r="L222" s="4"/>
+      <c r="M222" s="4"/>
+      <c r="N222" s="4"/>
+      <c r="O222" s="4"/>
+      <c r="P222" s="4"/>
+      <c r="Q222" s="4"/>
+      <c r="R222" s="3"/>
+      <c r="S222" s="4"/>
+      <c r="T222" s="4"/>
+    </row>
+    <row r="223" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B223" s="4"/>
+      <c r="C223" s="3"/>
+      <c r="D223" s="4"/>
+      <c r="E223" s="3"/>
+      <c r="F223" s="4"/>
+      <c r="G223" s="3"/>
+      <c r="H223" s="4"/>
+      <c r="I223" s="3"/>
+      <c r="J223" s="4"/>
+      <c r="K223" s="4"/>
+      <c r="L223" s="4"/>
+      <c r="M223" s="4"/>
+      <c r="N223" s="4"/>
+      <c r="O223" s="4"/>
+      <c r="P223" s="4"/>
+      <c r="Q223" s="4"/>
+      <c r="R223" s="3"/>
+      <c r="S223" s="4"/>
+      <c r="T223" s="4"/>
+    </row>
+    <row r="224" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B224" s="4"/>
+      <c r="C224" s="3"/>
+      <c r="D224" s="4"/>
+      <c r="E224" s="3"/>
+      <c r="F224" s="4"/>
+      <c r="G224" s="3"/>
+      <c r="H224" s="4"/>
+      <c r="I224" s="3"/>
+      <c r="J224" s="4"/>
+      <c r="K224" s="4"/>
+      <c r="L224" s="4"/>
+      <c r="M224" s="4"/>
+      <c r="N224" s="4"/>
+      <c r="O224" s="4"/>
+      <c r="P224" s="4"/>
+      <c r="Q224" s="4"/>
+      <c r="R224" s="3"/>
+      <c r="S224" s="4"/>
+      <c r="T224" s="4"/>
+    </row>
+    <row r="225" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B225" s="4"/>
+      <c r="C225" s="3"/>
+      <c r="D225" s="4"/>
+      <c r="E225" s="3"/>
+      <c r="F225" s="4"/>
+      <c r="G225" s="3"/>
+      <c r="H225" s="4"/>
+      <c r="I225" s="3"/>
+      <c r="J225" s="4"/>
+      <c r="K225" s="4"/>
+      <c r="L225" s="4"/>
+      <c r="M225" s="4"/>
+      <c r="N225" s="4"/>
+      <c r="O225" s="4"/>
+      <c r="P225" s="4"/>
+      <c r="Q225" s="4"/>
+      <c r="R225" s="3"/>
+      <c r="S225" s="4"/>
+      <c r="T225" s="4"/>
+    </row>
+    <row r="226" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B226" s="4"/>
+      <c r="C226" s="3"/>
+      <c r="D226" s="4"/>
+      <c r="E226" s="3"/>
+      <c r="F226" s="4"/>
+      <c r="G226" s="3"/>
+      <c r="H226" s="4"/>
+      <c r="I226" s="3"/>
+      <c r="J226" s="4"/>
+      <c r="K226" s="4"/>
+      <c r="L226" s="4"/>
+      <c r="M226" s="4"/>
+      <c r="N226" s="4"/>
+      <c r="O226" s="4"/>
+      <c r="P226" s="4"/>
+      <c r="Q226" s="4"/>
+      <c r="R226" s="3"/>
+      <c r="S226" s="4"/>
+      <c r="T226" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
closes #10 popup modal (#11)
* Docs: #10 Add FlowChart for Popup Modal

* Docs: #10 Add FlowChart for Popup Modal Module

* Docs: #10 Update FloawChart for Popup Modal Module

* Docs: #10 Update RS for Modal Module

* Docs: #10 Update + Rearrange Class Diagram
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE8671E-293D-4D7C-AF0A-7B02D8814E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E77F48-49CD-4B50-A588-9B26865DB0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16320" yWindow="0" windowWidth="12585" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="92">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,10 +107,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공지 메시지 = 시스템 메시지 출력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -171,14 +167,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FR-C-T-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FR-C-T-02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FR-C-01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -242,13 +230,6 @@
     <t>FR-C-E-01.04</t>
   </si>
   <si>
-    <t>FR-C-E-01.06</t>
-  </si>
-  <si>
-    <t>추상 함수 실행</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FR-C-E-01.04.01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -293,22 +274,112 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FR-C-E-01.04.07</t>
-  </si>
-  <si>
-    <t>다른 이름으로 저장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FR-C-E-01.05</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>마우스 이벤트 초기화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인 메뉴로 돌아가기</t>
+    <t>에디터용 인터페이스: 맵 에디터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 메뉴 UI 토글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-N-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-N-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-01.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 컨텐츠 프리펩 광역 컨포넌트에 전달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-01.02</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.03</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.04</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.05</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.06</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.07</t>
+  </si>
+  <si>
+    <t>모달 초기화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 초기값 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 타입 관련 컴포넌트 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 컨텐츠 적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 취소 / 확인 버튼 이벤트 적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 텍스트 모달 인터페이스 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-03</t>
+  </si>
+  <si>
+    <t>일반 텍스트 인풋 모달 인터페이스 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -403,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -411,8 +482,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -693,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:T65"/>
+  <dimension ref="B2:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="U72" sqref="U72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -731,19 +800,19 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
       </c>
       <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
         <v>26</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>27</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" t="s">
@@ -758,33 +827,53 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>32</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
       </c>
       <c r="H6" t="s">
         <v>16</v>
       </c>
       <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
         <v>29</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>73</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
@@ -1023,41 +1112,41 @@
       <c r="T21" s="4"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="7"/>
+      <c r="D22" s="4"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="7"/>
+      <c r="H22" s="4"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
       <c r="R22" s="3"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -1078,11 +1167,11 @@
       <c r="F24" s="4"/>
       <c r="G24" s="3"/>
       <c r="H24" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -1143,15 +1232,15 @@
       <c r="D27" s="4"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -1172,11 +1261,11 @@
       <c r="F28" s="4"/>
       <c r="G28" s="3"/>
       <c r="H28" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -1197,11 +1286,11 @@
       <c r="F29" s="4"/>
       <c r="G29" s="3"/>
       <c r="H29" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -1222,11 +1311,11 @@
       <c r="F30" s="4"/>
       <c r="G30" s="3"/>
       <c r="H30" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -1247,11 +1336,11 @@
       <c r="F31" s="4"/>
       <c r="G31" s="3"/>
       <c r="H31" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
@@ -1272,11 +1361,11 @@
       <c r="F32" s="4"/>
       <c r="G32" s="3"/>
       <c r="H32" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -1297,11 +1386,11 @@
       <c r="F33" s="4"/>
       <c r="G33" s="3"/>
       <c r="H33" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -1322,11 +1411,11 @@
       <c r="F34" s="4"/>
       <c r="G34" s="3"/>
       <c r="H34" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -1347,11 +1436,11 @@
       <c r="F35" s="4"/>
       <c r="G35" s="3"/>
       <c r="H35" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -1365,29 +1454,29 @@
       <c r="T35" s="4"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B36" s="7"/>
+      <c r="B36" s="4"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="7"/>
+      <c r="D36" s="4"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="7"/>
+      <c r="F36" s="4"/>
       <c r="G36" s="3"/>
       <c r="H36" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I36" s="3"/>
-      <c r="J36" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
+      <c r="J36" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
       <c r="R36" s="3"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="7"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="4"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
@@ -1397,11 +1486,11 @@
       <c r="F37" s="4"/>
       <c r="G37" s="3"/>
       <c r="H37" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -1422,11 +1511,11 @@
       <c r="F38" s="4"/>
       <c r="G38" s="3"/>
       <c r="H38" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
@@ -1446,13 +1535,9 @@
       <c r="E39" s="3"/>
       <c r="F39" s="4"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="H39" s="4"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -1461,7 +1546,7 @@
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
       <c r="R39" s="3"/>
-      <c r="S39" s="2"/>
+      <c r="S39" s="4"/>
       <c r="T39" s="4"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.3">
@@ -1471,13 +1556,9 @@
       <c r="E40" s="3"/>
       <c r="F40" s="4"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="H40" s="4"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -1486,7 +1567,7 @@
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
       <c r="R40" s="3"/>
-      <c r="S40" s="2"/>
+      <c r="S40" s="4"/>
       <c r="T40" s="4"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.3">
@@ -1709,11 +1790,11 @@
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
@@ -1734,11 +1815,11 @@
       <c r="F52" s="4"/>
       <c r="G52" s="3"/>
       <c r="H52" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I52" s="3"/>
       <c r="J52" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -1841,15 +1922,15 @@
       <c r="D57" s="4"/>
       <c r="E57" s="3"/>
       <c r="F57" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="4" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
@@ -1870,11 +1951,11 @@
       <c r="F58" s="4"/>
       <c r="G58" s="3"/>
       <c r="H58" s="4" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
@@ -2034,6 +2115,3431 @@
       <c r="S65" s="4"/>
       <c r="T65" s="4"/>
     </row>
+    <row r="66" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B66" s="4"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="4"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="4"/>
+      <c r="Q66" s="4"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="4"/>
+      <c r="T66" s="4"/>
+    </row>
+    <row r="67" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B67" s="4"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
+      <c r="P67" s="4"/>
+      <c r="Q67" s="4"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="4"/>
+    </row>
+    <row r="68" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B68" s="4"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="4"/>
+      <c r="Q68" s="4"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="4"/>
+      <c r="T68" s="4"/>
+    </row>
+    <row r="69" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B69" s="4"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
+      <c r="P69" s="4"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="4"/>
+      <c r="T69" s="4"/>
+    </row>
+    <row r="70" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B70" s="4"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="4"/>
+      <c r="Q70" s="4"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="4"/>
+      <c r="T70" s="4"/>
+    </row>
+    <row r="71" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B71" s="4"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
+      <c r="P71" s="4"/>
+      <c r="Q71" s="4"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="4"/>
+      <c r="T71" s="4"/>
+    </row>
+    <row r="72" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B72" s="4"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
+      <c r="P72" s="4"/>
+      <c r="Q72" s="4"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="4"/>
+      <c r="T72" s="4"/>
+    </row>
+    <row r="73" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B73" s="4"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4"/>
+      <c r="P73" s="4"/>
+      <c r="Q73" s="4"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="4"/>
+      <c r="T73" s="4"/>
+    </row>
+    <row r="74" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B74" s="4"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E74" s="3"/>
+      <c r="F74" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G74" s="3"/>
+      <c r="H74" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I74" s="3"/>
+      <c r="J74" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
+      <c r="P74" s="4"/>
+      <c r="Q74" s="4"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="4"/>
+    </row>
+    <row r="75" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B75" s="4"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I75" s="3"/>
+      <c r="J75" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
+      <c r="P75" s="4"/>
+      <c r="Q75" s="4"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="4"/>
+    </row>
+    <row r="76" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B76" s="4"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I76" s="3"/>
+      <c r="J76" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K76" s="4"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="4"/>
+      <c r="O76" s="4"/>
+      <c r="P76" s="4"/>
+      <c r="Q76" s="4"/>
+      <c r="R76" s="3"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="4"/>
+    </row>
+    <row r="77" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B77" s="4"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I77" s="3"/>
+      <c r="J77" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="3"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="4"/>
+    </row>
+    <row r="78" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B78" s="4"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="J78" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K78" s="4"/>
+      <c r="L78" s="4"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="4"/>
+      <c r="Q78" s="4"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="4"/>
+    </row>
+    <row r="79" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B79" s="4"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I79" s="3"/>
+      <c r="J79" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="4"/>
+      <c r="N79" s="4"/>
+      <c r="O79" s="4"/>
+      <c r="P79" s="4"/>
+      <c r="Q79" s="4"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="4"/>
+    </row>
+    <row r="80" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B80" s="4"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I80" s="3"/>
+      <c r="J80" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="3"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="4"/>
+    </row>
+    <row r="81" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B81" s="4"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I81" s="3"/>
+      <c r="J81" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="4"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="4"/>
+    </row>
+    <row r="82" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B82" s="4"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I82" s="3"/>
+      <c r="J82" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K82" s="4"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="4"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="4"/>
+      <c r="Q82" s="4"/>
+      <c r="R82" s="3"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="4"/>
+    </row>
+    <row r="83" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B83" s="4"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I83" s="3"/>
+      <c r="J83" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K83" s="4"/>
+      <c r="L83" s="4"/>
+      <c r="M83" s="4"/>
+      <c r="N83" s="4"/>
+      <c r="O83" s="4"/>
+      <c r="P83" s="4"/>
+      <c r="Q83" s="4"/>
+      <c r="R83" s="3"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="4"/>
+    </row>
+    <row r="84" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B84" s="4"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="3"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="4"/>
+      <c r="Q84" s="4"/>
+      <c r="R84" s="3"/>
+      <c r="S84" s="4"/>
+      <c r="T84" s="4"/>
+    </row>
+    <row r="85" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B85" s="4"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="4"/>
+      <c r="L85" s="4"/>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="4"/>
+      <c r="P85" s="4"/>
+      <c r="Q85" s="4"/>
+      <c r="R85" s="3"/>
+      <c r="S85" s="4"/>
+      <c r="T85" s="4"/>
+    </row>
+    <row r="86" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B86" s="4"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="4"/>
+      <c r="Q86" s="4"/>
+      <c r="R86" s="3"/>
+      <c r="S86" s="4"/>
+      <c r="T86" s="4"/>
+    </row>
+    <row r="87" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B87" s="4"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="3"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
+      <c r="L87" s="4"/>
+      <c r="M87" s="4"/>
+      <c r="N87" s="4"/>
+      <c r="O87" s="4"/>
+      <c r="P87" s="4"/>
+      <c r="Q87" s="4"/>
+      <c r="R87" s="3"/>
+      <c r="S87" s="4"/>
+      <c r="T87" s="4"/>
+    </row>
+    <row r="88" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B88" s="4"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="4"/>
+      <c r="Q88" s="4"/>
+      <c r="R88" s="3"/>
+      <c r="S88" s="4"/>
+      <c r="T88" s="4"/>
+    </row>
+    <row r="89" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B89" s="4"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="4"/>
+      <c r="O89" s="4"/>
+      <c r="P89" s="4"/>
+      <c r="Q89" s="4"/>
+      <c r="R89" s="3"/>
+      <c r="S89" s="4"/>
+      <c r="T89" s="4"/>
+    </row>
+    <row r="90" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B90" s="4"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+      <c r="M90" s="4"/>
+      <c r="N90" s="4"/>
+      <c r="O90" s="4"/>
+      <c r="P90" s="4"/>
+      <c r="Q90" s="4"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="4"/>
+      <c r="T90" s="4"/>
+    </row>
+    <row r="91" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B91" s="4"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
+      <c r="L91" s="4"/>
+      <c r="M91" s="4"/>
+      <c r="N91" s="4"/>
+      <c r="O91" s="4"/>
+      <c r="P91" s="4"/>
+      <c r="Q91" s="4"/>
+      <c r="R91" s="3"/>
+      <c r="S91" s="4"/>
+      <c r="T91" s="4"/>
+    </row>
+    <row r="92" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B92" s="4"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="4"/>
+      <c r="O92" s="4"/>
+      <c r="P92" s="4"/>
+      <c r="Q92" s="4"/>
+      <c r="R92" s="3"/>
+      <c r="S92" s="4"/>
+      <c r="T92" s="4"/>
+    </row>
+    <row r="93" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B93" s="4"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
+      <c r="L93" s="4"/>
+      <c r="M93" s="4"/>
+      <c r="N93" s="4"/>
+      <c r="O93" s="4"/>
+      <c r="P93" s="4"/>
+      <c r="Q93" s="4"/>
+      <c r="R93" s="3"/>
+      <c r="S93" s="4"/>
+      <c r="T93" s="4"/>
+    </row>
+    <row r="94" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B94" s="4"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="3"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
+      <c r="L94" s="4"/>
+      <c r="M94" s="4"/>
+      <c r="N94" s="4"/>
+      <c r="O94" s="4"/>
+      <c r="P94" s="4"/>
+      <c r="Q94" s="4"/>
+      <c r="R94" s="3"/>
+      <c r="S94" s="4"/>
+      <c r="T94" s="4"/>
+    </row>
+    <row r="95" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B95" s="4"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="4"/>
+      <c r="M95" s="4"/>
+      <c r="N95" s="4"/>
+      <c r="O95" s="4"/>
+      <c r="P95" s="4"/>
+      <c r="Q95" s="4"/>
+      <c r="R95" s="3"/>
+      <c r="S95" s="4"/>
+      <c r="T95" s="4"/>
+    </row>
+    <row r="96" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B96" s="4"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="3"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="4"/>
+      <c r="L96" s="4"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="4"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="4"/>
+      <c r="Q96" s="4"/>
+      <c r="R96" s="3"/>
+      <c r="S96" s="4"/>
+      <c r="T96" s="4"/>
+    </row>
+    <row r="97" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B97" s="4"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="3"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="4"/>
+      <c r="L97" s="4"/>
+      <c r="M97" s="4"/>
+      <c r="N97" s="4"/>
+      <c r="O97" s="4"/>
+      <c r="P97" s="4"/>
+      <c r="Q97" s="4"/>
+      <c r="R97" s="3"/>
+      <c r="S97" s="4"/>
+      <c r="T97" s="4"/>
+    </row>
+    <row r="98" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B98" s="4"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="3"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
+      <c r="L98" s="4"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="4"/>
+      <c r="O98" s="4"/>
+      <c r="P98" s="4"/>
+      <c r="Q98" s="4"/>
+      <c r="R98" s="3"/>
+      <c r="S98" s="4"/>
+      <c r="T98" s="4"/>
+    </row>
+    <row r="99" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B99" s="4"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="3"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="4"/>
+      <c r="L99" s="4"/>
+      <c r="M99" s="4"/>
+      <c r="N99" s="4"/>
+      <c r="O99" s="4"/>
+      <c r="P99" s="4"/>
+      <c r="Q99" s="4"/>
+      <c r="R99" s="3"/>
+      <c r="S99" s="4"/>
+      <c r="T99" s="4"/>
+    </row>
+    <row r="100" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B100" s="4"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="3"/>
+      <c r="J100" s="4"/>
+      <c r="K100" s="4"/>
+      <c r="L100" s="4"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="4"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="4"/>
+      <c r="Q100" s="4"/>
+      <c r="R100" s="3"/>
+      <c r="S100" s="4"/>
+      <c r="T100" s="4"/>
+    </row>
+    <row r="101" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B101" s="4"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="4"/>
+      <c r="K101" s="4"/>
+      <c r="L101" s="4"/>
+      <c r="M101" s="4"/>
+      <c r="N101" s="4"/>
+      <c r="O101" s="4"/>
+      <c r="P101" s="4"/>
+      <c r="Q101" s="4"/>
+      <c r="R101" s="3"/>
+      <c r="S101" s="4"/>
+      <c r="T101" s="4"/>
+    </row>
+    <row r="102" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B102" s="4"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="3"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="4"/>
+      <c r="L102" s="4"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="4"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="4"/>
+      <c r="Q102" s="4"/>
+      <c r="R102" s="3"/>
+      <c r="S102" s="4"/>
+      <c r="T102" s="4"/>
+    </row>
+    <row r="103" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B103" s="4"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="3"/>
+      <c r="J103" s="4"/>
+      <c r="K103" s="4"/>
+      <c r="L103" s="4"/>
+      <c r="M103" s="4"/>
+      <c r="N103" s="4"/>
+      <c r="O103" s="4"/>
+      <c r="P103" s="4"/>
+      <c r="Q103" s="4"/>
+      <c r="R103" s="3"/>
+      <c r="S103" s="4"/>
+      <c r="T103" s="4"/>
+    </row>
+    <row r="104" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B104" s="4"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="3"/>
+      <c r="J104" s="4"/>
+      <c r="K104" s="4"/>
+      <c r="L104" s="4"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="4"/>
+      <c r="O104" s="4"/>
+      <c r="P104" s="4"/>
+      <c r="Q104" s="4"/>
+      <c r="R104" s="3"/>
+      <c r="S104" s="4"/>
+      <c r="T104" s="4"/>
+    </row>
+    <row r="105" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B105" s="4"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="3"/>
+      <c r="J105" s="4"/>
+      <c r="K105" s="4"/>
+      <c r="L105" s="4"/>
+      <c r="M105" s="4"/>
+      <c r="N105" s="4"/>
+      <c r="O105" s="4"/>
+      <c r="P105" s="4"/>
+      <c r="Q105" s="4"/>
+      <c r="R105" s="3"/>
+      <c r="S105" s="4"/>
+      <c r="T105" s="4"/>
+    </row>
+    <row r="106" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B106" s="4"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="3"/>
+      <c r="J106" s="4"/>
+      <c r="K106" s="4"/>
+      <c r="L106" s="4"/>
+      <c r="M106" s="4"/>
+      <c r="N106" s="4"/>
+      <c r="O106" s="4"/>
+      <c r="P106" s="4"/>
+      <c r="Q106" s="4"/>
+      <c r="R106" s="3"/>
+      <c r="S106" s="4"/>
+      <c r="T106" s="4"/>
+    </row>
+    <row r="107" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B107" s="4"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="3"/>
+      <c r="J107" s="4"/>
+      <c r="K107" s="4"/>
+      <c r="L107" s="4"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="O107" s="4"/>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="4"/>
+      <c r="R107" s="3"/>
+      <c r="S107" s="4"/>
+      <c r="T107" s="4"/>
+    </row>
+    <row r="108" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B108" s="4"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="4"/>
+      <c r="K108" s="4"/>
+      <c r="L108" s="4"/>
+      <c r="M108" s="4"/>
+      <c r="N108" s="4"/>
+      <c r="O108" s="4"/>
+      <c r="P108" s="4"/>
+      <c r="Q108" s="4"/>
+      <c r="R108" s="3"/>
+      <c r="S108" s="4"/>
+      <c r="T108" s="4"/>
+    </row>
+    <row r="109" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B109" s="4"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="3"/>
+      <c r="J109" s="4"/>
+      <c r="K109" s="4"/>
+      <c r="L109" s="4"/>
+      <c r="M109" s="4"/>
+      <c r="N109" s="4"/>
+      <c r="O109" s="4"/>
+      <c r="P109" s="4"/>
+      <c r="Q109" s="4"/>
+      <c r="R109" s="3"/>
+      <c r="S109" s="4"/>
+      <c r="T109" s="4"/>
+    </row>
+    <row r="110" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B110" s="4"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="3"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="3"/>
+      <c r="J110" s="4"/>
+      <c r="K110" s="4"/>
+      <c r="L110" s="4"/>
+      <c r="M110" s="4"/>
+      <c r="N110" s="4"/>
+      <c r="O110" s="4"/>
+      <c r="P110" s="4"/>
+      <c r="Q110" s="4"/>
+      <c r="R110" s="3"/>
+      <c r="S110" s="4"/>
+      <c r="T110" s="4"/>
+    </row>
+    <row r="111" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B111" s="4"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="3"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="3"/>
+      <c r="J111" s="4"/>
+      <c r="K111" s="4"/>
+      <c r="L111" s="4"/>
+      <c r="M111" s="4"/>
+      <c r="N111" s="4"/>
+      <c r="O111" s="4"/>
+      <c r="P111" s="4"/>
+      <c r="Q111" s="4"/>
+      <c r="R111" s="3"/>
+      <c r="S111" s="4"/>
+      <c r="T111" s="4"/>
+    </row>
+    <row r="112" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B112" s="4"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="3"/>
+      <c r="J112" s="4"/>
+      <c r="K112" s="4"/>
+      <c r="L112" s="4"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="4"/>
+      <c r="O112" s="4"/>
+      <c r="P112" s="4"/>
+      <c r="Q112" s="4"/>
+      <c r="R112" s="3"/>
+      <c r="S112" s="4"/>
+      <c r="T112" s="4"/>
+    </row>
+    <row r="113" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B113" s="4"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="4"/>
+      <c r="I113" s="3"/>
+      <c r="J113" s="4"/>
+      <c r="K113" s="4"/>
+      <c r="L113" s="4"/>
+      <c r="M113" s="4"/>
+      <c r="N113" s="4"/>
+      <c r="O113" s="4"/>
+      <c r="P113" s="4"/>
+      <c r="Q113" s="4"/>
+      <c r="R113" s="3"/>
+      <c r="S113" s="4"/>
+      <c r="T113" s="4"/>
+    </row>
+    <row r="114" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B114" s="4"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="3"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="3"/>
+      <c r="J114" s="4"/>
+      <c r="K114" s="4"/>
+      <c r="L114" s="4"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="4"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="4"/>
+      <c r="Q114" s="4"/>
+      <c r="R114" s="3"/>
+      <c r="S114" s="4"/>
+      <c r="T114" s="4"/>
+    </row>
+    <row r="115" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B115" s="4"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="3"/>
+      <c r="H115" s="4"/>
+      <c r="I115" s="3"/>
+      <c r="J115" s="4"/>
+      <c r="K115" s="4"/>
+      <c r="L115" s="4"/>
+      <c r="M115" s="4"/>
+      <c r="N115" s="4"/>
+      <c r="O115" s="4"/>
+      <c r="P115" s="4"/>
+      <c r="Q115" s="4"/>
+      <c r="R115" s="3"/>
+      <c r="S115" s="4"/>
+      <c r="T115" s="4"/>
+    </row>
+    <row r="116" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B116" s="4"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="3"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="3"/>
+      <c r="J116" s="4"/>
+      <c r="K116" s="4"/>
+      <c r="L116" s="4"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="4"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="4"/>
+      <c r="Q116" s="4"/>
+      <c r="R116" s="3"/>
+      <c r="S116" s="4"/>
+      <c r="T116" s="4"/>
+    </row>
+    <row r="117" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B117" s="4"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="3"/>
+      <c r="H117" s="4"/>
+      <c r="I117" s="3"/>
+      <c r="J117" s="4"/>
+      <c r="K117" s="4"/>
+      <c r="L117" s="4"/>
+      <c r="M117" s="4"/>
+      <c r="N117" s="4"/>
+      <c r="O117" s="4"/>
+      <c r="P117" s="4"/>
+      <c r="Q117" s="4"/>
+      <c r="R117" s="3"/>
+      <c r="S117" s="4"/>
+      <c r="T117" s="4"/>
+    </row>
+    <row r="118" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B118" s="4"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="3"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="3"/>
+      <c r="J118" s="4"/>
+      <c r="K118" s="4"/>
+      <c r="L118" s="4"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="4"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="4"/>
+      <c r="Q118" s="4"/>
+      <c r="R118" s="3"/>
+      <c r="S118" s="4"/>
+      <c r="T118" s="4"/>
+    </row>
+    <row r="119" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B119" s="4"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="3"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="3"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="3"/>
+      <c r="J119" s="4"/>
+      <c r="K119" s="4"/>
+      <c r="L119" s="4"/>
+      <c r="M119" s="4"/>
+      <c r="N119" s="4"/>
+      <c r="O119" s="4"/>
+      <c r="P119" s="4"/>
+      <c r="Q119" s="4"/>
+      <c r="R119" s="3"/>
+      <c r="S119" s="4"/>
+      <c r="T119" s="4"/>
+    </row>
+    <row r="120" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B120" s="4"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="3"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="3"/>
+      <c r="J120" s="4"/>
+      <c r="K120" s="4"/>
+      <c r="L120" s="4"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="4"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="4"/>
+      <c r="Q120" s="4"/>
+      <c r="R120" s="3"/>
+      <c r="S120" s="4"/>
+      <c r="T120" s="4"/>
+    </row>
+    <row r="121" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B121" s="4"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="3"/>
+      <c r="H121" s="4"/>
+      <c r="I121" s="3"/>
+      <c r="J121" s="4"/>
+      <c r="K121" s="4"/>
+      <c r="L121" s="4"/>
+      <c r="M121" s="4"/>
+      <c r="N121" s="4"/>
+      <c r="O121" s="4"/>
+      <c r="P121" s="4"/>
+      <c r="Q121" s="4"/>
+      <c r="R121" s="3"/>
+      <c r="S121" s="4"/>
+      <c r="T121" s="4"/>
+    </row>
+    <row r="122" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B122" s="4"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="3"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="3"/>
+      <c r="J122" s="4"/>
+      <c r="K122" s="4"/>
+      <c r="L122" s="4"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="4"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="4"/>
+      <c r="Q122" s="4"/>
+      <c r="R122" s="3"/>
+      <c r="S122" s="4"/>
+      <c r="T122" s="4"/>
+    </row>
+    <row r="123" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B123" s="4"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="3"/>
+      <c r="H123" s="4"/>
+      <c r="I123" s="3"/>
+      <c r="J123" s="4"/>
+      <c r="K123" s="4"/>
+      <c r="L123" s="4"/>
+      <c r="M123" s="4"/>
+      <c r="N123" s="4"/>
+      <c r="O123" s="4"/>
+      <c r="P123" s="4"/>
+      <c r="Q123" s="4"/>
+      <c r="R123" s="3"/>
+      <c r="S123" s="4"/>
+      <c r="T123" s="4"/>
+    </row>
+    <row r="124" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B124" s="4"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="3"/>
+      <c r="H124" s="4"/>
+      <c r="I124" s="3"/>
+      <c r="J124" s="4"/>
+      <c r="K124" s="4"/>
+      <c r="L124" s="4"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="4"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="4"/>
+      <c r="Q124" s="4"/>
+      <c r="R124" s="3"/>
+      <c r="S124" s="4"/>
+      <c r="T124" s="4"/>
+    </row>
+    <row r="125" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B125" s="4"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="3"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="3"/>
+      <c r="H125" s="4"/>
+      <c r="I125" s="3"/>
+      <c r="J125" s="4"/>
+      <c r="K125" s="4"/>
+      <c r="L125" s="4"/>
+      <c r="M125" s="4"/>
+      <c r="N125" s="4"/>
+      <c r="O125" s="4"/>
+      <c r="P125" s="4"/>
+      <c r="Q125" s="4"/>
+      <c r="R125" s="3"/>
+      <c r="S125" s="4"/>
+      <c r="T125" s="4"/>
+    </row>
+    <row r="126" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B126" s="4"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="3"/>
+      <c r="H126" s="4"/>
+      <c r="I126" s="3"/>
+      <c r="J126" s="4"/>
+      <c r="K126" s="4"/>
+      <c r="L126" s="4"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="4"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="4"/>
+      <c r="Q126" s="4"/>
+      <c r="R126" s="3"/>
+      <c r="S126" s="4"/>
+      <c r="T126" s="4"/>
+    </row>
+    <row r="127" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B127" s="4"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="3"/>
+      <c r="F127" s="4"/>
+      <c r="G127" s="3"/>
+      <c r="H127" s="4"/>
+      <c r="I127" s="3"/>
+      <c r="J127" s="4"/>
+      <c r="K127" s="4"/>
+      <c r="L127" s="4"/>
+      <c r="M127" s="4"/>
+      <c r="N127" s="4"/>
+      <c r="O127" s="4"/>
+      <c r="P127" s="4"/>
+      <c r="Q127" s="4"/>
+      <c r="R127" s="3"/>
+      <c r="S127" s="4"/>
+      <c r="T127" s="4"/>
+    </row>
+    <row r="128" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B128" s="4"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="3"/>
+      <c r="H128" s="4"/>
+      <c r="I128" s="3"/>
+      <c r="J128" s="4"/>
+      <c r="K128" s="4"/>
+      <c r="L128" s="4"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="4"/>
+      <c r="O128" s="4"/>
+      <c r="P128" s="4"/>
+      <c r="Q128" s="4"/>
+      <c r="R128" s="3"/>
+      <c r="S128" s="4"/>
+      <c r="T128" s="4"/>
+    </row>
+    <row r="129" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B129" s="4"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="4"/>
+      <c r="G129" s="3"/>
+      <c r="H129" s="4"/>
+      <c r="I129" s="3"/>
+      <c r="J129" s="4"/>
+      <c r="K129" s="4"/>
+      <c r="L129" s="4"/>
+      <c r="M129" s="4"/>
+      <c r="N129" s="4"/>
+      <c r="O129" s="4"/>
+      <c r="P129" s="4"/>
+      <c r="Q129" s="4"/>
+      <c r="R129" s="3"/>
+      <c r="S129" s="4"/>
+      <c r="T129" s="4"/>
+    </row>
+    <row r="130" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B130" s="4"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="4"/>
+      <c r="G130" s="3"/>
+      <c r="H130" s="4"/>
+      <c r="I130" s="3"/>
+      <c r="J130" s="4"/>
+      <c r="K130" s="4"/>
+      <c r="L130" s="4"/>
+      <c r="M130" s="4"/>
+      <c r="N130" s="4"/>
+      <c r="O130" s="4"/>
+      <c r="P130" s="4"/>
+      <c r="Q130" s="4"/>
+      <c r="R130" s="3"/>
+      <c r="S130" s="4"/>
+      <c r="T130" s="4"/>
+    </row>
+    <row r="131" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B131" s="4"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="4"/>
+      <c r="G131" s="3"/>
+      <c r="H131" s="4"/>
+      <c r="I131" s="3"/>
+      <c r="J131" s="4"/>
+      <c r="K131" s="4"/>
+      <c r="L131" s="4"/>
+      <c r="M131" s="4"/>
+      <c r="N131" s="4"/>
+      <c r="O131" s="4"/>
+      <c r="P131" s="4"/>
+      <c r="Q131" s="4"/>
+      <c r="R131" s="3"/>
+      <c r="S131" s="4"/>
+      <c r="T131" s="4"/>
+    </row>
+    <row r="132" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B132" s="4"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="3"/>
+      <c r="H132" s="4"/>
+      <c r="I132" s="3"/>
+      <c r="J132" s="4"/>
+      <c r="K132" s="4"/>
+      <c r="L132" s="4"/>
+      <c r="M132" s="4"/>
+      <c r="N132" s="4"/>
+      <c r="O132" s="4"/>
+      <c r="P132" s="4"/>
+      <c r="Q132" s="4"/>
+      <c r="R132" s="3"/>
+      <c r="S132" s="4"/>
+      <c r="T132" s="4"/>
+    </row>
+    <row r="133" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B133" s="4"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="4"/>
+      <c r="E133" s="3"/>
+      <c r="F133" s="4"/>
+      <c r="G133" s="3"/>
+      <c r="H133" s="4"/>
+      <c r="I133" s="3"/>
+      <c r="J133" s="4"/>
+      <c r="K133" s="4"/>
+      <c r="L133" s="4"/>
+      <c r="M133" s="4"/>
+      <c r="N133" s="4"/>
+      <c r="O133" s="4"/>
+      <c r="P133" s="4"/>
+      <c r="Q133" s="4"/>
+      <c r="R133" s="3"/>
+      <c r="S133" s="4"/>
+      <c r="T133" s="4"/>
+    </row>
+    <row r="134" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B134" s="4"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="4"/>
+      <c r="G134" s="3"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="3"/>
+      <c r="J134" s="4"/>
+      <c r="K134" s="4"/>
+      <c r="L134" s="4"/>
+      <c r="M134" s="4"/>
+      <c r="N134" s="4"/>
+      <c r="O134" s="4"/>
+      <c r="P134" s="4"/>
+      <c r="Q134" s="4"/>
+      <c r="R134" s="3"/>
+      <c r="S134" s="4"/>
+      <c r="T134" s="4"/>
+    </row>
+    <row r="135" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B135" s="4"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="3"/>
+      <c r="H135" s="4"/>
+      <c r="I135" s="3"/>
+      <c r="J135" s="4"/>
+      <c r="K135" s="4"/>
+      <c r="L135" s="4"/>
+      <c r="M135" s="4"/>
+      <c r="N135" s="4"/>
+      <c r="O135" s="4"/>
+      <c r="P135" s="4"/>
+      <c r="Q135" s="4"/>
+      <c r="R135" s="3"/>
+      <c r="S135" s="4"/>
+      <c r="T135" s="4"/>
+    </row>
+    <row r="136" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B136" s="4"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="3"/>
+      <c r="H136" s="4"/>
+      <c r="I136" s="3"/>
+      <c r="J136" s="4"/>
+      <c r="K136" s="4"/>
+      <c r="L136" s="4"/>
+      <c r="M136" s="4"/>
+      <c r="N136" s="4"/>
+      <c r="O136" s="4"/>
+      <c r="P136" s="4"/>
+      <c r="Q136" s="4"/>
+      <c r="R136" s="3"/>
+      <c r="S136" s="4"/>
+      <c r="T136" s="4"/>
+    </row>
+    <row r="137" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B137" s="4"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="3"/>
+      <c r="H137" s="4"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="4"/>
+      <c r="K137" s="4"/>
+      <c r="L137" s="4"/>
+      <c r="M137" s="4"/>
+      <c r="N137" s="4"/>
+      <c r="O137" s="4"/>
+      <c r="P137" s="4"/>
+      <c r="Q137" s="4"/>
+      <c r="R137" s="3"/>
+      <c r="S137" s="4"/>
+      <c r="T137" s="4"/>
+    </row>
+    <row r="138" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B138" s="4"/>
+      <c r="C138" s="3"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="4"/>
+      <c r="G138" s="3"/>
+      <c r="H138" s="4"/>
+      <c r="I138" s="3"/>
+      <c r="J138" s="4"/>
+      <c r="K138" s="4"/>
+      <c r="L138" s="4"/>
+      <c r="M138" s="4"/>
+      <c r="N138" s="4"/>
+      <c r="O138" s="4"/>
+      <c r="P138" s="4"/>
+      <c r="Q138" s="4"/>
+      <c r="R138" s="3"/>
+      <c r="S138" s="4"/>
+      <c r="T138" s="4"/>
+    </row>
+    <row r="139" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B139" s="4"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="4"/>
+      <c r="E139" s="3"/>
+      <c r="F139" s="4"/>
+      <c r="G139" s="3"/>
+      <c r="H139" s="4"/>
+      <c r="I139" s="3"/>
+      <c r="J139" s="4"/>
+      <c r="K139" s="4"/>
+      <c r="L139" s="4"/>
+      <c r="M139" s="4"/>
+      <c r="N139" s="4"/>
+      <c r="O139" s="4"/>
+      <c r="P139" s="4"/>
+      <c r="Q139" s="4"/>
+      <c r="R139" s="3"/>
+      <c r="S139" s="4"/>
+      <c r="T139" s="4"/>
+    </row>
+    <row r="140" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B140" s="4"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="4"/>
+      <c r="G140" s="3"/>
+      <c r="H140" s="4"/>
+      <c r="I140" s="3"/>
+      <c r="J140" s="4"/>
+      <c r="K140" s="4"/>
+      <c r="L140" s="4"/>
+      <c r="M140" s="4"/>
+      <c r="N140" s="4"/>
+      <c r="O140" s="4"/>
+      <c r="P140" s="4"/>
+      <c r="Q140" s="4"/>
+      <c r="R140" s="3"/>
+      <c r="S140" s="4"/>
+      <c r="T140" s="4"/>
+    </row>
+    <row r="141" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B141" s="4"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="4"/>
+      <c r="E141" s="3"/>
+      <c r="F141" s="4"/>
+      <c r="G141" s="3"/>
+      <c r="H141" s="4"/>
+      <c r="I141" s="3"/>
+      <c r="J141" s="4"/>
+      <c r="K141" s="4"/>
+      <c r="L141" s="4"/>
+      <c r="M141" s="4"/>
+      <c r="N141" s="4"/>
+      <c r="O141" s="4"/>
+      <c r="P141" s="4"/>
+      <c r="Q141" s="4"/>
+      <c r="R141" s="3"/>
+      <c r="S141" s="4"/>
+      <c r="T141" s="4"/>
+    </row>
+    <row r="142" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B142" s="4"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="4"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="3"/>
+      <c r="H142" s="4"/>
+      <c r="I142" s="3"/>
+      <c r="J142" s="4"/>
+      <c r="K142" s="4"/>
+      <c r="L142" s="4"/>
+      <c r="M142" s="4"/>
+      <c r="N142" s="4"/>
+      <c r="O142" s="4"/>
+      <c r="P142" s="4"/>
+      <c r="Q142" s="4"/>
+      <c r="R142" s="3"/>
+      <c r="S142" s="4"/>
+      <c r="T142" s="4"/>
+    </row>
+    <row r="143" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B143" s="4"/>
+      <c r="C143" s="3"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="3"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="3"/>
+      <c r="H143" s="4"/>
+      <c r="I143" s="3"/>
+      <c r="J143" s="4"/>
+      <c r="K143" s="4"/>
+      <c r="L143" s="4"/>
+      <c r="M143" s="4"/>
+      <c r="N143" s="4"/>
+      <c r="O143" s="4"/>
+      <c r="P143" s="4"/>
+      <c r="Q143" s="4"/>
+      <c r="R143" s="3"/>
+      <c r="S143" s="4"/>
+      <c r="T143" s="4"/>
+    </row>
+    <row r="144" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B144" s="4"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="3"/>
+      <c r="H144" s="4"/>
+      <c r="I144" s="3"/>
+      <c r="J144" s="4"/>
+      <c r="K144" s="4"/>
+      <c r="L144" s="4"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="4"/>
+      <c r="O144" s="4"/>
+      <c r="P144" s="4"/>
+      <c r="Q144" s="4"/>
+      <c r="R144" s="3"/>
+      <c r="S144" s="4"/>
+      <c r="T144" s="4"/>
+    </row>
+    <row r="145" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B145" s="4"/>
+      <c r="C145" s="3"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="3"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="3"/>
+      <c r="H145" s="4"/>
+      <c r="I145" s="3"/>
+      <c r="J145" s="4"/>
+      <c r="K145" s="4"/>
+      <c r="L145" s="4"/>
+      <c r="M145" s="4"/>
+      <c r="N145" s="4"/>
+      <c r="O145" s="4"/>
+      <c r="P145" s="4"/>
+      <c r="Q145" s="4"/>
+      <c r="R145" s="3"/>
+      <c r="S145" s="4"/>
+      <c r="T145" s="4"/>
+    </row>
+    <row r="146" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B146" s="4"/>
+      <c r="C146" s="3"/>
+      <c r="D146" s="4"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="3"/>
+      <c r="H146" s="4"/>
+      <c r="I146" s="3"/>
+      <c r="J146" s="4"/>
+      <c r="K146" s="4"/>
+      <c r="L146" s="4"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="4"/>
+      <c r="O146" s="4"/>
+      <c r="P146" s="4"/>
+      <c r="Q146" s="4"/>
+      <c r="R146" s="3"/>
+      <c r="S146" s="4"/>
+      <c r="T146" s="4"/>
+    </row>
+    <row r="147" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B147" s="4"/>
+      <c r="C147" s="3"/>
+      <c r="D147" s="4"/>
+      <c r="E147" s="3"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="3"/>
+      <c r="H147" s="4"/>
+      <c r="I147" s="3"/>
+      <c r="J147" s="4"/>
+      <c r="K147" s="4"/>
+      <c r="L147" s="4"/>
+      <c r="M147" s="4"/>
+      <c r="N147" s="4"/>
+      <c r="O147" s="4"/>
+      <c r="P147" s="4"/>
+      <c r="Q147" s="4"/>
+      <c r="R147" s="3"/>
+      <c r="S147" s="4"/>
+      <c r="T147" s="4"/>
+    </row>
+    <row r="148" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B148" s="4"/>
+      <c r="C148" s="3"/>
+      <c r="D148" s="4"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="3"/>
+      <c r="H148" s="4"/>
+      <c r="I148" s="3"/>
+      <c r="J148" s="4"/>
+      <c r="K148" s="4"/>
+      <c r="L148" s="4"/>
+      <c r="M148" s="4"/>
+      <c r="N148" s="4"/>
+      <c r="O148" s="4"/>
+      <c r="P148" s="4"/>
+      <c r="Q148" s="4"/>
+      <c r="R148" s="3"/>
+      <c r="S148" s="4"/>
+      <c r="T148" s="4"/>
+    </row>
+    <row r="149" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B149" s="4"/>
+      <c r="C149" s="3"/>
+      <c r="D149" s="4"/>
+      <c r="E149" s="3"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="3"/>
+      <c r="H149" s="4"/>
+      <c r="I149" s="3"/>
+      <c r="J149" s="4"/>
+      <c r="K149" s="4"/>
+      <c r="L149" s="4"/>
+      <c r="M149" s="4"/>
+      <c r="N149" s="4"/>
+      <c r="O149" s="4"/>
+      <c r="P149" s="4"/>
+      <c r="Q149" s="4"/>
+      <c r="R149" s="3"/>
+      <c r="S149" s="4"/>
+      <c r="T149" s="4"/>
+    </row>
+    <row r="150" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B150" s="4"/>
+      <c r="C150" s="3"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="3"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="3"/>
+      <c r="H150" s="4"/>
+      <c r="I150" s="3"/>
+      <c r="J150" s="4"/>
+      <c r="K150" s="4"/>
+      <c r="L150" s="4"/>
+      <c r="M150" s="4"/>
+      <c r="N150" s="4"/>
+      <c r="O150" s="4"/>
+      <c r="P150" s="4"/>
+      <c r="Q150" s="4"/>
+      <c r="R150" s="3"/>
+      <c r="S150" s="4"/>
+      <c r="T150" s="4"/>
+    </row>
+    <row r="151" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B151" s="4"/>
+      <c r="C151" s="3"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="3"/>
+      <c r="F151" s="4"/>
+      <c r="G151" s="3"/>
+      <c r="H151" s="4"/>
+      <c r="I151" s="3"/>
+      <c r="J151" s="4"/>
+      <c r="K151" s="4"/>
+      <c r="L151" s="4"/>
+      <c r="M151" s="4"/>
+      <c r="N151" s="4"/>
+      <c r="O151" s="4"/>
+      <c r="P151" s="4"/>
+      <c r="Q151" s="4"/>
+      <c r="R151" s="3"/>
+      <c r="S151" s="4"/>
+      <c r="T151" s="4"/>
+    </row>
+    <row r="152" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B152" s="4"/>
+      <c r="C152" s="3"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="3"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="3"/>
+      <c r="H152" s="4"/>
+      <c r="I152" s="3"/>
+      <c r="J152" s="4"/>
+      <c r="K152" s="4"/>
+      <c r="L152" s="4"/>
+      <c r="M152" s="4"/>
+      <c r="N152" s="4"/>
+      <c r="O152" s="4"/>
+      <c r="P152" s="4"/>
+      <c r="Q152" s="4"/>
+      <c r="R152" s="3"/>
+      <c r="S152" s="4"/>
+      <c r="T152" s="4"/>
+    </row>
+    <row r="153" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B153" s="4"/>
+      <c r="C153" s="3"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="3"/>
+      <c r="F153" s="4"/>
+      <c r="G153" s="3"/>
+      <c r="H153" s="4"/>
+      <c r="I153" s="3"/>
+      <c r="J153" s="4"/>
+      <c r="K153" s="4"/>
+      <c r="L153" s="4"/>
+      <c r="M153" s="4"/>
+      <c r="N153" s="4"/>
+      <c r="O153" s="4"/>
+      <c r="P153" s="4"/>
+      <c r="Q153" s="4"/>
+      <c r="R153" s="3"/>
+      <c r="S153" s="4"/>
+      <c r="T153" s="4"/>
+    </row>
+    <row r="154" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B154" s="4"/>
+      <c r="C154" s="3"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="3"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="3"/>
+      <c r="H154" s="4"/>
+      <c r="I154" s="3"/>
+      <c r="J154" s="4"/>
+      <c r="K154" s="4"/>
+      <c r="L154" s="4"/>
+      <c r="M154" s="4"/>
+      <c r="N154" s="4"/>
+      <c r="O154" s="4"/>
+      <c r="P154" s="4"/>
+      <c r="Q154" s="4"/>
+      <c r="R154" s="3"/>
+      <c r="S154" s="4"/>
+      <c r="T154" s="4"/>
+    </row>
+    <row r="155" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B155" s="4"/>
+      <c r="C155" s="3"/>
+      <c r="D155" s="4"/>
+      <c r="E155" s="3"/>
+      <c r="F155" s="4"/>
+      <c r="G155" s="3"/>
+      <c r="H155" s="4"/>
+      <c r="I155" s="3"/>
+      <c r="J155" s="4"/>
+      <c r="K155" s="4"/>
+      <c r="L155" s="4"/>
+      <c r="M155" s="4"/>
+      <c r="N155" s="4"/>
+      <c r="O155" s="4"/>
+      <c r="P155" s="4"/>
+      <c r="Q155" s="4"/>
+      <c r="R155" s="3"/>
+      <c r="S155" s="4"/>
+      <c r="T155" s="4"/>
+    </row>
+    <row r="156" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B156" s="4"/>
+      <c r="C156" s="3"/>
+      <c r="D156" s="4"/>
+      <c r="E156" s="3"/>
+      <c r="F156" s="4"/>
+      <c r="G156" s="3"/>
+      <c r="H156" s="4"/>
+      <c r="I156" s="3"/>
+      <c r="J156" s="4"/>
+      <c r="K156" s="4"/>
+      <c r="L156" s="4"/>
+      <c r="M156" s="4"/>
+      <c r="N156" s="4"/>
+      <c r="O156" s="4"/>
+      <c r="P156" s="4"/>
+      <c r="Q156" s="4"/>
+      <c r="R156" s="3"/>
+      <c r="S156" s="4"/>
+      <c r="T156" s="4"/>
+    </row>
+    <row r="157" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B157" s="4"/>
+      <c r="C157" s="3"/>
+      <c r="D157" s="4"/>
+      <c r="E157" s="3"/>
+      <c r="F157" s="4"/>
+      <c r="G157" s="3"/>
+      <c r="H157" s="4"/>
+      <c r="I157" s="3"/>
+      <c r="J157" s="4"/>
+      <c r="K157" s="4"/>
+      <c r="L157" s="4"/>
+      <c r="M157" s="4"/>
+      <c r="N157" s="4"/>
+      <c r="O157" s="4"/>
+      <c r="P157" s="4"/>
+      <c r="Q157" s="4"/>
+      <c r="R157" s="3"/>
+      <c r="S157" s="4"/>
+      <c r="T157" s="4"/>
+    </row>
+    <row r="158" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B158" s="4"/>
+      <c r="C158" s="3"/>
+      <c r="D158" s="4"/>
+      <c r="E158" s="3"/>
+      <c r="F158" s="4"/>
+      <c r="G158" s="3"/>
+      <c r="H158" s="4"/>
+      <c r="I158" s="3"/>
+      <c r="J158" s="4"/>
+      <c r="K158" s="4"/>
+      <c r="L158" s="4"/>
+      <c r="M158" s="4"/>
+      <c r="N158" s="4"/>
+      <c r="O158" s="4"/>
+      <c r="P158" s="4"/>
+      <c r="Q158" s="4"/>
+      <c r="R158" s="3"/>
+      <c r="S158" s="4"/>
+      <c r="T158" s="4"/>
+    </row>
+    <row r="159" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B159" s="4"/>
+      <c r="C159" s="3"/>
+      <c r="D159" s="4"/>
+      <c r="E159" s="3"/>
+      <c r="F159" s="4"/>
+      <c r="G159" s="3"/>
+      <c r="H159" s="4"/>
+      <c r="I159" s="3"/>
+      <c r="J159" s="4"/>
+      <c r="K159" s="4"/>
+      <c r="L159" s="4"/>
+      <c r="M159" s="4"/>
+      <c r="N159" s="4"/>
+      <c r="O159" s="4"/>
+      <c r="P159" s="4"/>
+      <c r="Q159" s="4"/>
+      <c r="R159" s="3"/>
+      <c r="S159" s="4"/>
+      <c r="T159" s="4"/>
+    </row>
+    <row r="160" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B160" s="4"/>
+      <c r="C160" s="3"/>
+      <c r="D160" s="4"/>
+      <c r="E160" s="3"/>
+      <c r="F160" s="4"/>
+      <c r="G160" s="3"/>
+      <c r="H160" s="4"/>
+      <c r="I160" s="3"/>
+      <c r="J160" s="4"/>
+      <c r="K160" s="4"/>
+      <c r="L160" s="4"/>
+      <c r="M160" s="4"/>
+      <c r="N160" s="4"/>
+      <c r="O160" s="4"/>
+      <c r="P160" s="4"/>
+      <c r="Q160" s="4"/>
+      <c r="R160" s="3"/>
+      <c r="S160" s="4"/>
+      <c r="T160" s="4"/>
+    </row>
+    <row r="161" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B161" s="4"/>
+      <c r="C161" s="3"/>
+      <c r="D161" s="4"/>
+      <c r="E161" s="3"/>
+      <c r="F161" s="4"/>
+      <c r="G161" s="3"/>
+      <c r="H161" s="4"/>
+      <c r="I161" s="3"/>
+      <c r="J161" s="4"/>
+      <c r="K161" s="4"/>
+      <c r="L161" s="4"/>
+      <c r="M161" s="4"/>
+      <c r="N161" s="4"/>
+      <c r="O161" s="4"/>
+      <c r="P161" s="4"/>
+      <c r="Q161" s="4"/>
+      <c r="R161" s="3"/>
+      <c r="S161" s="4"/>
+      <c r="T161" s="4"/>
+    </row>
+    <row r="162" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B162" s="4"/>
+      <c r="C162" s="3"/>
+      <c r="D162" s="4"/>
+      <c r="E162" s="3"/>
+      <c r="F162" s="4"/>
+      <c r="G162" s="3"/>
+      <c r="H162" s="4"/>
+      <c r="I162" s="3"/>
+      <c r="J162" s="4"/>
+      <c r="K162" s="4"/>
+      <c r="L162" s="4"/>
+      <c r="M162" s="4"/>
+      <c r="N162" s="4"/>
+      <c r="O162" s="4"/>
+      <c r="P162" s="4"/>
+      <c r="Q162" s="4"/>
+      <c r="R162" s="3"/>
+      <c r="S162" s="4"/>
+      <c r="T162" s="4"/>
+    </row>
+    <row r="163" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B163" s="4"/>
+      <c r="C163" s="3"/>
+      <c r="D163" s="4"/>
+      <c r="E163" s="3"/>
+      <c r="F163" s="4"/>
+      <c r="G163" s="3"/>
+      <c r="H163" s="4"/>
+      <c r="I163" s="3"/>
+      <c r="J163" s="4"/>
+      <c r="K163" s="4"/>
+      <c r="L163" s="4"/>
+      <c r="M163" s="4"/>
+      <c r="N163" s="4"/>
+      <c r="O163" s="4"/>
+      <c r="P163" s="4"/>
+      <c r="Q163" s="4"/>
+      <c r="R163" s="3"/>
+      <c r="S163" s="4"/>
+      <c r="T163" s="4"/>
+    </row>
+    <row r="164" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B164" s="4"/>
+      <c r="C164" s="3"/>
+      <c r="D164" s="4"/>
+      <c r="E164" s="3"/>
+      <c r="F164" s="4"/>
+      <c r="G164" s="3"/>
+      <c r="H164" s="4"/>
+      <c r="I164" s="3"/>
+      <c r="J164" s="4"/>
+      <c r="K164" s="4"/>
+      <c r="L164" s="4"/>
+      <c r="M164" s="4"/>
+      <c r="N164" s="4"/>
+      <c r="O164" s="4"/>
+      <c r="P164" s="4"/>
+      <c r="Q164" s="4"/>
+      <c r="R164" s="3"/>
+      <c r="S164" s="4"/>
+      <c r="T164" s="4"/>
+    </row>
+    <row r="165" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B165" s="4"/>
+      <c r="C165" s="3"/>
+      <c r="D165" s="4"/>
+      <c r="E165" s="3"/>
+      <c r="F165" s="4"/>
+      <c r="G165" s="3"/>
+      <c r="H165" s="4"/>
+      <c r="I165" s="3"/>
+      <c r="J165" s="4"/>
+      <c r="K165" s="4"/>
+      <c r="L165" s="4"/>
+      <c r="M165" s="4"/>
+      <c r="N165" s="4"/>
+      <c r="O165" s="4"/>
+      <c r="P165" s="4"/>
+      <c r="Q165" s="4"/>
+      <c r="R165" s="3"/>
+      <c r="S165" s="4"/>
+      <c r="T165" s="4"/>
+    </row>
+    <row r="166" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B166" s="4"/>
+      <c r="C166" s="3"/>
+      <c r="D166" s="4"/>
+      <c r="E166" s="3"/>
+      <c r="F166" s="4"/>
+      <c r="G166" s="3"/>
+      <c r="H166" s="4"/>
+      <c r="I166" s="3"/>
+      <c r="J166" s="4"/>
+      <c r="K166" s="4"/>
+      <c r="L166" s="4"/>
+      <c r="M166" s="4"/>
+      <c r="N166" s="4"/>
+      <c r="O166" s="4"/>
+      <c r="P166" s="4"/>
+      <c r="Q166" s="4"/>
+      <c r="R166" s="3"/>
+      <c r="S166" s="4"/>
+      <c r="T166" s="4"/>
+    </row>
+    <row r="167" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B167" s="4"/>
+      <c r="C167" s="3"/>
+      <c r="D167" s="4"/>
+      <c r="E167" s="3"/>
+      <c r="F167" s="4"/>
+      <c r="G167" s="3"/>
+      <c r="H167" s="4"/>
+      <c r="I167" s="3"/>
+      <c r="J167" s="4"/>
+      <c r="K167" s="4"/>
+      <c r="L167" s="4"/>
+      <c r="M167" s="4"/>
+      <c r="N167" s="4"/>
+      <c r="O167" s="4"/>
+      <c r="P167" s="4"/>
+      <c r="Q167" s="4"/>
+      <c r="R167" s="3"/>
+      <c r="S167" s="4"/>
+      <c r="T167" s="4"/>
+    </row>
+    <row r="168" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B168" s="4"/>
+      <c r="C168" s="3"/>
+      <c r="D168" s="4"/>
+      <c r="E168" s="3"/>
+      <c r="F168" s="4"/>
+      <c r="G168" s="3"/>
+      <c r="H168" s="4"/>
+      <c r="I168" s="3"/>
+      <c r="J168" s="4"/>
+      <c r="K168" s="4"/>
+      <c r="L168" s="4"/>
+      <c r="M168" s="4"/>
+      <c r="N168" s="4"/>
+      <c r="O168" s="4"/>
+      <c r="P168" s="4"/>
+      <c r="Q168" s="4"/>
+      <c r="R168" s="3"/>
+      <c r="S168" s="4"/>
+      <c r="T168" s="4"/>
+    </row>
+    <row r="169" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B169" s="4"/>
+      <c r="C169" s="3"/>
+      <c r="D169" s="4"/>
+      <c r="E169" s="3"/>
+      <c r="F169" s="4"/>
+      <c r="G169" s="3"/>
+      <c r="H169" s="4"/>
+      <c r="I169" s="3"/>
+      <c r="J169" s="4"/>
+      <c r="K169" s="4"/>
+      <c r="L169" s="4"/>
+      <c r="M169" s="4"/>
+      <c r="N169" s="4"/>
+      <c r="O169" s="4"/>
+      <c r="P169" s="4"/>
+      <c r="Q169" s="4"/>
+      <c r="R169" s="3"/>
+      <c r="S169" s="4"/>
+      <c r="T169" s="4"/>
+    </row>
+    <row r="170" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B170" s="4"/>
+      <c r="C170" s="3"/>
+      <c r="D170" s="4"/>
+      <c r="E170" s="3"/>
+      <c r="F170" s="4"/>
+      <c r="G170" s="3"/>
+      <c r="H170" s="4"/>
+      <c r="I170" s="3"/>
+      <c r="J170" s="4"/>
+      <c r="K170" s="4"/>
+      <c r="L170" s="4"/>
+      <c r="M170" s="4"/>
+      <c r="N170" s="4"/>
+      <c r="O170" s="4"/>
+      <c r="P170" s="4"/>
+      <c r="Q170" s="4"/>
+      <c r="R170" s="3"/>
+      <c r="S170" s="4"/>
+      <c r="T170" s="4"/>
+    </row>
+    <row r="171" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B171" s="4"/>
+      <c r="C171" s="3"/>
+      <c r="D171" s="4"/>
+      <c r="E171" s="3"/>
+      <c r="F171" s="4"/>
+      <c r="G171" s="3"/>
+      <c r="H171" s="4"/>
+      <c r="I171" s="3"/>
+      <c r="J171" s="4"/>
+      <c r="K171" s="4"/>
+      <c r="L171" s="4"/>
+      <c r="M171" s="4"/>
+      <c r="N171" s="4"/>
+      <c r="O171" s="4"/>
+      <c r="P171" s="4"/>
+      <c r="Q171" s="4"/>
+      <c r="R171" s="3"/>
+      <c r="S171" s="4"/>
+      <c r="T171" s="4"/>
+    </row>
+    <row r="172" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B172" s="4"/>
+      <c r="C172" s="3"/>
+      <c r="D172" s="4"/>
+      <c r="E172" s="3"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="3"/>
+      <c r="H172" s="4"/>
+      <c r="I172" s="3"/>
+      <c r="J172" s="4"/>
+      <c r="K172" s="4"/>
+      <c r="L172" s="4"/>
+      <c r="M172" s="4"/>
+      <c r="N172" s="4"/>
+      <c r="O172" s="4"/>
+      <c r="P172" s="4"/>
+      <c r="Q172" s="4"/>
+      <c r="R172" s="3"/>
+      <c r="S172" s="4"/>
+      <c r="T172" s="4"/>
+    </row>
+    <row r="173" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B173" s="4"/>
+      <c r="C173" s="3"/>
+      <c r="D173" s="4"/>
+      <c r="E173" s="3"/>
+      <c r="F173" s="4"/>
+      <c r="G173" s="3"/>
+      <c r="H173" s="4"/>
+      <c r="I173" s="3"/>
+      <c r="J173" s="4"/>
+      <c r="K173" s="4"/>
+      <c r="L173" s="4"/>
+      <c r="M173" s="4"/>
+      <c r="N173" s="4"/>
+      <c r="O173" s="4"/>
+      <c r="P173" s="4"/>
+      <c r="Q173" s="4"/>
+      <c r="R173" s="3"/>
+      <c r="S173" s="4"/>
+      <c r="T173" s="4"/>
+    </row>
+    <row r="174" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B174" s="4"/>
+      <c r="C174" s="3"/>
+      <c r="D174" s="4"/>
+      <c r="E174" s="3"/>
+      <c r="F174" s="4"/>
+      <c r="G174" s="3"/>
+      <c r="H174" s="4"/>
+      <c r="I174" s="3"/>
+      <c r="J174" s="4"/>
+      <c r="K174" s="4"/>
+      <c r="L174" s="4"/>
+      <c r="M174" s="4"/>
+      <c r="N174" s="4"/>
+      <c r="O174" s="4"/>
+      <c r="P174" s="4"/>
+      <c r="Q174" s="4"/>
+      <c r="R174" s="3"/>
+      <c r="S174" s="4"/>
+      <c r="T174" s="4"/>
+    </row>
+    <row r="175" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B175" s="4"/>
+      <c r="C175" s="3"/>
+      <c r="D175" s="4"/>
+      <c r="E175" s="3"/>
+      <c r="F175" s="4"/>
+      <c r="G175" s="3"/>
+      <c r="H175" s="4"/>
+      <c r="I175" s="3"/>
+      <c r="J175" s="4"/>
+      <c r="K175" s="4"/>
+      <c r="L175" s="4"/>
+      <c r="M175" s="4"/>
+      <c r="N175" s="4"/>
+      <c r="O175" s="4"/>
+      <c r="P175" s="4"/>
+      <c r="Q175" s="4"/>
+      <c r="R175" s="3"/>
+      <c r="S175" s="4"/>
+      <c r="T175" s="4"/>
+    </row>
+    <row r="176" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B176" s="4"/>
+      <c r="C176" s="3"/>
+      <c r="D176" s="4"/>
+      <c r="E176" s="3"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="3"/>
+      <c r="H176" s="4"/>
+      <c r="I176" s="3"/>
+      <c r="J176" s="4"/>
+      <c r="K176" s="4"/>
+      <c r="L176" s="4"/>
+      <c r="M176" s="4"/>
+      <c r="N176" s="4"/>
+      <c r="O176" s="4"/>
+      <c r="P176" s="4"/>
+      <c r="Q176" s="4"/>
+      <c r="R176" s="3"/>
+      <c r="S176" s="4"/>
+      <c r="T176" s="4"/>
+    </row>
+    <row r="177" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B177" s="4"/>
+      <c r="C177" s="3"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="3"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="3"/>
+      <c r="H177" s="4"/>
+      <c r="I177" s="3"/>
+      <c r="J177" s="4"/>
+      <c r="K177" s="4"/>
+      <c r="L177" s="4"/>
+      <c r="M177" s="4"/>
+      <c r="N177" s="4"/>
+      <c r="O177" s="4"/>
+      <c r="P177" s="4"/>
+      <c r="Q177" s="4"/>
+      <c r="R177" s="3"/>
+      <c r="S177" s="4"/>
+      <c r="T177" s="4"/>
+    </row>
+    <row r="178" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B178" s="4"/>
+      <c r="C178" s="3"/>
+      <c r="D178" s="4"/>
+      <c r="E178" s="3"/>
+      <c r="F178" s="4"/>
+      <c r="G178" s="3"/>
+      <c r="H178" s="4"/>
+      <c r="I178" s="3"/>
+      <c r="J178" s="4"/>
+      <c r="K178" s="4"/>
+      <c r="L178" s="4"/>
+      <c r="M178" s="4"/>
+      <c r="N178" s="4"/>
+      <c r="O178" s="4"/>
+      <c r="P178" s="4"/>
+      <c r="Q178" s="4"/>
+      <c r="R178" s="3"/>
+      <c r="S178" s="4"/>
+      <c r="T178" s="4"/>
+    </row>
+    <row r="179" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B179" s="4"/>
+      <c r="C179" s="3"/>
+      <c r="D179" s="4"/>
+      <c r="E179" s="3"/>
+      <c r="F179" s="4"/>
+      <c r="G179" s="3"/>
+      <c r="H179" s="4"/>
+      <c r="I179" s="3"/>
+      <c r="J179" s="4"/>
+      <c r="K179" s="4"/>
+      <c r="L179" s="4"/>
+      <c r="M179" s="4"/>
+      <c r="N179" s="4"/>
+      <c r="O179" s="4"/>
+      <c r="P179" s="4"/>
+      <c r="Q179" s="4"/>
+      <c r="R179" s="3"/>
+      <c r="S179" s="4"/>
+      <c r="T179" s="4"/>
+    </row>
+    <row r="180" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B180" s="4"/>
+      <c r="C180" s="3"/>
+      <c r="D180" s="4"/>
+      <c r="E180" s="3"/>
+      <c r="F180" s="4"/>
+      <c r="G180" s="3"/>
+      <c r="H180" s="4"/>
+      <c r="I180" s="3"/>
+      <c r="J180" s="4"/>
+      <c r="K180" s="4"/>
+      <c r="L180" s="4"/>
+      <c r="M180" s="4"/>
+      <c r="N180" s="4"/>
+      <c r="O180" s="4"/>
+      <c r="P180" s="4"/>
+      <c r="Q180" s="4"/>
+      <c r="R180" s="3"/>
+      <c r="S180" s="4"/>
+      <c r="T180" s="4"/>
+    </row>
+    <row r="181" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B181" s="4"/>
+      <c r="C181" s="3"/>
+      <c r="D181" s="4"/>
+      <c r="E181" s="3"/>
+      <c r="F181" s="4"/>
+      <c r="G181" s="3"/>
+      <c r="H181" s="4"/>
+      <c r="I181" s="3"/>
+      <c r="J181" s="4"/>
+      <c r="K181" s="4"/>
+      <c r="L181" s="4"/>
+      <c r="M181" s="4"/>
+      <c r="N181" s="4"/>
+      <c r="O181" s="4"/>
+      <c r="P181" s="4"/>
+      <c r="Q181" s="4"/>
+      <c r="R181" s="3"/>
+      <c r="S181" s="4"/>
+      <c r="T181" s="4"/>
+    </row>
+    <row r="182" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B182" s="4"/>
+      <c r="C182" s="3"/>
+      <c r="D182" s="4"/>
+      <c r="E182" s="3"/>
+      <c r="F182" s="4"/>
+      <c r="G182" s="3"/>
+      <c r="H182" s="4"/>
+      <c r="I182" s="3"/>
+      <c r="J182" s="4"/>
+      <c r="K182" s="4"/>
+      <c r="L182" s="4"/>
+      <c r="M182" s="4"/>
+      <c r="N182" s="4"/>
+      <c r="O182" s="4"/>
+      <c r="P182" s="4"/>
+      <c r="Q182" s="4"/>
+      <c r="R182" s="3"/>
+      <c r="S182" s="4"/>
+      <c r="T182" s="4"/>
+    </row>
+    <row r="183" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B183" s="4"/>
+      <c r="C183" s="3"/>
+      <c r="D183" s="4"/>
+      <c r="E183" s="3"/>
+      <c r="F183" s="4"/>
+      <c r="G183" s="3"/>
+      <c r="H183" s="4"/>
+      <c r="I183" s="3"/>
+      <c r="J183" s="4"/>
+      <c r="K183" s="4"/>
+      <c r="L183" s="4"/>
+      <c r="M183" s="4"/>
+      <c r="N183" s="4"/>
+      <c r="O183" s="4"/>
+      <c r="P183" s="4"/>
+      <c r="Q183" s="4"/>
+      <c r="R183" s="3"/>
+      <c r="S183" s="4"/>
+      <c r="T183" s="4"/>
+    </row>
+    <row r="184" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B184" s="4"/>
+      <c r="C184" s="3"/>
+      <c r="D184" s="4"/>
+      <c r="E184" s="3"/>
+      <c r="F184" s="4"/>
+      <c r="G184" s="3"/>
+      <c r="H184" s="4"/>
+      <c r="I184" s="3"/>
+      <c r="J184" s="4"/>
+      <c r="K184" s="4"/>
+      <c r="L184" s="4"/>
+      <c r="M184" s="4"/>
+      <c r="N184" s="4"/>
+      <c r="O184" s="4"/>
+      <c r="P184" s="4"/>
+      <c r="Q184" s="4"/>
+      <c r="R184" s="3"/>
+      <c r="S184" s="4"/>
+      <c r="T184" s="4"/>
+    </row>
+    <row r="185" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B185" s="4"/>
+      <c r="C185" s="3"/>
+      <c r="D185" s="4"/>
+      <c r="E185" s="3"/>
+      <c r="F185" s="4"/>
+      <c r="G185" s="3"/>
+      <c r="H185" s="4"/>
+      <c r="I185" s="3"/>
+      <c r="J185" s="4"/>
+      <c r="K185" s="4"/>
+      <c r="L185" s="4"/>
+      <c r="M185" s="4"/>
+      <c r="N185" s="4"/>
+      <c r="O185" s="4"/>
+      <c r="P185" s="4"/>
+      <c r="Q185" s="4"/>
+      <c r="R185" s="3"/>
+      <c r="S185" s="4"/>
+      <c r="T185" s="4"/>
+    </row>
+    <row r="186" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B186" s="4"/>
+      <c r="C186" s="3"/>
+      <c r="D186" s="4"/>
+      <c r="E186" s="3"/>
+      <c r="F186" s="4"/>
+      <c r="G186" s="3"/>
+      <c r="H186" s="4"/>
+      <c r="I186" s="3"/>
+      <c r="J186" s="4"/>
+      <c r="K186" s="4"/>
+      <c r="L186" s="4"/>
+      <c r="M186" s="4"/>
+      <c r="N186" s="4"/>
+      <c r="O186" s="4"/>
+      <c r="P186" s="4"/>
+      <c r="Q186" s="4"/>
+      <c r="R186" s="3"/>
+      <c r="S186" s="4"/>
+      <c r="T186" s="4"/>
+    </row>
+    <row r="187" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B187" s="4"/>
+      <c r="C187" s="3"/>
+      <c r="D187" s="4"/>
+      <c r="E187" s="3"/>
+      <c r="F187" s="4"/>
+      <c r="G187" s="3"/>
+      <c r="H187" s="4"/>
+      <c r="I187" s="3"/>
+      <c r="J187" s="4"/>
+      <c r="K187" s="4"/>
+      <c r="L187" s="4"/>
+      <c r="M187" s="4"/>
+      <c r="N187" s="4"/>
+      <c r="O187" s="4"/>
+      <c r="P187" s="4"/>
+      <c r="Q187" s="4"/>
+      <c r="R187" s="3"/>
+      <c r="S187" s="4"/>
+      <c r="T187" s="4"/>
+    </row>
+    <row r="188" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B188" s="4"/>
+      <c r="C188" s="3"/>
+      <c r="D188" s="4"/>
+      <c r="E188" s="3"/>
+      <c r="F188" s="4"/>
+      <c r="G188" s="3"/>
+      <c r="H188" s="4"/>
+      <c r="I188" s="3"/>
+      <c r="J188" s="4"/>
+      <c r="K188" s="4"/>
+      <c r="L188" s="4"/>
+      <c r="M188" s="4"/>
+      <c r="N188" s="4"/>
+      <c r="O188" s="4"/>
+      <c r="P188" s="4"/>
+      <c r="Q188" s="4"/>
+      <c r="R188" s="3"/>
+      <c r="S188" s="4"/>
+      <c r="T188" s="4"/>
+    </row>
+    <row r="189" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B189" s="4"/>
+      <c r="C189" s="3"/>
+      <c r="D189" s="4"/>
+      <c r="E189" s="3"/>
+      <c r="F189" s="4"/>
+      <c r="G189" s="3"/>
+      <c r="H189" s="4"/>
+      <c r="I189" s="3"/>
+      <c r="J189" s="4"/>
+      <c r="K189" s="4"/>
+      <c r="L189" s="4"/>
+      <c r="M189" s="4"/>
+      <c r="N189" s="4"/>
+      <c r="O189" s="4"/>
+      <c r="P189" s="4"/>
+      <c r="Q189" s="4"/>
+      <c r="R189" s="3"/>
+      <c r="S189" s="4"/>
+      <c r="T189" s="4"/>
+    </row>
+    <row r="190" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B190" s="4"/>
+      <c r="C190" s="3"/>
+      <c r="D190" s="4"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="4"/>
+      <c r="G190" s="3"/>
+      <c r="H190" s="4"/>
+      <c r="I190" s="3"/>
+      <c r="J190" s="4"/>
+      <c r="K190" s="4"/>
+      <c r="L190" s="4"/>
+      <c r="M190" s="4"/>
+      <c r="N190" s="4"/>
+      <c r="O190" s="4"/>
+      <c r="P190" s="4"/>
+      <c r="Q190" s="4"/>
+      <c r="R190" s="3"/>
+      <c r="S190" s="4"/>
+      <c r="T190" s="4"/>
+    </row>
+    <row r="191" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B191" s="4"/>
+      <c r="C191" s="3"/>
+      <c r="D191" s="4"/>
+      <c r="E191" s="3"/>
+      <c r="F191" s="4"/>
+      <c r="G191" s="3"/>
+      <c r="H191" s="4"/>
+      <c r="I191" s="3"/>
+      <c r="J191" s="4"/>
+      <c r="K191" s="4"/>
+      <c r="L191" s="4"/>
+      <c r="M191" s="4"/>
+      <c r="N191" s="4"/>
+      <c r="O191" s="4"/>
+      <c r="P191" s="4"/>
+      <c r="Q191" s="4"/>
+      <c r="R191" s="3"/>
+      <c r="S191" s="4"/>
+      <c r="T191" s="4"/>
+    </row>
+    <row r="192" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B192" s="4"/>
+      <c r="C192" s="3"/>
+      <c r="D192" s="4"/>
+      <c r="E192" s="3"/>
+      <c r="F192" s="4"/>
+      <c r="G192" s="3"/>
+      <c r="H192" s="4"/>
+      <c r="I192" s="3"/>
+      <c r="J192" s="4"/>
+      <c r="K192" s="4"/>
+      <c r="L192" s="4"/>
+      <c r="M192" s="4"/>
+      <c r="N192" s="4"/>
+      <c r="O192" s="4"/>
+      <c r="P192" s="4"/>
+      <c r="Q192" s="4"/>
+      <c r="R192" s="3"/>
+      <c r="S192" s="4"/>
+      <c r="T192" s="4"/>
+    </row>
+    <row r="193" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B193" s="4"/>
+      <c r="C193" s="3"/>
+      <c r="D193" s="4"/>
+      <c r="E193" s="3"/>
+      <c r="F193" s="4"/>
+      <c r="G193" s="3"/>
+      <c r="H193" s="4"/>
+      <c r="I193" s="3"/>
+      <c r="J193" s="4"/>
+      <c r="K193" s="4"/>
+      <c r="L193" s="4"/>
+      <c r="M193" s="4"/>
+      <c r="N193" s="4"/>
+      <c r="O193" s="4"/>
+      <c r="P193" s="4"/>
+      <c r="Q193" s="4"/>
+      <c r="R193" s="3"/>
+      <c r="S193" s="4"/>
+      <c r="T193" s="4"/>
+    </row>
+    <row r="194" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B194" s="4"/>
+      <c r="C194" s="3"/>
+      <c r="D194" s="4"/>
+      <c r="E194" s="3"/>
+      <c r="F194" s="4"/>
+      <c r="G194" s="3"/>
+      <c r="H194" s="4"/>
+      <c r="I194" s="3"/>
+      <c r="J194" s="4"/>
+      <c r="K194" s="4"/>
+      <c r="L194" s="4"/>
+      <c r="M194" s="4"/>
+      <c r="N194" s="4"/>
+      <c r="O194" s="4"/>
+      <c r="P194" s="4"/>
+      <c r="Q194" s="4"/>
+      <c r="R194" s="3"/>
+      <c r="S194" s="4"/>
+      <c r="T194" s="4"/>
+    </row>
+    <row r="195" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B195" s="4"/>
+      <c r="C195" s="3"/>
+      <c r="D195" s="4"/>
+      <c r="E195" s="3"/>
+      <c r="F195" s="4"/>
+      <c r="G195" s="3"/>
+      <c r="H195" s="4"/>
+      <c r="I195" s="3"/>
+      <c r="J195" s="4"/>
+      <c r="K195" s="4"/>
+      <c r="L195" s="4"/>
+      <c r="M195" s="4"/>
+      <c r="N195" s="4"/>
+      <c r="O195" s="4"/>
+      <c r="P195" s="4"/>
+      <c r="Q195" s="4"/>
+      <c r="R195" s="3"/>
+      <c r="S195" s="4"/>
+      <c r="T195" s="4"/>
+    </row>
+    <row r="196" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B196" s="4"/>
+      <c r="C196" s="3"/>
+      <c r="D196" s="4"/>
+      <c r="E196" s="3"/>
+      <c r="F196" s="4"/>
+      <c r="G196" s="3"/>
+      <c r="H196" s="4"/>
+      <c r="I196" s="3"/>
+      <c r="J196" s="4"/>
+      <c r="K196" s="4"/>
+      <c r="L196" s="4"/>
+      <c r="M196" s="4"/>
+      <c r="N196" s="4"/>
+      <c r="O196" s="4"/>
+      <c r="P196" s="4"/>
+      <c r="Q196" s="4"/>
+      <c r="R196" s="3"/>
+      <c r="S196" s="4"/>
+      <c r="T196" s="4"/>
+    </row>
+    <row r="197" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B197" s="4"/>
+      <c r="C197" s="3"/>
+      <c r="D197" s="4"/>
+      <c r="E197" s="3"/>
+      <c r="F197" s="4"/>
+      <c r="G197" s="3"/>
+      <c r="H197" s="4"/>
+      <c r="I197" s="3"/>
+      <c r="J197" s="4"/>
+      <c r="K197" s="4"/>
+      <c r="L197" s="4"/>
+      <c r="M197" s="4"/>
+      <c r="N197" s="4"/>
+      <c r="O197" s="4"/>
+      <c r="P197" s="4"/>
+      <c r="Q197" s="4"/>
+      <c r="R197" s="3"/>
+      <c r="S197" s="4"/>
+      <c r="T197" s="4"/>
+    </row>
+    <row r="198" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B198" s="4"/>
+      <c r="C198" s="3"/>
+      <c r="D198" s="4"/>
+      <c r="E198" s="3"/>
+      <c r="F198" s="4"/>
+      <c r="G198" s="3"/>
+      <c r="H198" s="4"/>
+      <c r="I198" s="3"/>
+      <c r="J198" s="4"/>
+      <c r="K198" s="4"/>
+      <c r="L198" s="4"/>
+      <c r="M198" s="4"/>
+      <c r="N198" s="4"/>
+      <c r="O198" s="4"/>
+      <c r="P198" s="4"/>
+      <c r="Q198" s="4"/>
+      <c r="R198" s="3"/>
+      <c r="S198" s="4"/>
+      <c r="T198" s="4"/>
+    </row>
+    <row r="199" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B199" s="4"/>
+      <c r="C199" s="3"/>
+      <c r="D199" s="4"/>
+      <c r="E199" s="3"/>
+      <c r="F199" s="4"/>
+      <c r="G199" s="3"/>
+      <c r="H199" s="4"/>
+      <c r="I199" s="3"/>
+      <c r="J199" s="4"/>
+      <c r="K199" s="4"/>
+      <c r="L199" s="4"/>
+      <c r="M199" s="4"/>
+      <c r="N199" s="4"/>
+      <c r="O199" s="4"/>
+      <c r="P199" s="4"/>
+      <c r="Q199" s="4"/>
+      <c r="R199" s="3"/>
+      <c r="S199" s="4"/>
+      <c r="T199" s="4"/>
+    </row>
+    <row r="200" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B200" s="4"/>
+      <c r="C200" s="3"/>
+      <c r="D200" s="4"/>
+      <c r="E200" s="3"/>
+      <c r="F200" s="4"/>
+      <c r="G200" s="3"/>
+      <c r="H200" s="4"/>
+      <c r="I200" s="3"/>
+      <c r="J200" s="4"/>
+      <c r="K200" s="4"/>
+      <c r="L200" s="4"/>
+      <c r="M200" s="4"/>
+      <c r="N200" s="4"/>
+      <c r="O200" s="4"/>
+      <c r="P200" s="4"/>
+      <c r="Q200" s="4"/>
+      <c r="R200" s="3"/>
+      <c r="S200" s="4"/>
+      <c r="T200" s="4"/>
+    </row>
+    <row r="201" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B201" s="4"/>
+      <c r="C201" s="3"/>
+      <c r="D201" s="4"/>
+      <c r="E201" s="3"/>
+      <c r="F201" s="4"/>
+      <c r="G201" s="3"/>
+      <c r="H201" s="4"/>
+      <c r="I201" s="3"/>
+      <c r="J201" s="4"/>
+      <c r="K201" s="4"/>
+      <c r="L201" s="4"/>
+      <c r="M201" s="4"/>
+      <c r="N201" s="4"/>
+      <c r="O201" s="4"/>
+      <c r="P201" s="4"/>
+      <c r="Q201" s="4"/>
+      <c r="R201" s="3"/>
+      <c r="S201" s="4"/>
+      <c r="T201" s="4"/>
+    </row>
+    <row r="202" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B202" s="4"/>
+      <c r="C202" s="3"/>
+      <c r="D202" s="4"/>
+      <c r="E202" s="3"/>
+      <c r="F202" s="4"/>
+      <c r="G202" s="3"/>
+      <c r="H202" s="4"/>
+      <c r="I202" s="3"/>
+      <c r="J202" s="4"/>
+      <c r="K202" s="4"/>
+      <c r="L202" s="4"/>
+      <c r="M202" s="4"/>
+      <c r="N202" s="4"/>
+      <c r="O202" s="4"/>
+      <c r="P202" s="4"/>
+      <c r="Q202" s="4"/>
+      <c r="R202" s="3"/>
+      <c r="S202" s="4"/>
+      <c r="T202" s="4"/>
+    </row>
+    <row r="203" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B203" s="4"/>
+      <c r="C203" s="3"/>
+      <c r="D203" s="4"/>
+      <c r="E203" s="3"/>
+      <c r="F203" s="4"/>
+      <c r="G203" s="3"/>
+      <c r="H203" s="4"/>
+      <c r="I203" s="3"/>
+      <c r="J203" s="4"/>
+      <c r="K203" s="4"/>
+      <c r="L203" s="4"/>
+      <c r="M203" s="4"/>
+      <c r="N203" s="4"/>
+      <c r="O203" s="4"/>
+      <c r="P203" s="4"/>
+      <c r="Q203" s="4"/>
+      <c r="R203" s="3"/>
+      <c r="S203" s="4"/>
+      <c r="T203" s="4"/>
+    </row>
+    <row r="204" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B204" s="4"/>
+      <c r="C204" s="3"/>
+      <c r="D204" s="4"/>
+      <c r="E204" s="3"/>
+      <c r="F204" s="4"/>
+      <c r="G204" s="3"/>
+      <c r="H204" s="4"/>
+      <c r="I204" s="3"/>
+      <c r="J204" s="4"/>
+      <c r="K204" s="4"/>
+      <c r="L204" s="4"/>
+      <c r="M204" s="4"/>
+      <c r="N204" s="4"/>
+      <c r="O204" s="4"/>
+      <c r="P204" s="4"/>
+      <c r="Q204" s="4"/>
+      <c r="R204" s="3"/>
+      <c r="S204" s="4"/>
+      <c r="T204" s="4"/>
+    </row>
+    <row r="205" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B205" s="4"/>
+      <c r="C205" s="3"/>
+      <c r="D205" s="4"/>
+      <c r="E205" s="3"/>
+      <c r="F205" s="4"/>
+      <c r="G205" s="3"/>
+      <c r="H205" s="4"/>
+      <c r="I205" s="3"/>
+      <c r="J205" s="4"/>
+      <c r="K205" s="4"/>
+      <c r="L205" s="4"/>
+      <c r="M205" s="4"/>
+      <c r="N205" s="4"/>
+      <c r="O205" s="4"/>
+      <c r="P205" s="4"/>
+      <c r="Q205" s="4"/>
+      <c r="R205" s="3"/>
+      <c r="S205" s="4"/>
+      <c r="T205" s="4"/>
+    </row>
+    <row r="206" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B206" s="4"/>
+      <c r="C206" s="3"/>
+      <c r="D206" s="4"/>
+      <c r="E206" s="3"/>
+      <c r="F206" s="4"/>
+      <c r="G206" s="3"/>
+      <c r="H206" s="4"/>
+      <c r="I206" s="3"/>
+      <c r="J206" s="4"/>
+      <c r="K206" s="4"/>
+      <c r="L206" s="4"/>
+      <c r="M206" s="4"/>
+      <c r="N206" s="4"/>
+      <c r="O206" s="4"/>
+      <c r="P206" s="4"/>
+      <c r="Q206" s="4"/>
+      <c r="R206" s="3"/>
+      <c r="S206" s="4"/>
+      <c r="T206" s="4"/>
+    </row>
+    <row r="207" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B207" s="4"/>
+      <c r="C207" s="3"/>
+      <c r="D207" s="4"/>
+      <c r="E207" s="3"/>
+      <c r="F207" s="4"/>
+      <c r="G207" s="3"/>
+      <c r="H207" s="4"/>
+      <c r="I207" s="3"/>
+      <c r="J207" s="4"/>
+      <c r="K207" s="4"/>
+      <c r="L207" s="4"/>
+      <c r="M207" s="4"/>
+      <c r="N207" s="4"/>
+      <c r="O207" s="4"/>
+      <c r="P207" s="4"/>
+      <c r="Q207" s="4"/>
+      <c r="R207" s="3"/>
+      <c r="S207" s="4"/>
+      <c r="T207" s="4"/>
+    </row>
+    <row r="208" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B208" s="4"/>
+      <c r="C208" s="3"/>
+      <c r="D208" s="4"/>
+      <c r="E208" s="3"/>
+      <c r="F208" s="4"/>
+      <c r="G208" s="3"/>
+      <c r="H208" s="4"/>
+      <c r="I208" s="3"/>
+      <c r="J208" s="4"/>
+      <c r="K208" s="4"/>
+      <c r="L208" s="4"/>
+      <c r="M208" s="4"/>
+      <c r="N208" s="4"/>
+      <c r="O208" s="4"/>
+      <c r="P208" s="4"/>
+      <c r="Q208" s="4"/>
+      <c r="R208" s="3"/>
+      <c r="S208" s="4"/>
+      <c r="T208" s="4"/>
+    </row>
+    <row r="209" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B209" s="4"/>
+      <c r="C209" s="3"/>
+      <c r="D209" s="4"/>
+      <c r="E209" s="3"/>
+      <c r="F209" s="4"/>
+      <c r="G209" s="3"/>
+      <c r="H209" s="4"/>
+      <c r="I209" s="3"/>
+      <c r="J209" s="4"/>
+      <c r="K209" s="4"/>
+      <c r="L209" s="4"/>
+      <c r="M209" s="4"/>
+      <c r="N209" s="4"/>
+      <c r="O209" s="4"/>
+      <c r="P209" s="4"/>
+      <c r="Q209" s="4"/>
+      <c r="R209" s="3"/>
+      <c r="S209" s="4"/>
+      <c r="T209" s="4"/>
+    </row>
+    <row r="210" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B210" s="4"/>
+      <c r="C210" s="3"/>
+      <c r="D210" s="4"/>
+      <c r="E210" s="3"/>
+      <c r="F210" s="4"/>
+      <c r="G210" s="3"/>
+      <c r="H210" s="4"/>
+      <c r="I210" s="3"/>
+      <c r="J210" s="4"/>
+      <c r="K210" s="4"/>
+      <c r="L210" s="4"/>
+      <c r="M210" s="4"/>
+      <c r="N210" s="4"/>
+      <c r="O210" s="4"/>
+      <c r="P210" s="4"/>
+      <c r="Q210" s="4"/>
+      <c r="R210" s="3"/>
+      <c r="S210" s="4"/>
+      <c r="T210" s="4"/>
+    </row>
+    <row r="211" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B211" s="4"/>
+      <c r="C211" s="3"/>
+      <c r="D211" s="4"/>
+      <c r="E211" s="3"/>
+      <c r="F211" s="4"/>
+      <c r="G211" s="3"/>
+      <c r="H211" s="4"/>
+      <c r="I211" s="3"/>
+      <c r="J211" s="4"/>
+      <c r="K211" s="4"/>
+      <c r="L211" s="4"/>
+      <c r="M211" s="4"/>
+      <c r="N211" s="4"/>
+      <c r="O211" s="4"/>
+      <c r="P211" s="4"/>
+      <c r="Q211" s="4"/>
+      <c r="R211" s="3"/>
+      <c r="S211" s="4"/>
+      <c r="T211" s="4"/>
+    </row>
+    <row r="212" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B212" s="4"/>
+      <c r="C212" s="3"/>
+      <c r="D212" s="4"/>
+      <c r="E212" s="3"/>
+      <c r="F212" s="4"/>
+      <c r="G212" s="3"/>
+      <c r="H212" s="4"/>
+      <c r="I212" s="3"/>
+      <c r="J212" s="4"/>
+      <c r="K212" s="4"/>
+      <c r="L212" s="4"/>
+      <c r="M212" s="4"/>
+      <c r="N212" s="4"/>
+      <c r="O212" s="4"/>
+      <c r="P212" s="4"/>
+      <c r="Q212" s="4"/>
+      <c r="R212" s="3"/>
+      <c r="S212" s="4"/>
+      <c r="T212" s="4"/>
+    </row>
+    <row r="213" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B213" s="4"/>
+      <c r="C213" s="3"/>
+      <c r="D213" s="4"/>
+      <c r="E213" s="3"/>
+      <c r="F213" s="4"/>
+      <c r="G213" s="3"/>
+      <c r="H213" s="4"/>
+      <c r="I213" s="3"/>
+      <c r="J213" s="4"/>
+      <c r="K213" s="4"/>
+      <c r="L213" s="4"/>
+      <c r="M213" s="4"/>
+      <c r="N213" s="4"/>
+      <c r="O213" s="4"/>
+      <c r="P213" s="4"/>
+      <c r="Q213" s="4"/>
+      <c r="R213" s="3"/>
+      <c r="S213" s="4"/>
+      <c r="T213" s="4"/>
+    </row>
+    <row r="214" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B214" s="4"/>
+      <c r="C214" s="3"/>
+      <c r="D214" s="4"/>
+      <c r="E214" s="3"/>
+      <c r="F214" s="4"/>
+      <c r="G214" s="3"/>
+      <c r="H214" s="4"/>
+      <c r="I214" s="3"/>
+      <c r="J214" s="4"/>
+      <c r="K214" s="4"/>
+      <c r="L214" s="4"/>
+      <c r="M214" s="4"/>
+      <c r="N214" s="4"/>
+      <c r="O214" s="4"/>
+      <c r="P214" s="4"/>
+      <c r="Q214" s="4"/>
+      <c r="R214" s="3"/>
+      <c r="S214" s="4"/>
+      <c r="T214" s="4"/>
+    </row>
+    <row r="215" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B215" s="4"/>
+      <c r="C215" s="3"/>
+      <c r="D215" s="4"/>
+      <c r="E215" s="3"/>
+      <c r="F215" s="4"/>
+      <c r="G215" s="3"/>
+      <c r="H215" s="4"/>
+      <c r="I215" s="3"/>
+      <c r="J215" s="4"/>
+      <c r="K215" s="4"/>
+      <c r="L215" s="4"/>
+      <c r="M215" s="4"/>
+      <c r="N215" s="4"/>
+      <c r="O215" s="4"/>
+      <c r="P215" s="4"/>
+      <c r="Q215" s="4"/>
+      <c r="R215" s="3"/>
+      <c r="S215" s="4"/>
+      <c r="T215" s="4"/>
+    </row>
+    <row r="216" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B216" s="4"/>
+      <c r="C216" s="3"/>
+      <c r="D216" s="4"/>
+      <c r="E216" s="3"/>
+      <c r="F216" s="4"/>
+      <c r="G216" s="3"/>
+      <c r="H216" s="4"/>
+      <c r="I216" s="3"/>
+      <c r="J216" s="4"/>
+      <c r="K216" s="4"/>
+      <c r="L216" s="4"/>
+      <c r="M216" s="4"/>
+      <c r="N216" s="4"/>
+      <c r="O216" s="4"/>
+      <c r="P216" s="4"/>
+      <c r="Q216" s="4"/>
+      <c r="R216" s="3"/>
+      <c r="S216" s="4"/>
+      <c r="T216" s="4"/>
+    </row>
+    <row r="217" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B217" s="4"/>
+      <c r="C217" s="3"/>
+      <c r="D217" s="4"/>
+      <c r="E217" s="3"/>
+      <c r="F217" s="4"/>
+      <c r="G217" s="3"/>
+      <c r="H217" s="4"/>
+      <c r="I217" s="3"/>
+      <c r="J217" s="4"/>
+      <c r="K217" s="4"/>
+      <c r="L217" s="4"/>
+      <c r="M217" s="4"/>
+      <c r="N217" s="4"/>
+      <c r="O217" s="4"/>
+      <c r="P217" s="4"/>
+      <c r="Q217" s="4"/>
+      <c r="R217" s="3"/>
+      <c r="S217" s="4"/>
+      <c r="T217" s="4"/>
+    </row>
+    <row r="218" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B218" s="4"/>
+      <c r="C218" s="3"/>
+      <c r="D218" s="4"/>
+      <c r="E218" s="3"/>
+      <c r="F218" s="4"/>
+      <c r="G218" s="3"/>
+      <c r="H218" s="4"/>
+      <c r="I218" s="3"/>
+      <c r="J218" s="4"/>
+      <c r="K218" s="4"/>
+      <c r="L218" s="4"/>
+      <c r="M218" s="4"/>
+      <c r="N218" s="4"/>
+      <c r="O218" s="4"/>
+      <c r="P218" s="4"/>
+      <c r="Q218" s="4"/>
+      <c r="R218" s="3"/>
+      <c r="S218" s="4"/>
+      <c r="T218" s="4"/>
+    </row>
+    <row r="219" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B219" s="4"/>
+      <c r="C219" s="3"/>
+      <c r="D219" s="4"/>
+      <c r="E219" s="3"/>
+      <c r="F219" s="4"/>
+      <c r="G219" s="3"/>
+      <c r="H219" s="4"/>
+      <c r="I219" s="3"/>
+      <c r="J219" s="4"/>
+      <c r="K219" s="4"/>
+      <c r="L219" s="4"/>
+      <c r="M219" s="4"/>
+      <c r="N219" s="4"/>
+      <c r="O219" s="4"/>
+      <c r="P219" s="4"/>
+      <c r="Q219" s="4"/>
+      <c r="R219" s="3"/>
+      <c r="S219" s="4"/>
+      <c r="T219" s="4"/>
+    </row>
+    <row r="220" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B220" s="4"/>
+      <c r="C220" s="3"/>
+      <c r="D220" s="4"/>
+      <c r="E220" s="3"/>
+      <c r="F220" s="4"/>
+      <c r="G220" s="3"/>
+      <c r="H220" s="4"/>
+      <c r="I220" s="3"/>
+      <c r="J220" s="4"/>
+      <c r="K220" s="4"/>
+      <c r="L220" s="4"/>
+      <c r="M220" s="4"/>
+      <c r="N220" s="4"/>
+      <c r="O220" s="4"/>
+      <c r="P220" s="4"/>
+      <c r="Q220" s="4"/>
+      <c r="R220" s="3"/>
+      <c r="S220" s="4"/>
+      <c r="T220" s="4"/>
+    </row>
+    <row r="221" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B221" s="4"/>
+      <c r="C221" s="3"/>
+      <c r="D221" s="4"/>
+      <c r="E221" s="3"/>
+      <c r="F221" s="4"/>
+      <c r="G221" s="3"/>
+      <c r="H221" s="4"/>
+      <c r="I221" s="3"/>
+      <c r="J221" s="4"/>
+      <c r="K221" s="4"/>
+      <c r="L221" s="4"/>
+      <c r="M221" s="4"/>
+      <c r="N221" s="4"/>
+      <c r="O221" s="4"/>
+      <c r="P221" s="4"/>
+      <c r="Q221" s="4"/>
+      <c r="R221" s="3"/>
+      <c r="S221" s="4"/>
+      <c r="T221" s="4"/>
+    </row>
+    <row r="222" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B222" s="4"/>
+      <c r="C222" s="3"/>
+      <c r="D222" s="4"/>
+      <c r="E222" s="3"/>
+      <c r="F222" s="4"/>
+      <c r="G222" s="3"/>
+      <c r="H222" s="4"/>
+      <c r="I222" s="3"/>
+      <c r="J222" s="4"/>
+      <c r="K222" s="4"/>
+      <c r="L222" s="4"/>
+      <c r="M222" s="4"/>
+      <c r="N222" s="4"/>
+      <c r="O222" s="4"/>
+      <c r="P222" s="4"/>
+      <c r="Q222" s="4"/>
+      <c r="R222" s="3"/>
+      <c r="S222" s="4"/>
+      <c r="T222" s="4"/>
+    </row>
+    <row r="223" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B223" s="4"/>
+      <c r="C223" s="3"/>
+      <c r="D223" s="4"/>
+      <c r="E223" s="3"/>
+      <c r="F223" s="4"/>
+      <c r="G223" s="3"/>
+      <c r="H223" s="4"/>
+      <c r="I223" s="3"/>
+      <c r="J223" s="4"/>
+      <c r="K223" s="4"/>
+      <c r="L223" s="4"/>
+      <c r="M223" s="4"/>
+      <c r="N223" s="4"/>
+      <c r="O223" s="4"/>
+      <c r="P223" s="4"/>
+      <c r="Q223" s="4"/>
+      <c r="R223" s="3"/>
+      <c r="S223" s="4"/>
+      <c r="T223" s="4"/>
+    </row>
+    <row r="224" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B224" s="4"/>
+      <c r="C224" s="3"/>
+      <c r="D224" s="4"/>
+      <c r="E224" s="3"/>
+      <c r="F224" s="4"/>
+      <c r="G224" s="3"/>
+      <c r="H224" s="4"/>
+      <c r="I224" s="3"/>
+      <c r="J224" s="4"/>
+      <c r="K224" s="4"/>
+      <c r="L224" s="4"/>
+      <c r="M224" s="4"/>
+      <c r="N224" s="4"/>
+      <c r="O224" s="4"/>
+      <c r="P224" s="4"/>
+      <c r="Q224" s="4"/>
+      <c r="R224" s="3"/>
+      <c r="S224" s="4"/>
+      <c r="T224" s="4"/>
+    </row>
+    <row r="225" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B225" s="4"/>
+      <c r="C225" s="3"/>
+      <c r="D225" s="4"/>
+      <c r="E225" s="3"/>
+      <c r="F225" s="4"/>
+      <c r="G225" s="3"/>
+      <c r="H225" s="4"/>
+      <c r="I225" s="3"/>
+      <c r="J225" s="4"/>
+      <c r="K225" s="4"/>
+      <c r="L225" s="4"/>
+      <c r="M225" s="4"/>
+      <c r="N225" s="4"/>
+      <c r="O225" s="4"/>
+      <c r="P225" s="4"/>
+      <c r="Q225" s="4"/>
+      <c r="R225" s="3"/>
+      <c r="S225" s="4"/>
+      <c r="T225" s="4"/>
+    </row>
+    <row r="226" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B226" s="4"/>
+      <c r="C226" s="3"/>
+      <c r="D226" s="4"/>
+      <c r="E226" s="3"/>
+      <c r="F226" s="4"/>
+      <c r="G226" s="3"/>
+      <c r="H226" s="4"/>
+      <c r="I226" s="3"/>
+      <c r="J226" s="4"/>
+      <c r="K226" s="4"/>
+      <c r="L226" s="4"/>
+      <c r="M226" s="4"/>
+      <c r="N226" s="4"/>
+      <c r="O226" s="4"/>
+      <c r="P226" s="4"/>
+      <c r="Q226" s="4"/>
+      <c r="R226" s="3"/>
+      <c r="S226" s="4"/>
+      <c r="T226" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Docs: #9 Update RS including Refactoring Editor Structure
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E77F48-49CD-4B50-A588-9B26865DB0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE277A06-2E49-4A5C-9E51-A513D772ABED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="103">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,10 +55,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>씬 관련</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>S</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -123,10 +119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Scene</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>N</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -207,18 +199,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>새로 만들기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>불러오기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>종료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FR-C-E-01.02</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -227,65 +207,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FR-C-E-01.04</t>
-  </si>
-  <si>
-    <t>FR-C-E-01.04.01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FR-C-E-01.04.02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FR-C-E-01.04.03</t>
-  </si>
-  <si>
-    <t>FR-C-E-01.04.04</t>
-  </si>
-  <si>
-    <t>FR-C-E-01.04.05</t>
-  </si>
-  <si>
-    <t>FR-C-E-01.04.06</t>
-  </si>
-  <si>
-    <t>에디터 켜기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>에디터 초기화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>마우스 이벤트 할당</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>커스텀 버튼들 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>데이터 불러오기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>에디터 끄기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FR-C-E-01.05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>에디터용 인터페이스: 맵 에디터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인 메뉴 UI 토글</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>M</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -381,6 +310,118 @@
   <si>
     <t>일반 텍스트 인풋 모달 인터페이스 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시스템</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFR-S-E-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 에디터 시스템 구조 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 메뉴 버튼 기능 : 새로 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 메뉴 버튼 기능 : 불러오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 메뉴 버튼 기능 : 종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에디터용 인터페이스 함수 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-02.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-S-02.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>json 데이터 불러오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>json 데이터 저장하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-S-02.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFR-S-E-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 및 폴더 구조 정립</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에디터 토글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 내보내기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-02.02</t>
+  </si>
+  <si>
+    <t>FR-C-E-02.03</t>
+  </si>
+  <si>
+    <t>FR-C-E-02.04</t>
+  </si>
+  <si>
+    <t>FR-C-E-02.05</t>
+  </si>
+  <si>
+    <t>FR-C-E-03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지도 에디터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-03.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-03.02</t>
+  </si>
+  <si>
+    <t>FR-C-E-03.03</t>
+  </si>
+  <si>
+    <t>FR-C-E-03.04</t>
+  </si>
+  <si>
+    <t>FR-C-E-03.05</t>
   </si>
 </sst>
 </file>
@@ -764,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U72" sqref="U72"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="U40" sqref="U40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -777,7 +818,7 @@
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
@@ -786,7 +827,7 @@
       </c>
       <c r="S4" s="1"/>
       <c r="T4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
@@ -797,26 +838,26 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" t="s">
-        <v>27</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
@@ -827,53 +868,53 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="H7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
         <v>39</v>
-      </c>
-      <c r="I7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="H8" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="I8" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="J8" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
@@ -883,23 +924,23 @@
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -910,7 +951,7 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="6"/>
       <c r="S12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T12" s="5"/>
     </row>
@@ -920,17 +961,17 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="3"/>
       <c r="H13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -950,9 +991,13 @@
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="4"/>
+      <c r="J14" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
@@ -961,7 +1006,7 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="4"/>
+      <c r="S14" s="1"/>
       <c r="T14" s="4"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
@@ -971,9 +1016,13 @@
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="4"/>
+      <c r="J15" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
@@ -982,7 +1031,7 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="3"/>
-      <c r="S15" s="4"/>
+      <c r="S15" s="1"/>
       <c r="T15" s="4"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
@@ -1136,17 +1185,17 @@
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -1167,11 +1216,11 @@
       <c r="F24" s="4"/>
       <c r="G24" s="3"/>
       <c r="H24" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -1232,15 +1281,15 @@
       <c r="D27" s="4"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -1250,7 +1299,7 @@
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="3"/>
-      <c r="S27" s="2"/>
+      <c r="S27" s="1"/>
       <c r="T27" s="4"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.3">
@@ -1261,11 +1310,11 @@
       <c r="F28" s="4"/>
       <c r="G28" s="3"/>
       <c r="H28" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="4" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -1275,7 +1324,7 @@
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="3"/>
-      <c r="S28" s="2"/>
+      <c r="S28" s="1"/>
       <c r="T28" s="4"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.3">
@@ -1286,11 +1335,11 @@
       <c r="F29" s="4"/>
       <c r="G29" s="3"/>
       <c r="H29" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="4" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -1300,7 +1349,7 @@
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="3"/>
-      <c r="S29" s="2"/>
+      <c r="S29" s="1"/>
       <c r="T29" s="4"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.3">
@@ -1311,11 +1360,11 @@
       <c r="F30" s="4"/>
       <c r="G30" s="3"/>
       <c r="H30" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="4" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -1325,7 +1374,7 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="3"/>
-      <c r="S30" s="2"/>
+      <c r="S30" s="1"/>
       <c r="T30" s="4"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.3">
@@ -1336,11 +1385,11 @@
       <c r="F31" s="4"/>
       <c r="G31" s="3"/>
       <c r="H31" s="4" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="4" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
@@ -1350,7 +1399,7 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="2"/>
+      <c r="S31" s="1"/>
       <c r="T31" s="4"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
@@ -1361,11 +1410,11 @@
       <c r="F32" s="4"/>
       <c r="G32" s="3"/>
       <c r="H32" s="4" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="4" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -1375,7 +1424,7 @@
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="3"/>
-      <c r="S32" s="2"/>
+      <c r="S32" s="1"/>
       <c r="T32" s="4"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.3">
@@ -1386,11 +1435,11 @@
       <c r="F33" s="4"/>
       <c r="G33" s="3"/>
       <c r="H33" s="4" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="4" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -1400,7 +1449,7 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="3"/>
-      <c r="S33" s="2"/>
+      <c r="S33" s="1"/>
       <c r="T33" s="4"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.3">
@@ -1411,11 +1460,11 @@
       <c r="F34" s="4"/>
       <c r="G34" s="3"/>
       <c r="H34" s="4" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -1425,7 +1474,7 @@
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="3"/>
-      <c r="S34" s="2"/>
+      <c r="S34" s="1"/>
       <c r="T34" s="4"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.3">
@@ -1436,11 +1485,11 @@
       <c r="F35" s="4"/>
       <c r="G35" s="3"/>
       <c r="H35" s="4" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="4" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -1450,7 +1499,7 @@
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="3"/>
-      <c r="S35" s="2"/>
+      <c r="S35" s="1"/>
       <c r="T35" s="4"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.3">
@@ -1461,11 +1510,11 @@
       <c r="F36" s="4"/>
       <c r="G36" s="3"/>
       <c r="H36" s="4" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="4" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
@@ -1475,7 +1524,7 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="3"/>
-      <c r="S36" s="2"/>
+      <c r="S36" s="1"/>
       <c r="T36" s="4"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.3">
@@ -1486,11 +1535,11 @@
       <c r="F37" s="4"/>
       <c r="G37" s="3"/>
       <c r="H37" s="4" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="4" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -1511,11 +1560,11 @@
       <c r="F38" s="4"/>
       <c r="G38" s="3"/>
       <c r="H38" s="4" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="4" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
@@ -1535,9 +1584,13 @@
       <c r="E39" s="3"/>
       <c r="F39" s="4"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="4"/>
+      <c r="H39" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="I39" s="3"/>
-      <c r="J39" s="4"/>
+      <c r="J39" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -1546,7 +1599,7 @@
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
       <c r="R39" s="3"/>
-      <c r="S39" s="4"/>
+      <c r="S39" s="2"/>
       <c r="T39" s="4"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.3">
@@ -1556,9 +1609,13 @@
       <c r="E40" s="3"/>
       <c r="F40" s="4"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="4"/>
+      <c r="H40" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="I40" s="3"/>
-      <c r="J40" s="4"/>
+      <c r="J40" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -1567,7 +1624,7 @@
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
       <c r="R40" s="3"/>
-      <c r="S40" s="4"/>
+      <c r="S40" s="2"/>
       <c r="T40" s="4"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.3">
@@ -1577,9 +1634,13 @@
       <c r="E41" s="3"/>
       <c r="F41" s="4"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="4"/>
+      <c r="H41" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="I41" s="3"/>
-      <c r="J41" s="4"/>
+      <c r="J41" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -1588,7 +1649,7 @@
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
       <c r="R41" s="3"/>
-      <c r="S41" s="4"/>
+      <c r="S41" s="2"/>
       <c r="T41" s="4"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.3">
@@ -1598,9 +1659,13 @@
       <c r="E42" s="3"/>
       <c r="F42" s="4"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="4"/>
+      <c r="H42" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="I42" s="3"/>
-      <c r="J42" s="4"/>
+      <c r="J42" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
@@ -1609,7 +1674,7 @@
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="3"/>
-      <c r="S42" s="4"/>
+      <c r="S42" s="2"/>
       <c r="T42" s="4"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.3">
@@ -1786,15 +1851,15 @@
       <c r="D51" s="4"/>
       <c r="E51" s="3"/>
       <c r="F51" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
@@ -1815,11 +1880,11 @@
       <c r="F52" s="4"/>
       <c r="G52" s="3"/>
       <c r="H52" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I52" s="3"/>
       <c r="J52" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -1922,15 +1987,15 @@
       <c r="D57" s="4"/>
       <c r="E57" s="3"/>
       <c r="F57" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="4" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
@@ -1951,11 +2016,11 @@
       <c r="F58" s="4"/>
       <c r="G58" s="3"/>
       <c r="H58" s="4" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
@@ -2287,19 +2352,19 @@
       <c r="B74" s="4"/>
       <c r="C74" s="3"/>
       <c r="D74" s="4" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="4" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="G74" s="3"/>
       <c r="H74" s="4" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="I74" s="3"/>
       <c r="J74" s="4" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
@@ -2320,11 +2385,11 @@
       <c r="F75" s="4"/>
       <c r="G75" s="3"/>
       <c r="H75" s="4" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="I75" s="3"/>
       <c r="J75" s="4" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
@@ -2345,11 +2410,11 @@
       <c r="F76" s="4"/>
       <c r="G76" s="3"/>
       <c r="H76" s="4" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="I76" s="3"/>
       <c r="J76" s="4" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
@@ -2370,11 +2435,11 @@
       <c r="F77" s="4"/>
       <c r="G77" s="3"/>
       <c r="H77" s="4" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="I77" s="3"/>
       <c r="J77" s="4" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
@@ -2395,11 +2460,11 @@
       <c r="F78" s="4"/>
       <c r="G78" s="3"/>
       <c r="H78" s="4" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="I78" s="3"/>
       <c r="J78" s="4" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
@@ -2420,11 +2485,11 @@
       <c r="F79" s="4"/>
       <c r="G79" s="3"/>
       <c r="H79" s="4" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="I79" s="3"/>
       <c r="J79" s="4" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
@@ -2445,11 +2510,11 @@
       <c r="F80" s="4"/>
       <c r="G80" s="3"/>
       <c r="H80" s="4" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="I80" s="3"/>
       <c r="J80" s="4" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="K80" s="4"/>
       <c r="L80" s="4"/>
@@ -2470,11 +2535,11 @@
       <c r="F81" s="4"/>
       <c r="G81" s="3"/>
       <c r="H81" s="4" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="I81" s="3"/>
       <c r="J81" s="4" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="K81" s="4"/>
       <c r="L81" s="4"/>
@@ -2495,11 +2560,11 @@
       <c r="F82" s="4"/>
       <c r="G82" s="3"/>
       <c r="H82" s="4" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="I82" s="3"/>
       <c r="J82" s="4" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
@@ -2520,11 +2585,11 @@
       <c r="F83" s="4"/>
       <c r="G83" s="3"/>
       <c r="H83" s="4" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="I83" s="3"/>
       <c r="J83" s="4" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="K83" s="4"/>
       <c r="L83" s="4"/>
@@ -2685,15 +2750,25 @@
       <c r="T90" s="4"/>
     </row>
     <row r="91" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B91" s="4"/>
+      <c r="B91" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C91" s="3"/>
-      <c r="D91" s="4"/>
+      <c r="D91" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E91" s="3"/>
-      <c r="F91" s="4"/>
+      <c r="F91" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="G91" s="3"/>
-      <c r="H91" s="4"/>
+      <c r="H91" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="I91" s="3"/>
-      <c r="J91" s="4"/>
+      <c r="J91" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
       <c r="M91" s="4"/>
@@ -2702,7 +2777,7 @@
       <c r="P91" s="4"/>
       <c r="Q91" s="4"/>
       <c r="R91" s="3"/>
-      <c r="S91" s="4"/>
+      <c r="S91" s="1"/>
       <c r="T91" s="4"/>
     </row>
     <row r="92" spans="2:20" x14ac:dyDescent="0.3">
@@ -2712,9 +2787,13 @@
       <c r="E92" s="3"/>
       <c r="F92" s="4"/>
       <c r="G92" s="3"/>
-      <c r="H92" s="4"/>
+      <c r="H92" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="I92" s="3"/>
-      <c r="J92" s="4"/>
+      <c r="J92" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
@@ -2723,7 +2802,7 @@
       <c r="P92" s="4"/>
       <c r="Q92" s="4"/>
       <c r="R92" s="3"/>
-      <c r="S92" s="4"/>
+      <c r="S92" s="1"/>
       <c r="T92" s="4"/>
     </row>
     <row r="93" spans="2:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Closes #9 basic editor manager (#13)
* Docs: #9 Add FlowChart for Basic Editor

* Docs: #9 FlowChart for Basic Editor

* Docs: #9 Add Functions for Basic Editor to RS

* Docs: #9 Updating FlowChart for Basic Editor including Modal Module

* Docs: #9 Update FlowChart-Basic-Editor including interface functions

* Docs: #9 Update Class Diagram for Editor

* closes #10 popup modal (#11)

* Docs: #10 Add FlowChart for Popup Modal

* Docs: #10 Add FlowChart for Popup Modal Module

* Docs: #10 Update FloawChart for Popup Modal Module

* Docs: #10 Update RS for Modal Module

* Docs: #10 Update + Rearrange Class Diagram

* Docs: #9 Refactoring Editor System Class Diagram

* Docs: #9 Update RS including Refactoring Editor Structure
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCEBB73-4B11-4188-8C58-23ECF942686E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE277A06-2E49-4A5C-9E51-A513D772ABED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="0" windowWidth="20445" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="103">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,10 +55,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>씬 관련</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>S</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -107,10 +103,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공지 메시지 = 시스템 메시지 출력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -127,10 +119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Scene</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>N</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -143,10 +131,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>`</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Animation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -175,14 +159,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FR-C-T-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FR-C-T-02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FR-C-01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -197,6 +173,255 @@
   <si>
     <t>마우스 이벤트 메니저에 이벤트 전달</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Editor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에디터 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 에디터 기능등</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-01.03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마우스 이벤트 할당</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 불러오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-N-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-N-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI 관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-01.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 컨텐츠 프리펩 광역 컨포넌트에 전달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-01.02</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.03</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.04</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.05</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.06</t>
+  </si>
+  <si>
+    <t>FR-U-M-01.07</t>
+  </si>
+  <si>
+    <t>모달 초기화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 초기값 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 타입 관련 컴포넌트 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 컨텐츠 적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모달 취소 / 확인 버튼 이벤트 적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 텍스트 모달 인터페이스 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-03</t>
+  </si>
+  <si>
+    <t>일반 텍스트 인풋 모달 인터페이스 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시스템</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFR-S-E-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 에디터 시스템 구조 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 메뉴 버튼 기능 : 새로 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 메뉴 버튼 기능 : 불러오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 메뉴 버튼 기능 : 종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에디터용 인터페이스 함수 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-02.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-S-02.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>json 데이터 불러오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>json 데이터 저장하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-S-02.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFR-S-E-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 및 폴더 구조 정립</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에디터 토글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 내보내기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-02.02</t>
+  </si>
+  <si>
+    <t>FR-C-E-02.03</t>
+  </si>
+  <si>
+    <t>FR-C-E-02.04</t>
+  </si>
+  <si>
+    <t>FR-C-E-02.05</t>
+  </si>
+  <si>
+    <t>FR-C-E-03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지도 에디터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-03.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-C-E-03.02</t>
+  </si>
+  <si>
+    <t>FR-C-E-03.03</t>
+  </si>
+  <si>
+    <t>FR-C-E-03.04</t>
+  </si>
+  <si>
+    <t>FR-C-E-03.05</t>
   </si>
 </sst>
 </file>
@@ -245,7 +470,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -275,26 +500,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -310,16 +515,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -600,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:T65"/>
+  <dimension ref="B2:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="U40" sqref="U40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -615,7 +818,7 @@
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
@@ -624,7 +827,7 @@
       </c>
       <c r="S4" s="1"/>
       <c r="T4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
@@ -635,26 +838,26 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
         <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
@@ -665,22 +868,53 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
@@ -689,37 +923,37 @@
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7" t="s">
+      <c r="I12" s="6"/>
+      <c r="J12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="T12" s="7"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="T12" s="5"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
@@ -727,17 +961,17 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="3"/>
       <c r="H13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -757,9 +991,13 @@
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="4"/>
+      <c r="J14" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
@@ -768,7 +1006,7 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="4"/>
+      <c r="S14" s="1"/>
       <c r="T14" s="4"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
@@ -778,9 +1016,13 @@
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="4"/>
+      <c r="J15" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
@@ -789,7 +1031,7 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="3"/>
-      <c r="S15" s="4"/>
+      <c r="S15" s="1"/>
       <c r="T15" s="4"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
@@ -919,41 +1161,41 @@
       <c r="T21" s="4"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -974,11 +1216,11 @@
       <c r="F24" s="4"/>
       <c r="G24" s="3"/>
       <c r="H24" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -1038,11 +1280,17 @@
       <c r="C27" s="3"/>
       <c r="D27" s="4"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="4"/>
+      <c r="H27" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="I27" s="3"/>
-      <c r="J27" s="4"/>
+      <c r="J27" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -1051,7 +1299,7 @@
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="3"/>
-      <c r="S27" s="4"/>
+      <c r="S27" s="1"/>
       <c r="T27" s="4"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.3">
@@ -1059,16 +1307,14 @@
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="F28" s="4"/>
       <c r="G28" s="3"/>
       <c r="H28" s="4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="4" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -1089,11 +1335,11 @@
       <c r="F29" s="4"/>
       <c r="G29" s="3"/>
       <c r="H29" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="4" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -1113,9 +1359,13 @@
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="4"/>
+      <c r="H30" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
@@ -1124,7 +1374,7 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="3"/>
-      <c r="S30" s="4"/>
+      <c r="S30" s="1"/>
       <c r="T30" s="4"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.3">
@@ -1134,9 +1384,13 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="4"/>
+      <c r="H31" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="I31" s="3"/>
-      <c r="J31" s="4"/>
+      <c r="J31" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
@@ -1145,7 +1399,7 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="4"/>
+      <c r="S31" s="1"/>
       <c r="T31" s="4"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
@@ -1155,9 +1409,13 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="4"/>
+      <c r="H32" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="I32" s="3"/>
-      <c r="J32" s="4"/>
+      <c r="J32" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
@@ -1166,7 +1424,7 @@
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="3"/>
-      <c r="S32" s="4"/>
+      <c r="S32" s="1"/>
       <c r="T32" s="4"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.3">
@@ -1176,9 +1434,13 @@
       <c r="E33" s="3"/>
       <c r="F33" s="4"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="4"/>
+      <c r="H33" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="I33" s="3"/>
-      <c r="J33" s="4"/>
+      <c r="J33" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -1187,7 +1449,7 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="3"/>
-      <c r="S33" s="4"/>
+      <c r="S33" s="1"/>
       <c r="T33" s="4"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.3">
@@ -1197,20 +1459,22 @@
       <c r="E34" s="3"/>
       <c r="F34" s="4"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="4"/>
+      <c r="H34" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="I34" s="3"/>
-      <c r="J34" s="4"/>
+      <c r="J34" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
-      <c r="P34" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="3"/>
-      <c r="S34" s="4"/>
+      <c r="S34" s="1"/>
       <c r="T34" s="4"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.3">
@@ -1220,9 +1484,13 @@
       <c r="E35" s="3"/>
       <c r="F35" s="4"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="4"/>
+      <c r="H35" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="I35" s="3"/>
-      <c r="J35" s="4"/>
+      <c r="J35" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -1231,45 +1499,47 @@
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="3"/>
-      <c r="S35" s="4"/>
+      <c r="S35" s="1"/>
       <c r="T35" s="4"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B36" s="5"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="4"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="F37" s="4"/>
       <c r="G37" s="3"/>
       <c r="H37" s="4" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="4" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -1279,7 +1549,7 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="3"/>
-      <c r="S37" s="1"/>
+      <c r="S37" s="2"/>
       <c r="T37" s="4"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.3">
@@ -1290,11 +1560,11 @@
       <c r="F38" s="4"/>
       <c r="G38" s="3"/>
       <c r="H38" s="4" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="4" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
@@ -1304,7 +1574,7 @@
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
       <c r="R38" s="3"/>
-      <c r="S38" s="1"/>
+      <c r="S38" s="2"/>
       <c r="T38" s="4"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.3">
@@ -1314,9 +1584,13 @@
       <c r="E39" s="3"/>
       <c r="F39" s="4"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="4"/>
+      <c r="H39" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="I39" s="3"/>
-      <c r="J39" s="4"/>
+      <c r="J39" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -1325,7 +1599,7 @@
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
       <c r="R39" s="3"/>
-      <c r="S39" s="4"/>
+      <c r="S39" s="2"/>
       <c r="T39" s="4"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.3">
@@ -1335,9 +1609,13 @@
       <c r="E40" s="3"/>
       <c r="F40" s="4"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="4"/>
+      <c r="H40" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="I40" s="3"/>
-      <c r="J40" s="4"/>
+      <c r="J40" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -1346,7 +1624,7 @@
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
       <c r="R40" s="3"/>
-      <c r="S40" s="4"/>
+      <c r="S40" s="2"/>
       <c r="T40" s="4"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.3">
@@ -1356,9 +1634,13 @@
       <c r="E41" s="3"/>
       <c r="F41" s="4"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="4"/>
+      <c r="H41" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="I41" s="3"/>
-      <c r="J41" s="4"/>
+      <c r="J41" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -1367,7 +1649,7 @@
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
       <c r="R41" s="3"/>
-      <c r="S41" s="4"/>
+      <c r="S41" s="2"/>
       <c r="T41" s="4"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.3">
@@ -1377,9 +1659,13 @@
       <c r="E42" s="3"/>
       <c r="F42" s="4"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="4"/>
+      <c r="H42" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="I42" s="3"/>
-      <c r="J42" s="4"/>
+      <c r="J42" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
@@ -1388,7 +1674,7 @@
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="3"/>
-      <c r="S42" s="4"/>
+      <c r="S42" s="2"/>
       <c r="T42" s="4"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.3">
@@ -1564,11 +1850,17 @@
       <c r="C51" s="3"/>
       <c r="D51" s="4"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="4"/>
+      <c r="F51" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="G51" s="3"/>
-      <c r="H51" s="4"/>
+      <c r="H51" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="I51" s="3"/>
-      <c r="J51" s="4"/>
+      <c r="J51" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
@@ -1577,7 +1869,7 @@
       <c r="P51" s="4"/>
       <c r="Q51" s="4"/>
       <c r="R51" s="3"/>
-      <c r="S51" s="4"/>
+      <c r="S51" s="1"/>
       <c r="T51" s="4"/>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.3">
@@ -1587,9 +1879,13 @@
       <c r="E52" s="3"/>
       <c r="F52" s="4"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="4"/>
+      <c r="H52" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="I52" s="3"/>
-      <c r="J52" s="4"/>
+      <c r="J52" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
@@ -1598,7 +1894,7 @@
       <c r="P52" s="4"/>
       <c r="Q52" s="4"/>
       <c r="R52" s="3"/>
-      <c r="S52" s="4"/>
+      <c r="S52" s="1"/>
       <c r="T52" s="4"/>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.3">
@@ -1690,11 +1986,17 @@
       <c r="C57" s="3"/>
       <c r="D57" s="4"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="4"/>
+      <c r="F57" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="G57" s="3"/>
-      <c r="H57" s="4"/>
+      <c r="H57" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="I57" s="3"/>
-      <c r="J57" s="4"/>
+      <c r="J57" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
@@ -1703,7 +2005,7 @@
       <c r="P57" s="4"/>
       <c r="Q57" s="4"/>
       <c r="R57" s="3"/>
-      <c r="S57" s="4"/>
+      <c r="S57" s="1"/>
       <c r="T57" s="4"/>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.3">
@@ -1713,9 +2015,13 @@
       <c r="E58" s="3"/>
       <c r="F58" s="4"/>
       <c r="G58" s="3"/>
-      <c r="H58" s="4"/>
+      <c r="H58" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="I58" s="3"/>
-      <c r="J58" s="4"/>
+      <c r="J58" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
@@ -1724,7 +2030,7 @@
       <c r="P58" s="4"/>
       <c r="Q58" s="4"/>
       <c r="R58" s="3"/>
-      <c r="S58" s="4"/>
+      <c r="S58" s="1"/>
       <c r="T58" s="4"/>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.3">
@@ -1874,6 +2180,3445 @@
       <c r="S65" s="4"/>
       <c r="T65" s="4"/>
     </row>
+    <row r="66" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B66" s="4"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="4"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="4"/>
+      <c r="Q66" s="4"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="4"/>
+      <c r="T66" s="4"/>
+    </row>
+    <row r="67" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B67" s="4"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
+      <c r="P67" s="4"/>
+      <c r="Q67" s="4"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="4"/>
+    </row>
+    <row r="68" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B68" s="4"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="4"/>
+      <c r="Q68" s="4"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="4"/>
+      <c r="T68" s="4"/>
+    </row>
+    <row r="69" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B69" s="4"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
+      <c r="P69" s="4"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="4"/>
+      <c r="T69" s="4"/>
+    </row>
+    <row r="70" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B70" s="4"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="4"/>
+      <c r="Q70" s="4"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="4"/>
+      <c r="T70" s="4"/>
+    </row>
+    <row r="71" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B71" s="4"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
+      <c r="P71" s="4"/>
+      <c r="Q71" s="4"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="4"/>
+      <c r="T71" s="4"/>
+    </row>
+    <row r="72" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B72" s="4"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
+      <c r="P72" s="4"/>
+      <c r="Q72" s="4"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="4"/>
+      <c r="T72" s="4"/>
+    </row>
+    <row r="73" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B73" s="4"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4"/>
+      <c r="P73" s="4"/>
+      <c r="Q73" s="4"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="4"/>
+      <c r="T73" s="4"/>
+    </row>
+    <row r="74" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B74" s="4"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E74" s="3"/>
+      <c r="F74" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G74" s="3"/>
+      <c r="H74" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I74" s="3"/>
+      <c r="J74" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
+      <c r="P74" s="4"/>
+      <c r="Q74" s="4"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="4"/>
+    </row>
+    <row r="75" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B75" s="4"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I75" s="3"/>
+      <c r="J75" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
+      <c r="P75" s="4"/>
+      <c r="Q75" s="4"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="4"/>
+    </row>
+    <row r="76" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B76" s="4"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I76" s="3"/>
+      <c r="J76" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K76" s="4"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="4"/>
+      <c r="O76" s="4"/>
+      <c r="P76" s="4"/>
+      <c r="Q76" s="4"/>
+      <c r="R76" s="3"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="4"/>
+    </row>
+    <row r="77" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B77" s="4"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I77" s="3"/>
+      <c r="J77" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="3"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="4"/>
+    </row>
+    <row r="78" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B78" s="4"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="J78" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K78" s="4"/>
+      <c r="L78" s="4"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="4"/>
+      <c r="Q78" s="4"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="4"/>
+    </row>
+    <row r="79" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B79" s="4"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I79" s="3"/>
+      <c r="J79" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="4"/>
+      <c r="N79" s="4"/>
+      <c r="O79" s="4"/>
+      <c r="P79" s="4"/>
+      <c r="Q79" s="4"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="4"/>
+    </row>
+    <row r="80" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B80" s="4"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I80" s="3"/>
+      <c r="J80" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="3"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="4"/>
+    </row>
+    <row r="81" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B81" s="4"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I81" s="3"/>
+      <c r="J81" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="4"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="4"/>
+    </row>
+    <row r="82" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B82" s="4"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I82" s="3"/>
+      <c r="J82" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K82" s="4"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="4"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="4"/>
+      <c r="Q82" s="4"/>
+      <c r="R82" s="3"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="4"/>
+    </row>
+    <row r="83" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B83" s="4"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I83" s="3"/>
+      <c r="J83" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K83" s="4"/>
+      <c r="L83" s="4"/>
+      <c r="M83" s="4"/>
+      <c r="N83" s="4"/>
+      <c r="O83" s="4"/>
+      <c r="P83" s="4"/>
+      <c r="Q83" s="4"/>
+      <c r="R83" s="3"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="4"/>
+    </row>
+    <row r="84" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B84" s="4"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="3"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="4"/>
+      <c r="Q84" s="4"/>
+      <c r="R84" s="3"/>
+      <c r="S84" s="4"/>
+      <c r="T84" s="4"/>
+    </row>
+    <row r="85" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B85" s="4"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="4"/>
+      <c r="L85" s="4"/>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="4"/>
+      <c r="P85" s="4"/>
+      <c r="Q85" s="4"/>
+      <c r="R85" s="3"/>
+      <c r="S85" s="4"/>
+      <c r="T85" s="4"/>
+    </row>
+    <row r="86" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B86" s="4"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="4"/>
+      <c r="Q86" s="4"/>
+      <c r="R86" s="3"/>
+      <c r="S86" s="4"/>
+      <c r="T86" s="4"/>
+    </row>
+    <row r="87" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B87" s="4"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="3"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
+      <c r="L87" s="4"/>
+      <c r="M87" s="4"/>
+      <c r="N87" s="4"/>
+      <c r="O87" s="4"/>
+      <c r="P87" s="4"/>
+      <c r="Q87" s="4"/>
+      <c r="R87" s="3"/>
+      <c r="S87" s="4"/>
+      <c r="T87" s="4"/>
+    </row>
+    <row r="88" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B88" s="4"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="4"/>
+      <c r="Q88" s="4"/>
+      <c r="R88" s="3"/>
+      <c r="S88" s="4"/>
+      <c r="T88" s="4"/>
+    </row>
+    <row r="89" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B89" s="4"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="4"/>
+      <c r="O89" s="4"/>
+      <c r="P89" s="4"/>
+      <c r="Q89" s="4"/>
+      <c r="R89" s="3"/>
+      <c r="S89" s="4"/>
+      <c r="T89" s="4"/>
+    </row>
+    <row r="90" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B90" s="4"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+      <c r="M90" s="4"/>
+      <c r="N90" s="4"/>
+      <c r="O90" s="4"/>
+      <c r="P90" s="4"/>
+      <c r="Q90" s="4"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="4"/>
+      <c r="T90" s="4"/>
+    </row>
+    <row r="91" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B91" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="3"/>
+      <c r="D91" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E91" s="3"/>
+      <c r="F91" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G91" s="3"/>
+      <c r="H91" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I91" s="3"/>
+      <c r="J91" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K91" s="4"/>
+      <c r="L91" s="4"/>
+      <c r="M91" s="4"/>
+      <c r="N91" s="4"/>
+      <c r="O91" s="4"/>
+      <c r="P91" s="4"/>
+      <c r="Q91" s="4"/>
+      <c r="R91" s="3"/>
+      <c r="S91" s="1"/>
+      <c r="T91" s="4"/>
+    </row>
+    <row r="92" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B92" s="4"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I92" s="3"/>
+      <c r="J92" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="4"/>
+      <c r="O92" s="4"/>
+      <c r="P92" s="4"/>
+      <c r="Q92" s="4"/>
+      <c r="R92" s="3"/>
+      <c r="S92" s="1"/>
+      <c r="T92" s="4"/>
+    </row>
+    <row r="93" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B93" s="4"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
+      <c r="L93" s="4"/>
+      <c r="M93" s="4"/>
+      <c r="N93" s="4"/>
+      <c r="O93" s="4"/>
+      <c r="P93" s="4"/>
+      <c r="Q93" s="4"/>
+      <c r="R93" s="3"/>
+      <c r="S93" s="4"/>
+      <c r="T93" s="4"/>
+    </row>
+    <row r="94" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B94" s="4"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="3"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
+      <c r="L94" s="4"/>
+      <c r="M94" s="4"/>
+      <c r="N94" s="4"/>
+      <c r="O94" s="4"/>
+      <c r="P94" s="4"/>
+      <c r="Q94" s="4"/>
+      <c r="R94" s="3"/>
+      <c r="S94" s="4"/>
+      <c r="T94" s="4"/>
+    </row>
+    <row r="95" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B95" s="4"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="4"/>
+      <c r="M95" s="4"/>
+      <c r="N95" s="4"/>
+      <c r="O95" s="4"/>
+      <c r="P95" s="4"/>
+      <c r="Q95" s="4"/>
+      <c r="R95" s="3"/>
+      <c r="S95" s="4"/>
+      <c r="T95" s="4"/>
+    </row>
+    <row r="96" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B96" s="4"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="3"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="4"/>
+      <c r="L96" s="4"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="4"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="4"/>
+      <c r="Q96" s="4"/>
+      <c r="R96" s="3"/>
+      <c r="S96" s="4"/>
+      <c r="T96" s="4"/>
+    </row>
+    <row r="97" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B97" s="4"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="3"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="4"/>
+      <c r="L97" s="4"/>
+      <c r="M97" s="4"/>
+      <c r="N97" s="4"/>
+      <c r="O97" s="4"/>
+      <c r="P97" s="4"/>
+      <c r="Q97" s="4"/>
+      <c r="R97" s="3"/>
+      <c r="S97" s="4"/>
+      <c r="T97" s="4"/>
+    </row>
+    <row r="98" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B98" s="4"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="3"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
+      <c r="L98" s="4"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="4"/>
+      <c r="O98" s="4"/>
+      <c r="P98" s="4"/>
+      <c r="Q98" s="4"/>
+      <c r="R98" s="3"/>
+      <c r="S98" s="4"/>
+      <c r="T98" s="4"/>
+    </row>
+    <row r="99" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B99" s="4"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="3"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="4"/>
+      <c r="L99" s="4"/>
+      <c r="M99" s="4"/>
+      <c r="N99" s="4"/>
+      <c r="O99" s="4"/>
+      <c r="P99" s="4"/>
+      <c r="Q99" s="4"/>
+      <c r="R99" s="3"/>
+      <c r="S99" s="4"/>
+      <c r="T99" s="4"/>
+    </row>
+    <row r="100" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B100" s="4"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="3"/>
+      <c r="J100" s="4"/>
+      <c r="K100" s="4"/>
+      <c r="L100" s="4"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="4"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="4"/>
+      <c r="Q100" s="4"/>
+      <c r="R100" s="3"/>
+      <c r="S100" s="4"/>
+      <c r="T100" s="4"/>
+    </row>
+    <row r="101" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B101" s="4"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="4"/>
+      <c r="K101" s="4"/>
+      <c r="L101" s="4"/>
+      <c r="M101" s="4"/>
+      <c r="N101" s="4"/>
+      <c r="O101" s="4"/>
+      <c r="P101" s="4"/>
+      <c r="Q101" s="4"/>
+      <c r="R101" s="3"/>
+      <c r="S101" s="4"/>
+      <c r="T101" s="4"/>
+    </row>
+    <row r="102" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B102" s="4"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="3"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="4"/>
+      <c r="L102" s="4"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="4"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="4"/>
+      <c r="Q102" s="4"/>
+      <c r="R102" s="3"/>
+      <c r="S102" s="4"/>
+      <c r="T102" s="4"/>
+    </row>
+    <row r="103" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B103" s="4"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="3"/>
+      <c r="J103" s="4"/>
+      <c r="K103" s="4"/>
+      <c r="L103" s="4"/>
+      <c r="M103" s="4"/>
+      <c r="N103" s="4"/>
+      <c r="O103" s="4"/>
+      <c r="P103" s="4"/>
+      <c r="Q103" s="4"/>
+      <c r="R103" s="3"/>
+      <c r="S103" s="4"/>
+      <c r="T103" s="4"/>
+    </row>
+    <row r="104" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B104" s="4"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="3"/>
+      <c r="J104" s="4"/>
+      <c r="K104" s="4"/>
+      <c r="L104" s="4"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="4"/>
+      <c r="O104" s="4"/>
+      <c r="P104" s="4"/>
+      <c r="Q104" s="4"/>
+      <c r="R104" s="3"/>
+      <c r="S104" s="4"/>
+      <c r="T104" s="4"/>
+    </row>
+    <row r="105" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B105" s="4"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="3"/>
+      <c r="J105" s="4"/>
+      <c r="K105" s="4"/>
+      <c r="L105" s="4"/>
+      <c r="M105" s="4"/>
+      <c r="N105" s="4"/>
+      <c r="O105" s="4"/>
+      <c r="P105" s="4"/>
+      <c r="Q105" s="4"/>
+      <c r="R105" s="3"/>
+      <c r="S105" s="4"/>
+      <c r="T105" s="4"/>
+    </row>
+    <row r="106" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B106" s="4"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="3"/>
+      <c r="J106" s="4"/>
+      <c r="K106" s="4"/>
+      <c r="L106" s="4"/>
+      <c r="M106" s="4"/>
+      <c r="N106" s="4"/>
+      <c r="O106" s="4"/>
+      <c r="P106" s="4"/>
+      <c r="Q106" s="4"/>
+      <c r="R106" s="3"/>
+      <c r="S106" s="4"/>
+      <c r="T106" s="4"/>
+    </row>
+    <row r="107" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B107" s="4"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="3"/>
+      <c r="J107" s="4"/>
+      <c r="K107" s="4"/>
+      <c r="L107" s="4"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="O107" s="4"/>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="4"/>
+      <c r="R107" s="3"/>
+      <c r="S107" s="4"/>
+      <c r="T107" s="4"/>
+    </row>
+    <row r="108" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B108" s="4"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="4"/>
+      <c r="K108" s="4"/>
+      <c r="L108" s="4"/>
+      <c r="M108" s="4"/>
+      <c r="N108" s="4"/>
+      <c r="O108" s="4"/>
+      <c r="P108" s="4"/>
+      <c r="Q108" s="4"/>
+      <c r="R108" s="3"/>
+      <c r="S108" s="4"/>
+      <c r="T108" s="4"/>
+    </row>
+    <row r="109" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B109" s="4"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="3"/>
+      <c r="J109" s="4"/>
+      <c r="K109" s="4"/>
+      <c r="L109" s="4"/>
+      <c r="M109" s="4"/>
+      <c r="N109" s="4"/>
+      <c r="O109" s="4"/>
+      <c r="P109" s="4"/>
+      <c r="Q109" s="4"/>
+      <c r="R109" s="3"/>
+      <c r="S109" s="4"/>
+      <c r="T109" s="4"/>
+    </row>
+    <row r="110" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B110" s="4"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="3"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="3"/>
+      <c r="J110" s="4"/>
+      <c r="K110" s="4"/>
+      <c r="L110" s="4"/>
+      <c r="M110" s="4"/>
+      <c r="N110" s="4"/>
+      <c r="O110" s="4"/>
+      <c r="P110" s="4"/>
+      <c r="Q110" s="4"/>
+      <c r="R110" s="3"/>
+      <c r="S110" s="4"/>
+      <c r="T110" s="4"/>
+    </row>
+    <row r="111" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B111" s="4"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="3"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="3"/>
+      <c r="J111" s="4"/>
+      <c r="K111" s="4"/>
+      <c r="L111" s="4"/>
+      <c r="M111" s="4"/>
+      <c r="N111" s="4"/>
+      <c r="O111" s="4"/>
+      <c r="P111" s="4"/>
+      <c r="Q111" s="4"/>
+      <c r="R111" s="3"/>
+      <c r="S111" s="4"/>
+      <c r="T111" s="4"/>
+    </row>
+    <row r="112" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B112" s="4"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="3"/>
+      <c r="J112" s="4"/>
+      <c r="K112" s="4"/>
+      <c r="L112" s="4"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="4"/>
+      <c r="O112" s="4"/>
+      <c r="P112" s="4"/>
+      <c r="Q112" s="4"/>
+      <c r="R112" s="3"/>
+      <c r="S112" s="4"/>
+      <c r="T112" s="4"/>
+    </row>
+    <row r="113" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B113" s="4"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="4"/>
+      <c r="I113" s="3"/>
+      <c r="J113" s="4"/>
+      <c r="K113" s="4"/>
+      <c r="L113" s="4"/>
+      <c r="M113" s="4"/>
+      <c r="N113" s="4"/>
+      <c r="O113" s="4"/>
+      <c r="P113" s="4"/>
+      <c r="Q113" s="4"/>
+      <c r="R113" s="3"/>
+      <c r="S113" s="4"/>
+      <c r="T113" s="4"/>
+    </row>
+    <row r="114" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B114" s="4"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="3"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="3"/>
+      <c r="J114" s="4"/>
+      <c r="K114" s="4"/>
+      <c r="L114" s="4"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="4"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="4"/>
+      <c r="Q114" s="4"/>
+      <c r="R114" s="3"/>
+      <c r="S114" s="4"/>
+      <c r="T114" s="4"/>
+    </row>
+    <row r="115" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B115" s="4"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="3"/>
+      <c r="H115" s="4"/>
+      <c r="I115" s="3"/>
+      <c r="J115" s="4"/>
+      <c r="K115" s="4"/>
+      <c r="L115" s="4"/>
+      <c r="M115" s="4"/>
+      <c r="N115" s="4"/>
+      <c r="O115" s="4"/>
+      <c r="P115" s="4"/>
+      <c r="Q115" s="4"/>
+      <c r="R115" s="3"/>
+      <c r="S115" s="4"/>
+      <c r="T115" s="4"/>
+    </row>
+    <row r="116" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B116" s="4"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="3"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="3"/>
+      <c r="J116" s="4"/>
+      <c r="K116" s="4"/>
+      <c r="L116" s="4"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="4"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="4"/>
+      <c r="Q116" s="4"/>
+      <c r="R116" s="3"/>
+      <c r="S116" s="4"/>
+      <c r="T116" s="4"/>
+    </row>
+    <row r="117" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B117" s="4"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="3"/>
+      <c r="H117" s="4"/>
+      <c r="I117" s="3"/>
+      <c r="J117" s="4"/>
+      <c r="K117" s="4"/>
+      <c r="L117" s="4"/>
+      <c r="M117" s="4"/>
+      <c r="N117" s="4"/>
+      <c r="O117" s="4"/>
+      <c r="P117" s="4"/>
+      <c r="Q117" s="4"/>
+      <c r="R117" s="3"/>
+      <c r="S117" s="4"/>
+      <c r="T117" s="4"/>
+    </row>
+    <row r="118" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B118" s="4"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="3"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="3"/>
+      <c r="J118" s="4"/>
+      <c r="K118" s="4"/>
+      <c r="L118" s="4"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="4"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="4"/>
+      <c r="Q118" s="4"/>
+      <c r="R118" s="3"/>
+      <c r="S118" s="4"/>
+      <c r="T118" s="4"/>
+    </row>
+    <row r="119" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B119" s="4"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="3"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="3"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="3"/>
+      <c r="J119" s="4"/>
+      <c r="K119" s="4"/>
+      <c r="L119" s="4"/>
+      <c r="M119" s="4"/>
+      <c r="N119" s="4"/>
+      <c r="O119" s="4"/>
+      <c r="P119" s="4"/>
+      <c r="Q119" s="4"/>
+      <c r="R119" s="3"/>
+      <c r="S119" s="4"/>
+      <c r="T119" s="4"/>
+    </row>
+    <row r="120" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B120" s="4"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="3"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="3"/>
+      <c r="J120" s="4"/>
+      <c r="K120" s="4"/>
+      <c r="L120" s="4"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="4"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="4"/>
+      <c r="Q120" s="4"/>
+      <c r="R120" s="3"/>
+      <c r="S120" s="4"/>
+      <c r="T120" s="4"/>
+    </row>
+    <row r="121" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B121" s="4"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="3"/>
+      <c r="H121" s="4"/>
+      <c r="I121" s="3"/>
+      <c r="J121" s="4"/>
+      <c r="K121" s="4"/>
+      <c r="L121" s="4"/>
+      <c r="M121" s="4"/>
+      <c r="N121" s="4"/>
+      <c r="O121" s="4"/>
+      <c r="P121" s="4"/>
+      <c r="Q121" s="4"/>
+      <c r="R121" s="3"/>
+      <c r="S121" s="4"/>
+      <c r="T121" s="4"/>
+    </row>
+    <row r="122" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B122" s="4"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="3"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="3"/>
+      <c r="J122" s="4"/>
+      <c r="K122" s="4"/>
+      <c r="L122" s="4"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="4"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="4"/>
+      <c r="Q122" s="4"/>
+      <c r="R122" s="3"/>
+      <c r="S122" s="4"/>
+      <c r="T122" s="4"/>
+    </row>
+    <row r="123" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B123" s="4"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="3"/>
+      <c r="H123" s="4"/>
+      <c r="I123" s="3"/>
+      <c r="J123" s="4"/>
+      <c r="K123" s="4"/>
+      <c r="L123" s="4"/>
+      <c r="M123" s="4"/>
+      <c r="N123" s="4"/>
+      <c r="O123" s="4"/>
+      <c r="P123" s="4"/>
+      <c r="Q123" s="4"/>
+      <c r="R123" s="3"/>
+      <c r="S123" s="4"/>
+      <c r="T123" s="4"/>
+    </row>
+    <row r="124" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B124" s="4"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="3"/>
+      <c r="H124" s="4"/>
+      <c r="I124" s="3"/>
+      <c r="J124" s="4"/>
+      <c r="K124" s="4"/>
+      <c r="L124" s="4"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="4"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="4"/>
+      <c r="Q124" s="4"/>
+      <c r="R124" s="3"/>
+      <c r="S124" s="4"/>
+      <c r="T124" s="4"/>
+    </row>
+    <row r="125" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B125" s="4"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="3"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="3"/>
+      <c r="H125" s="4"/>
+      <c r="I125" s="3"/>
+      <c r="J125" s="4"/>
+      <c r="K125" s="4"/>
+      <c r="L125" s="4"/>
+      <c r="M125" s="4"/>
+      <c r="N125" s="4"/>
+      <c r="O125" s="4"/>
+      <c r="P125" s="4"/>
+      <c r="Q125" s="4"/>
+      <c r="R125" s="3"/>
+      <c r="S125" s="4"/>
+      <c r="T125" s="4"/>
+    </row>
+    <row r="126" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B126" s="4"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="3"/>
+      <c r="H126" s="4"/>
+      <c r="I126" s="3"/>
+      <c r="J126" s="4"/>
+      <c r="K126" s="4"/>
+      <c r="L126" s="4"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="4"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="4"/>
+      <c r="Q126" s="4"/>
+      <c r="R126" s="3"/>
+      <c r="S126" s="4"/>
+      <c r="T126" s="4"/>
+    </row>
+    <row r="127" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B127" s="4"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="3"/>
+      <c r="F127" s="4"/>
+      <c r="G127" s="3"/>
+      <c r="H127" s="4"/>
+      <c r="I127" s="3"/>
+      <c r="J127" s="4"/>
+      <c r="K127" s="4"/>
+      <c r="L127" s="4"/>
+      <c r="M127" s="4"/>
+      <c r="N127" s="4"/>
+      <c r="O127" s="4"/>
+      <c r="P127" s="4"/>
+      <c r="Q127" s="4"/>
+      <c r="R127" s="3"/>
+      <c r="S127" s="4"/>
+      <c r="T127" s="4"/>
+    </row>
+    <row r="128" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B128" s="4"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="3"/>
+      <c r="H128" s="4"/>
+      <c r="I128" s="3"/>
+      <c r="J128" s="4"/>
+      <c r="K128" s="4"/>
+      <c r="L128" s="4"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="4"/>
+      <c r="O128" s="4"/>
+      <c r="P128" s="4"/>
+      <c r="Q128" s="4"/>
+      <c r="R128" s="3"/>
+      <c r="S128" s="4"/>
+      <c r="T128" s="4"/>
+    </row>
+    <row r="129" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B129" s="4"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="4"/>
+      <c r="G129" s="3"/>
+      <c r="H129" s="4"/>
+      <c r="I129" s="3"/>
+      <c r="J129" s="4"/>
+      <c r="K129" s="4"/>
+      <c r="L129" s="4"/>
+      <c r="M129" s="4"/>
+      <c r="N129" s="4"/>
+      <c r="O129" s="4"/>
+      <c r="P129" s="4"/>
+      <c r="Q129" s="4"/>
+      <c r="R129" s="3"/>
+      <c r="S129" s="4"/>
+      <c r="T129" s="4"/>
+    </row>
+    <row r="130" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B130" s="4"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="4"/>
+      <c r="G130" s="3"/>
+      <c r="H130" s="4"/>
+      <c r="I130" s="3"/>
+      <c r="J130" s="4"/>
+      <c r="K130" s="4"/>
+      <c r="L130" s="4"/>
+      <c r="M130" s="4"/>
+      <c r="N130" s="4"/>
+      <c r="O130" s="4"/>
+      <c r="P130" s="4"/>
+      <c r="Q130" s="4"/>
+      <c r="R130" s="3"/>
+      <c r="S130" s="4"/>
+      <c r="T130" s="4"/>
+    </row>
+    <row r="131" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B131" s="4"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="4"/>
+      <c r="G131" s="3"/>
+      <c r="H131" s="4"/>
+      <c r="I131" s="3"/>
+      <c r="J131" s="4"/>
+      <c r="K131" s="4"/>
+      <c r="L131" s="4"/>
+      <c r="M131" s="4"/>
+      <c r="N131" s="4"/>
+      <c r="O131" s="4"/>
+      <c r="P131" s="4"/>
+      <c r="Q131" s="4"/>
+      <c r="R131" s="3"/>
+      <c r="S131" s="4"/>
+      <c r="T131" s="4"/>
+    </row>
+    <row r="132" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B132" s="4"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="3"/>
+      <c r="H132" s="4"/>
+      <c r="I132" s="3"/>
+      <c r="J132" s="4"/>
+      <c r="K132" s="4"/>
+      <c r="L132" s="4"/>
+      <c r="M132" s="4"/>
+      <c r="N132" s="4"/>
+      <c r="O132" s="4"/>
+      <c r="P132" s="4"/>
+      <c r="Q132" s="4"/>
+      <c r="R132" s="3"/>
+      <c r="S132" s="4"/>
+      <c r="T132" s="4"/>
+    </row>
+    <row r="133" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B133" s="4"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="4"/>
+      <c r="E133" s="3"/>
+      <c r="F133" s="4"/>
+      <c r="G133" s="3"/>
+      <c r="H133" s="4"/>
+      <c r="I133" s="3"/>
+      <c r="J133" s="4"/>
+      <c r="K133" s="4"/>
+      <c r="L133" s="4"/>
+      <c r="M133" s="4"/>
+      <c r="N133" s="4"/>
+      <c r="O133" s="4"/>
+      <c r="P133" s="4"/>
+      <c r="Q133" s="4"/>
+      <c r="R133" s="3"/>
+      <c r="S133" s="4"/>
+      <c r="T133" s="4"/>
+    </row>
+    <row r="134" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B134" s="4"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="4"/>
+      <c r="G134" s="3"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="3"/>
+      <c r="J134" s="4"/>
+      <c r="K134" s="4"/>
+      <c r="L134" s="4"/>
+      <c r="M134" s="4"/>
+      <c r="N134" s="4"/>
+      <c r="O134" s="4"/>
+      <c r="P134" s="4"/>
+      <c r="Q134" s="4"/>
+      <c r="R134" s="3"/>
+      <c r="S134" s="4"/>
+      <c r="T134" s="4"/>
+    </row>
+    <row r="135" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B135" s="4"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="3"/>
+      <c r="H135" s="4"/>
+      <c r="I135" s="3"/>
+      <c r="J135" s="4"/>
+      <c r="K135" s="4"/>
+      <c r="L135" s="4"/>
+      <c r="M135" s="4"/>
+      <c r="N135" s="4"/>
+      <c r="O135" s="4"/>
+      <c r="P135" s="4"/>
+      <c r="Q135" s="4"/>
+      <c r="R135" s="3"/>
+      <c r="S135" s="4"/>
+      <c r="T135" s="4"/>
+    </row>
+    <row r="136" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B136" s="4"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="3"/>
+      <c r="H136" s="4"/>
+      <c r="I136" s="3"/>
+      <c r="J136" s="4"/>
+      <c r="K136" s="4"/>
+      <c r="L136" s="4"/>
+      <c r="M136" s="4"/>
+      <c r="N136" s="4"/>
+      <c r="O136" s="4"/>
+      <c r="P136" s="4"/>
+      <c r="Q136" s="4"/>
+      <c r="R136" s="3"/>
+      <c r="S136" s="4"/>
+      <c r="T136" s="4"/>
+    </row>
+    <row r="137" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B137" s="4"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="3"/>
+      <c r="H137" s="4"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="4"/>
+      <c r="K137" s="4"/>
+      <c r="L137" s="4"/>
+      <c r="M137" s="4"/>
+      <c r="N137" s="4"/>
+      <c r="O137" s="4"/>
+      <c r="P137" s="4"/>
+      <c r="Q137" s="4"/>
+      <c r="R137" s="3"/>
+      <c r="S137" s="4"/>
+      <c r="T137" s="4"/>
+    </row>
+    <row r="138" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B138" s="4"/>
+      <c r="C138" s="3"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="4"/>
+      <c r="G138" s="3"/>
+      <c r="H138" s="4"/>
+      <c r="I138" s="3"/>
+      <c r="J138" s="4"/>
+      <c r="K138" s="4"/>
+      <c r="L138" s="4"/>
+      <c r="M138" s="4"/>
+      <c r="N138" s="4"/>
+      <c r="O138" s="4"/>
+      <c r="P138" s="4"/>
+      <c r="Q138" s="4"/>
+      <c r="R138" s="3"/>
+      <c r="S138" s="4"/>
+      <c r="T138" s="4"/>
+    </row>
+    <row r="139" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B139" s="4"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="4"/>
+      <c r="E139" s="3"/>
+      <c r="F139" s="4"/>
+      <c r="G139" s="3"/>
+      <c r="H139" s="4"/>
+      <c r="I139" s="3"/>
+      <c r="J139" s="4"/>
+      <c r="K139" s="4"/>
+      <c r="L139" s="4"/>
+      <c r="M139" s="4"/>
+      <c r="N139" s="4"/>
+      <c r="O139" s="4"/>
+      <c r="P139" s="4"/>
+      <c r="Q139" s="4"/>
+      <c r="R139" s="3"/>
+      <c r="S139" s="4"/>
+      <c r="T139" s="4"/>
+    </row>
+    <row r="140" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B140" s="4"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="4"/>
+      <c r="G140" s="3"/>
+      <c r="H140" s="4"/>
+      <c r="I140" s="3"/>
+      <c r="J140" s="4"/>
+      <c r="K140" s="4"/>
+      <c r="L140" s="4"/>
+      <c r="M140" s="4"/>
+      <c r="N140" s="4"/>
+      <c r="O140" s="4"/>
+      <c r="P140" s="4"/>
+      <c r="Q140" s="4"/>
+      <c r="R140" s="3"/>
+      <c r="S140" s="4"/>
+      <c r="T140" s="4"/>
+    </row>
+    <row r="141" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B141" s="4"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="4"/>
+      <c r="E141" s="3"/>
+      <c r="F141" s="4"/>
+      <c r="G141" s="3"/>
+      <c r="H141" s="4"/>
+      <c r="I141" s="3"/>
+      <c r="J141" s="4"/>
+      <c r="K141" s="4"/>
+      <c r="L141" s="4"/>
+      <c r="M141" s="4"/>
+      <c r="N141" s="4"/>
+      <c r="O141" s="4"/>
+      <c r="P141" s="4"/>
+      <c r="Q141" s="4"/>
+      <c r="R141" s="3"/>
+      <c r="S141" s="4"/>
+      <c r="T141" s="4"/>
+    </row>
+    <row r="142" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B142" s="4"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="4"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="3"/>
+      <c r="H142" s="4"/>
+      <c r="I142" s="3"/>
+      <c r="J142" s="4"/>
+      <c r="K142" s="4"/>
+      <c r="L142" s="4"/>
+      <c r="M142" s="4"/>
+      <c r="N142" s="4"/>
+      <c r="O142" s="4"/>
+      <c r="P142" s="4"/>
+      <c r="Q142" s="4"/>
+      <c r="R142" s="3"/>
+      <c r="S142" s="4"/>
+      <c r="T142" s="4"/>
+    </row>
+    <row r="143" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B143" s="4"/>
+      <c r="C143" s="3"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="3"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="3"/>
+      <c r="H143" s="4"/>
+      <c r="I143" s="3"/>
+      <c r="J143" s="4"/>
+      <c r="K143" s="4"/>
+      <c r="L143" s="4"/>
+      <c r="M143" s="4"/>
+      <c r="N143" s="4"/>
+      <c r="O143" s="4"/>
+      <c r="P143" s="4"/>
+      <c r="Q143" s="4"/>
+      <c r="R143" s="3"/>
+      <c r="S143" s="4"/>
+      <c r="T143" s="4"/>
+    </row>
+    <row r="144" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B144" s="4"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="3"/>
+      <c r="H144" s="4"/>
+      <c r="I144" s="3"/>
+      <c r="J144" s="4"/>
+      <c r="K144" s="4"/>
+      <c r="L144" s="4"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="4"/>
+      <c r="O144" s="4"/>
+      <c r="P144" s="4"/>
+      <c r="Q144" s="4"/>
+      <c r="R144" s="3"/>
+      <c r="S144" s="4"/>
+      <c r="T144" s="4"/>
+    </row>
+    <row r="145" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B145" s="4"/>
+      <c r="C145" s="3"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="3"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="3"/>
+      <c r="H145" s="4"/>
+      <c r="I145" s="3"/>
+      <c r="J145" s="4"/>
+      <c r="K145" s="4"/>
+      <c r="L145" s="4"/>
+      <c r="M145" s="4"/>
+      <c r="N145" s="4"/>
+      <c r="O145" s="4"/>
+      <c r="P145" s="4"/>
+      <c r="Q145" s="4"/>
+      <c r="R145" s="3"/>
+      <c r="S145" s="4"/>
+      <c r="T145" s="4"/>
+    </row>
+    <row r="146" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B146" s="4"/>
+      <c r="C146" s="3"/>
+      <c r="D146" s="4"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="3"/>
+      <c r="H146" s="4"/>
+      <c r="I146" s="3"/>
+      <c r="J146" s="4"/>
+      <c r="K146" s="4"/>
+      <c r="L146" s="4"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="4"/>
+      <c r="O146" s="4"/>
+      <c r="P146" s="4"/>
+      <c r="Q146" s="4"/>
+      <c r="R146" s="3"/>
+      <c r="S146" s="4"/>
+      <c r="T146" s="4"/>
+    </row>
+    <row r="147" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B147" s="4"/>
+      <c r="C147" s="3"/>
+      <c r="D147" s="4"/>
+      <c r="E147" s="3"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="3"/>
+      <c r="H147" s="4"/>
+      <c r="I147" s="3"/>
+      <c r="J147" s="4"/>
+      <c r="K147" s="4"/>
+      <c r="L147" s="4"/>
+      <c r="M147" s="4"/>
+      <c r="N147" s="4"/>
+      <c r="O147" s="4"/>
+      <c r="P147" s="4"/>
+      <c r="Q147" s="4"/>
+      <c r="R147" s="3"/>
+      <c r="S147" s="4"/>
+      <c r="T147" s="4"/>
+    </row>
+    <row r="148" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B148" s="4"/>
+      <c r="C148" s="3"/>
+      <c r="D148" s="4"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="3"/>
+      <c r="H148" s="4"/>
+      <c r="I148" s="3"/>
+      <c r="J148" s="4"/>
+      <c r="K148" s="4"/>
+      <c r="L148" s="4"/>
+      <c r="M148" s="4"/>
+      <c r="N148" s="4"/>
+      <c r="O148" s="4"/>
+      <c r="P148" s="4"/>
+      <c r="Q148" s="4"/>
+      <c r="R148" s="3"/>
+      <c r="S148" s="4"/>
+      <c r="T148" s="4"/>
+    </row>
+    <row r="149" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B149" s="4"/>
+      <c r="C149" s="3"/>
+      <c r="D149" s="4"/>
+      <c r="E149" s="3"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="3"/>
+      <c r="H149" s="4"/>
+      <c r="I149" s="3"/>
+      <c r="J149" s="4"/>
+      <c r="K149" s="4"/>
+      <c r="L149" s="4"/>
+      <c r="M149" s="4"/>
+      <c r="N149" s="4"/>
+      <c r="O149" s="4"/>
+      <c r="P149" s="4"/>
+      <c r="Q149" s="4"/>
+      <c r="R149" s="3"/>
+      <c r="S149" s="4"/>
+      <c r="T149" s="4"/>
+    </row>
+    <row r="150" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B150" s="4"/>
+      <c r="C150" s="3"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="3"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="3"/>
+      <c r="H150" s="4"/>
+      <c r="I150" s="3"/>
+      <c r="J150" s="4"/>
+      <c r="K150" s="4"/>
+      <c r="L150" s="4"/>
+      <c r="M150" s="4"/>
+      <c r="N150" s="4"/>
+      <c r="O150" s="4"/>
+      <c r="P150" s="4"/>
+      <c r="Q150" s="4"/>
+      <c r="R150" s="3"/>
+      <c r="S150" s="4"/>
+      <c r="T150" s="4"/>
+    </row>
+    <row r="151" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B151" s="4"/>
+      <c r="C151" s="3"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="3"/>
+      <c r="F151" s="4"/>
+      <c r="G151" s="3"/>
+      <c r="H151" s="4"/>
+      <c r="I151" s="3"/>
+      <c r="J151" s="4"/>
+      <c r="K151" s="4"/>
+      <c r="L151" s="4"/>
+      <c r="M151" s="4"/>
+      <c r="N151" s="4"/>
+      <c r="O151" s="4"/>
+      <c r="P151" s="4"/>
+      <c r="Q151" s="4"/>
+      <c r="R151" s="3"/>
+      <c r="S151" s="4"/>
+      <c r="T151" s="4"/>
+    </row>
+    <row r="152" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B152" s="4"/>
+      <c r="C152" s="3"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="3"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="3"/>
+      <c r="H152" s="4"/>
+      <c r="I152" s="3"/>
+      <c r="J152" s="4"/>
+      <c r="K152" s="4"/>
+      <c r="L152" s="4"/>
+      <c r="M152" s="4"/>
+      <c r="N152" s="4"/>
+      <c r="O152" s="4"/>
+      <c r="P152" s="4"/>
+      <c r="Q152" s="4"/>
+      <c r="R152" s="3"/>
+      <c r="S152" s="4"/>
+      <c r="T152" s="4"/>
+    </row>
+    <row r="153" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B153" s="4"/>
+      <c r="C153" s="3"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="3"/>
+      <c r="F153" s="4"/>
+      <c r="G153" s="3"/>
+      <c r="H153" s="4"/>
+      <c r="I153" s="3"/>
+      <c r="J153" s="4"/>
+      <c r="K153" s="4"/>
+      <c r="L153" s="4"/>
+      <c r="M153" s="4"/>
+      <c r="N153" s="4"/>
+      <c r="O153" s="4"/>
+      <c r="P153" s="4"/>
+      <c r="Q153" s="4"/>
+      <c r="R153" s="3"/>
+      <c r="S153" s="4"/>
+      <c r="T153" s="4"/>
+    </row>
+    <row r="154" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B154" s="4"/>
+      <c r="C154" s="3"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="3"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="3"/>
+      <c r="H154" s="4"/>
+      <c r="I154" s="3"/>
+      <c r="J154" s="4"/>
+      <c r="K154" s="4"/>
+      <c r="L154" s="4"/>
+      <c r="M154" s="4"/>
+      <c r="N154" s="4"/>
+      <c r="O154" s="4"/>
+      <c r="P154" s="4"/>
+      <c r="Q154" s="4"/>
+      <c r="R154" s="3"/>
+      <c r="S154" s="4"/>
+      <c r="T154" s="4"/>
+    </row>
+    <row r="155" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B155" s="4"/>
+      <c r="C155" s="3"/>
+      <c r="D155" s="4"/>
+      <c r="E155" s="3"/>
+      <c r="F155" s="4"/>
+      <c r="G155" s="3"/>
+      <c r="H155" s="4"/>
+      <c r="I155" s="3"/>
+      <c r="J155" s="4"/>
+      <c r="K155" s="4"/>
+      <c r="L155" s="4"/>
+      <c r="M155" s="4"/>
+      <c r="N155" s="4"/>
+      <c r="O155" s="4"/>
+      <c r="P155" s="4"/>
+      <c r="Q155" s="4"/>
+      <c r="R155" s="3"/>
+      <c r="S155" s="4"/>
+      <c r="T155" s="4"/>
+    </row>
+    <row r="156" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B156" s="4"/>
+      <c r="C156" s="3"/>
+      <c r="D156" s="4"/>
+      <c r="E156" s="3"/>
+      <c r="F156" s="4"/>
+      <c r="G156" s="3"/>
+      <c r="H156" s="4"/>
+      <c r="I156" s="3"/>
+      <c r="J156" s="4"/>
+      <c r="K156" s="4"/>
+      <c r="L156" s="4"/>
+      <c r="M156" s="4"/>
+      <c r="N156" s="4"/>
+      <c r="O156" s="4"/>
+      <c r="P156" s="4"/>
+      <c r="Q156" s="4"/>
+      <c r="R156" s="3"/>
+      <c r="S156" s="4"/>
+      <c r="T156" s="4"/>
+    </row>
+    <row r="157" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B157" s="4"/>
+      <c r="C157" s="3"/>
+      <c r="D157" s="4"/>
+      <c r="E157" s="3"/>
+      <c r="F157" s="4"/>
+      <c r="G157" s="3"/>
+      <c r="H157" s="4"/>
+      <c r="I157" s="3"/>
+      <c r="J157" s="4"/>
+      <c r="K157" s="4"/>
+      <c r="L157" s="4"/>
+      <c r="M157" s="4"/>
+      <c r="N157" s="4"/>
+      <c r="O157" s="4"/>
+      <c r="P157" s="4"/>
+      <c r="Q157" s="4"/>
+      <c r="R157" s="3"/>
+      <c r="S157" s="4"/>
+      <c r="T157" s="4"/>
+    </row>
+    <row r="158" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B158" s="4"/>
+      <c r="C158" s="3"/>
+      <c r="D158" s="4"/>
+      <c r="E158" s="3"/>
+      <c r="F158" s="4"/>
+      <c r="G158" s="3"/>
+      <c r="H158" s="4"/>
+      <c r="I158" s="3"/>
+      <c r="J158" s="4"/>
+      <c r="K158" s="4"/>
+      <c r="L158" s="4"/>
+      <c r="M158" s="4"/>
+      <c r="N158" s="4"/>
+      <c r="O158" s="4"/>
+      <c r="P158" s="4"/>
+      <c r="Q158" s="4"/>
+      <c r="R158" s="3"/>
+      <c r="S158" s="4"/>
+      <c r="T158" s="4"/>
+    </row>
+    <row r="159" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B159" s="4"/>
+      <c r="C159" s="3"/>
+      <c r="D159" s="4"/>
+      <c r="E159" s="3"/>
+      <c r="F159" s="4"/>
+      <c r="G159" s="3"/>
+      <c r="H159" s="4"/>
+      <c r="I159" s="3"/>
+      <c r="J159" s="4"/>
+      <c r="K159" s="4"/>
+      <c r="L159" s="4"/>
+      <c r="M159" s="4"/>
+      <c r="N159" s="4"/>
+      <c r="O159" s="4"/>
+      <c r="P159" s="4"/>
+      <c r="Q159" s="4"/>
+      <c r="R159" s="3"/>
+      <c r="S159" s="4"/>
+      <c r="T159" s="4"/>
+    </row>
+    <row r="160" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B160" s="4"/>
+      <c r="C160" s="3"/>
+      <c r="D160" s="4"/>
+      <c r="E160" s="3"/>
+      <c r="F160" s="4"/>
+      <c r="G160" s="3"/>
+      <c r="H160" s="4"/>
+      <c r="I160" s="3"/>
+      <c r="J160" s="4"/>
+      <c r="K160" s="4"/>
+      <c r="L160" s="4"/>
+      <c r="M160" s="4"/>
+      <c r="N160" s="4"/>
+      <c r="O160" s="4"/>
+      <c r="P160" s="4"/>
+      <c r="Q160" s="4"/>
+      <c r="R160" s="3"/>
+      <c r="S160" s="4"/>
+      <c r="T160" s="4"/>
+    </row>
+    <row r="161" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B161" s="4"/>
+      <c r="C161" s="3"/>
+      <c r="D161" s="4"/>
+      <c r="E161" s="3"/>
+      <c r="F161" s="4"/>
+      <c r="G161" s="3"/>
+      <c r="H161" s="4"/>
+      <c r="I161" s="3"/>
+      <c r="J161" s="4"/>
+      <c r="K161" s="4"/>
+      <c r="L161" s="4"/>
+      <c r="M161" s="4"/>
+      <c r="N161" s="4"/>
+      <c r="O161" s="4"/>
+      <c r="P161" s="4"/>
+      <c r="Q161" s="4"/>
+      <c r="R161" s="3"/>
+      <c r="S161" s="4"/>
+      <c r="T161" s="4"/>
+    </row>
+    <row r="162" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B162" s="4"/>
+      <c r="C162" s="3"/>
+      <c r="D162" s="4"/>
+      <c r="E162" s="3"/>
+      <c r="F162" s="4"/>
+      <c r="G162" s="3"/>
+      <c r="H162" s="4"/>
+      <c r="I162" s="3"/>
+      <c r="J162" s="4"/>
+      <c r="K162" s="4"/>
+      <c r="L162" s="4"/>
+      <c r="M162" s="4"/>
+      <c r="N162" s="4"/>
+      <c r="O162" s="4"/>
+      <c r="P162" s="4"/>
+      <c r="Q162" s="4"/>
+      <c r="R162" s="3"/>
+      <c r="S162" s="4"/>
+      <c r="T162" s="4"/>
+    </row>
+    <row r="163" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B163" s="4"/>
+      <c r="C163" s="3"/>
+      <c r="D163" s="4"/>
+      <c r="E163" s="3"/>
+      <c r="F163" s="4"/>
+      <c r="G163" s="3"/>
+      <c r="H163" s="4"/>
+      <c r="I163" s="3"/>
+      <c r="J163" s="4"/>
+      <c r="K163" s="4"/>
+      <c r="L163" s="4"/>
+      <c r="M163" s="4"/>
+      <c r="N163" s="4"/>
+      <c r="O163" s="4"/>
+      <c r="P163" s="4"/>
+      <c r="Q163" s="4"/>
+      <c r="R163" s="3"/>
+      <c r="S163" s="4"/>
+      <c r="T163" s="4"/>
+    </row>
+    <row r="164" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B164" s="4"/>
+      <c r="C164" s="3"/>
+      <c r="D164" s="4"/>
+      <c r="E164" s="3"/>
+      <c r="F164" s="4"/>
+      <c r="G164" s="3"/>
+      <c r="H164" s="4"/>
+      <c r="I164" s="3"/>
+      <c r="J164" s="4"/>
+      <c r="K164" s="4"/>
+      <c r="L164" s="4"/>
+      <c r="M164" s="4"/>
+      <c r="N164" s="4"/>
+      <c r="O164" s="4"/>
+      <c r="P164" s="4"/>
+      <c r="Q164" s="4"/>
+      <c r="R164" s="3"/>
+      <c r="S164" s="4"/>
+      <c r="T164" s="4"/>
+    </row>
+    <row r="165" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B165" s="4"/>
+      <c r="C165" s="3"/>
+      <c r="D165" s="4"/>
+      <c r="E165" s="3"/>
+      <c r="F165" s="4"/>
+      <c r="G165" s="3"/>
+      <c r="H165" s="4"/>
+      <c r="I165" s="3"/>
+      <c r="J165" s="4"/>
+      <c r="K165" s="4"/>
+      <c r="L165" s="4"/>
+      <c r="M165" s="4"/>
+      <c r="N165" s="4"/>
+      <c r="O165" s="4"/>
+      <c r="P165" s="4"/>
+      <c r="Q165" s="4"/>
+      <c r="R165" s="3"/>
+      <c r="S165" s="4"/>
+      <c r="T165" s="4"/>
+    </row>
+    <row r="166" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B166" s="4"/>
+      <c r="C166" s="3"/>
+      <c r="D166" s="4"/>
+      <c r="E166" s="3"/>
+      <c r="F166" s="4"/>
+      <c r="G166" s="3"/>
+      <c r="H166" s="4"/>
+      <c r="I166" s="3"/>
+      <c r="J166" s="4"/>
+      <c r="K166" s="4"/>
+      <c r="L166" s="4"/>
+      <c r="M166" s="4"/>
+      <c r="N166" s="4"/>
+      <c r="O166" s="4"/>
+      <c r="P166" s="4"/>
+      <c r="Q166" s="4"/>
+      <c r="R166" s="3"/>
+      <c r="S166" s="4"/>
+      <c r="T166" s="4"/>
+    </row>
+    <row r="167" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B167" s="4"/>
+      <c r="C167" s="3"/>
+      <c r="D167" s="4"/>
+      <c r="E167" s="3"/>
+      <c r="F167" s="4"/>
+      <c r="G167" s="3"/>
+      <c r="H167" s="4"/>
+      <c r="I167" s="3"/>
+      <c r="J167" s="4"/>
+      <c r="K167" s="4"/>
+      <c r="L167" s="4"/>
+      <c r="M167" s="4"/>
+      <c r="N167" s="4"/>
+      <c r="O167" s="4"/>
+      <c r="P167" s="4"/>
+      <c r="Q167" s="4"/>
+      <c r="R167" s="3"/>
+      <c r="S167" s="4"/>
+      <c r="T167" s="4"/>
+    </row>
+    <row r="168" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B168" s="4"/>
+      <c r="C168" s="3"/>
+      <c r="D168" s="4"/>
+      <c r="E168" s="3"/>
+      <c r="F168" s="4"/>
+      <c r="G168" s="3"/>
+      <c r="H168" s="4"/>
+      <c r="I168" s="3"/>
+      <c r="J168" s="4"/>
+      <c r="K168" s="4"/>
+      <c r="L168" s="4"/>
+      <c r="M168" s="4"/>
+      <c r="N168" s="4"/>
+      <c r="O168" s="4"/>
+      <c r="P168" s="4"/>
+      <c r="Q168" s="4"/>
+      <c r="R168" s="3"/>
+      <c r="S168" s="4"/>
+      <c r="T168" s="4"/>
+    </row>
+    <row r="169" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B169" s="4"/>
+      <c r="C169" s="3"/>
+      <c r="D169" s="4"/>
+      <c r="E169" s="3"/>
+      <c r="F169" s="4"/>
+      <c r="G169" s="3"/>
+      <c r="H169" s="4"/>
+      <c r="I169" s="3"/>
+      <c r="J169" s="4"/>
+      <c r="K169" s="4"/>
+      <c r="L169" s="4"/>
+      <c r="M169" s="4"/>
+      <c r="N169" s="4"/>
+      <c r="O169" s="4"/>
+      <c r="P169" s="4"/>
+      <c r="Q169" s="4"/>
+      <c r="R169" s="3"/>
+      <c r="S169" s="4"/>
+      <c r="T169" s="4"/>
+    </row>
+    <row r="170" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B170" s="4"/>
+      <c r="C170" s="3"/>
+      <c r="D170" s="4"/>
+      <c r="E170" s="3"/>
+      <c r="F170" s="4"/>
+      <c r="G170" s="3"/>
+      <c r="H170" s="4"/>
+      <c r="I170" s="3"/>
+      <c r="J170" s="4"/>
+      <c r="K170" s="4"/>
+      <c r="L170" s="4"/>
+      <c r="M170" s="4"/>
+      <c r="N170" s="4"/>
+      <c r="O170" s="4"/>
+      <c r="P170" s="4"/>
+      <c r="Q170" s="4"/>
+      <c r="R170" s="3"/>
+      <c r="S170" s="4"/>
+      <c r="T170" s="4"/>
+    </row>
+    <row r="171" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B171" s="4"/>
+      <c r="C171" s="3"/>
+      <c r="D171" s="4"/>
+      <c r="E171" s="3"/>
+      <c r="F171" s="4"/>
+      <c r="G171" s="3"/>
+      <c r="H171" s="4"/>
+      <c r="I171" s="3"/>
+      <c r="J171" s="4"/>
+      <c r="K171" s="4"/>
+      <c r="L171" s="4"/>
+      <c r="M171" s="4"/>
+      <c r="N171" s="4"/>
+      <c r="O171" s="4"/>
+      <c r="P171" s="4"/>
+      <c r="Q171" s="4"/>
+      <c r="R171" s="3"/>
+      <c r="S171" s="4"/>
+      <c r="T171" s="4"/>
+    </row>
+    <row r="172" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B172" s="4"/>
+      <c r="C172" s="3"/>
+      <c r="D172" s="4"/>
+      <c r="E172" s="3"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="3"/>
+      <c r="H172" s="4"/>
+      <c r="I172" s="3"/>
+      <c r="J172" s="4"/>
+      <c r="K172" s="4"/>
+      <c r="L172" s="4"/>
+      <c r="M172" s="4"/>
+      <c r="N172" s="4"/>
+      <c r="O172" s="4"/>
+      <c r="P172" s="4"/>
+      <c r="Q172" s="4"/>
+      <c r="R172" s="3"/>
+      <c r="S172" s="4"/>
+      <c r="T172" s="4"/>
+    </row>
+    <row r="173" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B173" s="4"/>
+      <c r="C173" s="3"/>
+      <c r="D173" s="4"/>
+      <c r="E173" s="3"/>
+      <c r="F173" s="4"/>
+      <c r="G173" s="3"/>
+      <c r="H173" s="4"/>
+      <c r="I173" s="3"/>
+      <c r="J173" s="4"/>
+      <c r="K173" s="4"/>
+      <c r="L173" s="4"/>
+      <c r="M173" s="4"/>
+      <c r="N173" s="4"/>
+      <c r="O173" s="4"/>
+      <c r="P173" s="4"/>
+      <c r="Q173" s="4"/>
+      <c r="R173" s="3"/>
+      <c r="S173" s="4"/>
+      <c r="T173" s="4"/>
+    </row>
+    <row r="174" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B174" s="4"/>
+      <c r="C174" s="3"/>
+      <c r="D174" s="4"/>
+      <c r="E174" s="3"/>
+      <c r="F174" s="4"/>
+      <c r="G174" s="3"/>
+      <c r="H174" s="4"/>
+      <c r="I174" s="3"/>
+      <c r="J174" s="4"/>
+      <c r="K174" s="4"/>
+      <c r="L174" s="4"/>
+      <c r="M174" s="4"/>
+      <c r="N174" s="4"/>
+      <c r="O174" s="4"/>
+      <c r="P174" s="4"/>
+      <c r="Q174" s="4"/>
+      <c r="R174" s="3"/>
+      <c r="S174" s="4"/>
+      <c r="T174" s="4"/>
+    </row>
+    <row r="175" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B175" s="4"/>
+      <c r="C175" s="3"/>
+      <c r="D175" s="4"/>
+      <c r="E175" s="3"/>
+      <c r="F175" s="4"/>
+      <c r="G175" s="3"/>
+      <c r="H175" s="4"/>
+      <c r="I175" s="3"/>
+      <c r="J175" s="4"/>
+      <c r="K175" s="4"/>
+      <c r="L175" s="4"/>
+      <c r="M175" s="4"/>
+      <c r="N175" s="4"/>
+      <c r="O175" s="4"/>
+      <c r="P175" s="4"/>
+      <c r="Q175" s="4"/>
+      <c r="R175" s="3"/>
+      <c r="S175" s="4"/>
+      <c r="T175" s="4"/>
+    </row>
+    <row r="176" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B176" s="4"/>
+      <c r="C176" s="3"/>
+      <c r="D176" s="4"/>
+      <c r="E176" s="3"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="3"/>
+      <c r="H176" s="4"/>
+      <c r="I176" s="3"/>
+      <c r="J176" s="4"/>
+      <c r="K176" s="4"/>
+      <c r="L176" s="4"/>
+      <c r="M176" s="4"/>
+      <c r="N176" s="4"/>
+      <c r="O176" s="4"/>
+      <c r="P176" s="4"/>
+      <c r="Q176" s="4"/>
+      <c r="R176" s="3"/>
+      <c r="S176" s="4"/>
+      <c r="T176" s="4"/>
+    </row>
+    <row r="177" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B177" s="4"/>
+      <c r="C177" s="3"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="3"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="3"/>
+      <c r="H177" s="4"/>
+      <c r="I177" s="3"/>
+      <c r="J177" s="4"/>
+      <c r="K177" s="4"/>
+      <c r="L177" s="4"/>
+      <c r="M177" s="4"/>
+      <c r="N177" s="4"/>
+      <c r="O177" s="4"/>
+      <c r="P177" s="4"/>
+      <c r="Q177" s="4"/>
+      <c r="R177" s="3"/>
+      <c r="S177" s="4"/>
+      <c r="T177" s="4"/>
+    </row>
+    <row r="178" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B178" s="4"/>
+      <c r="C178" s="3"/>
+      <c r="D178" s="4"/>
+      <c r="E178" s="3"/>
+      <c r="F178" s="4"/>
+      <c r="G178" s="3"/>
+      <c r="H178" s="4"/>
+      <c r="I178" s="3"/>
+      <c r="J178" s="4"/>
+      <c r="K178" s="4"/>
+      <c r="L178" s="4"/>
+      <c r="M178" s="4"/>
+      <c r="N178" s="4"/>
+      <c r="O178" s="4"/>
+      <c r="P178" s="4"/>
+      <c r="Q178" s="4"/>
+      <c r="R178" s="3"/>
+      <c r="S178" s="4"/>
+      <c r="T178" s="4"/>
+    </row>
+    <row r="179" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B179" s="4"/>
+      <c r="C179" s="3"/>
+      <c r="D179" s="4"/>
+      <c r="E179" s="3"/>
+      <c r="F179" s="4"/>
+      <c r="G179" s="3"/>
+      <c r="H179" s="4"/>
+      <c r="I179" s="3"/>
+      <c r="J179" s="4"/>
+      <c r="K179" s="4"/>
+      <c r="L179" s="4"/>
+      <c r="M179" s="4"/>
+      <c r="N179" s="4"/>
+      <c r="O179" s="4"/>
+      <c r="P179" s="4"/>
+      <c r="Q179" s="4"/>
+      <c r="R179" s="3"/>
+      <c r="S179" s="4"/>
+      <c r="T179" s="4"/>
+    </row>
+    <row r="180" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B180" s="4"/>
+      <c r="C180" s="3"/>
+      <c r="D180" s="4"/>
+      <c r="E180" s="3"/>
+      <c r="F180" s="4"/>
+      <c r="G180" s="3"/>
+      <c r="H180" s="4"/>
+      <c r="I180" s="3"/>
+      <c r="J180" s="4"/>
+      <c r="K180" s="4"/>
+      <c r="L180" s="4"/>
+      <c r="M180" s="4"/>
+      <c r="N180" s="4"/>
+      <c r="O180" s="4"/>
+      <c r="P180" s="4"/>
+      <c r="Q180" s="4"/>
+      <c r="R180" s="3"/>
+      <c r="S180" s="4"/>
+      <c r="T180" s="4"/>
+    </row>
+    <row r="181" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B181" s="4"/>
+      <c r="C181" s="3"/>
+      <c r="D181" s="4"/>
+      <c r="E181" s="3"/>
+      <c r="F181" s="4"/>
+      <c r="G181" s="3"/>
+      <c r="H181" s="4"/>
+      <c r="I181" s="3"/>
+      <c r="J181" s="4"/>
+      <c r="K181" s="4"/>
+      <c r="L181" s="4"/>
+      <c r="M181" s="4"/>
+      <c r="N181" s="4"/>
+      <c r="O181" s="4"/>
+      <c r="P181" s="4"/>
+      <c r="Q181" s="4"/>
+      <c r="R181" s="3"/>
+      <c r="S181" s="4"/>
+      <c r="T181" s="4"/>
+    </row>
+    <row r="182" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B182" s="4"/>
+      <c r="C182" s="3"/>
+      <c r="D182" s="4"/>
+      <c r="E182" s="3"/>
+      <c r="F182" s="4"/>
+      <c r="G182" s="3"/>
+      <c r="H182" s="4"/>
+      <c r="I182" s="3"/>
+      <c r="J182" s="4"/>
+      <c r="K182" s="4"/>
+      <c r="L182" s="4"/>
+      <c r="M182" s="4"/>
+      <c r="N182" s="4"/>
+      <c r="O182" s="4"/>
+      <c r="P182" s="4"/>
+      <c r="Q182" s="4"/>
+      <c r="R182" s="3"/>
+      <c r="S182" s="4"/>
+      <c r="T182" s="4"/>
+    </row>
+    <row r="183" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B183" s="4"/>
+      <c r="C183" s="3"/>
+      <c r="D183" s="4"/>
+      <c r="E183" s="3"/>
+      <c r="F183" s="4"/>
+      <c r="G183" s="3"/>
+      <c r="H183" s="4"/>
+      <c r="I183" s="3"/>
+      <c r="J183" s="4"/>
+      <c r="K183" s="4"/>
+      <c r="L183" s="4"/>
+      <c r="M183" s="4"/>
+      <c r="N183" s="4"/>
+      <c r="O183" s="4"/>
+      <c r="P183" s="4"/>
+      <c r="Q183" s="4"/>
+      <c r="R183" s="3"/>
+      <c r="S183" s="4"/>
+      <c r="T183" s="4"/>
+    </row>
+    <row r="184" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B184" s="4"/>
+      <c r="C184" s="3"/>
+      <c r="D184" s="4"/>
+      <c r="E184" s="3"/>
+      <c r="F184" s="4"/>
+      <c r="G184" s="3"/>
+      <c r="H184" s="4"/>
+      <c r="I184" s="3"/>
+      <c r="J184" s="4"/>
+      <c r="K184" s="4"/>
+      <c r="L184" s="4"/>
+      <c r="M184" s="4"/>
+      <c r="N184" s="4"/>
+      <c r="O184" s="4"/>
+      <c r="P184" s="4"/>
+      <c r="Q184" s="4"/>
+      <c r="R184" s="3"/>
+      <c r="S184" s="4"/>
+      <c r="T184" s="4"/>
+    </row>
+    <row r="185" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B185" s="4"/>
+      <c r="C185" s="3"/>
+      <c r="D185" s="4"/>
+      <c r="E185" s="3"/>
+      <c r="F185" s="4"/>
+      <c r="G185" s="3"/>
+      <c r="H185" s="4"/>
+      <c r="I185" s="3"/>
+      <c r="J185" s="4"/>
+      <c r="K185" s="4"/>
+      <c r="L185" s="4"/>
+      <c r="M185" s="4"/>
+      <c r="N185" s="4"/>
+      <c r="O185" s="4"/>
+      <c r="P185" s="4"/>
+      <c r="Q185" s="4"/>
+      <c r="R185" s="3"/>
+      <c r="S185" s="4"/>
+      <c r="T185" s="4"/>
+    </row>
+    <row r="186" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B186" s="4"/>
+      <c r="C186" s="3"/>
+      <c r="D186" s="4"/>
+      <c r="E186" s="3"/>
+      <c r="F186" s="4"/>
+      <c r="G186" s="3"/>
+      <c r="H186" s="4"/>
+      <c r="I186" s="3"/>
+      <c r="J186" s="4"/>
+      <c r="K186" s="4"/>
+      <c r="L186" s="4"/>
+      <c r="M186" s="4"/>
+      <c r="N186" s="4"/>
+      <c r="O186" s="4"/>
+      <c r="P186" s="4"/>
+      <c r="Q186" s="4"/>
+      <c r="R186" s="3"/>
+      <c r="S186" s="4"/>
+      <c r="T186" s="4"/>
+    </row>
+    <row r="187" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B187" s="4"/>
+      <c r="C187" s="3"/>
+      <c r="D187" s="4"/>
+      <c r="E187" s="3"/>
+      <c r="F187" s="4"/>
+      <c r="G187" s="3"/>
+      <c r="H187" s="4"/>
+      <c r="I187" s="3"/>
+      <c r="J187" s="4"/>
+      <c r="K187" s="4"/>
+      <c r="L187" s="4"/>
+      <c r="M187" s="4"/>
+      <c r="N187" s="4"/>
+      <c r="O187" s="4"/>
+      <c r="P187" s="4"/>
+      <c r="Q187" s="4"/>
+      <c r="R187" s="3"/>
+      <c r="S187" s="4"/>
+      <c r="T187" s="4"/>
+    </row>
+    <row r="188" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B188" s="4"/>
+      <c r="C188" s="3"/>
+      <c r="D188" s="4"/>
+      <c r="E188" s="3"/>
+      <c r="F188" s="4"/>
+      <c r="G188" s="3"/>
+      <c r="H188" s="4"/>
+      <c r="I188" s="3"/>
+      <c r="J188" s="4"/>
+      <c r="K188" s="4"/>
+      <c r="L188" s="4"/>
+      <c r="M188" s="4"/>
+      <c r="N188" s="4"/>
+      <c r="O188" s="4"/>
+      <c r="P188" s="4"/>
+      <c r="Q188" s="4"/>
+      <c r="R188" s="3"/>
+      <c r="S188" s="4"/>
+      <c r="T188" s="4"/>
+    </row>
+    <row r="189" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B189" s="4"/>
+      <c r="C189" s="3"/>
+      <c r="D189" s="4"/>
+      <c r="E189" s="3"/>
+      <c r="F189" s="4"/>
+      <c r="G189" s="3"/>
+      <c r="H189" s="4"/>
+      <c r="I189" s="3"/>
+      <c r="J189" s="4"/>
+      <c r="K189" s="4"/>
+      <c r="L189" s="4"/>
+      <c r="M189" s="4"/>
+      <c r="N189" s="4"/>
+      <c r="O189" s="4"/>
+      <c r="P189" s="4"/>
+      <c r="Q189" s="4"/>
+      <c r="R189" s="3"/>
+      <c r="S189" s="4"/>
+      <c r="T189" s="4"/>
+    </row>
+    <row r="190" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B190" s="4"/>
+      <c r="C190" s="3"/>
+      <c r="D190" s="4"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="4"/>
+      <c r="G190" s="3"/>
+      <c r="H190" s="4"/>
+      <c r="I190" s="3"/>
+      <c r="J190" s="4"/>
+      <c r="K190" s="4"/>
+      <c r="L190" s="4"/>
+      <c r="M190" s="4"/>
+      <c r="N190" s="4"/>
+      <c r="O190" s="4"/>
+      <c r="P190" s="4"/>
+      <c r="Q190" s="4"/>
+      <c r="R190" s="3"/>
+      <c r="S190" s="4"/>
+      <c r="T190" s="4"/>
+    </row>
+    <row r="191" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B191" s="4"/>
+      <c r="C191" s="3"/>
+      <c r="D191" s="4"/>
+      <c r="E191" s="3"/>
+      <c r="F191" s="4"/>
+      <c r="G191" s="3"/>
+      <c r="H191" s="4"/>
+      <c r="I191" s="3"/>
+      <c r="J191" s="4"/>
+      <c r="K191" s="4"/>
+      <c r="L191" s="4"/>
+      <c r="M191" s="4"/>
+      <c r="N191" s="4"/>
+      <c r="O191" s="4"/>
+      <c r="P191" s="4"/>
+      <c r="Q191" s="4"/>
+      <c r="R191" s="3"/>
+      <c r="S191" s="4"/>
+      <c r="T191" s="4"/>
+    </row>
+    <row r="192" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B192" s="4"/>
+      <c r="C192" s="3"/>
+      <c r="D192" s="4"/>
+      <c r="E192" s="3"/>
+      <c r="F192" s="4"/>
+      <c r="G192" s="3"/>
+      <c r="H192" s="4"/>
+      <c r="I192" s="3"/>
+      <c r="J192" s="4"/>
+      <c r="K192" s="4"/>
+      <c r="L192" s="4"/>
+      <c r="M192" s="4"/>
+      <c r="N192" s="4"/>
+      <c r="O192" s="4"/>
+      <c r="P192" s="4"/>
+      <c r="Q192" s="4"/>
+      <c r="R192" s="3"/>
+      <c r="S192" s="4"/>
+      <c r="T192" s="4"/>
+    </row>
+    <row r="193" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B193" s="4"/>
+      <c r="C193" s="3"/>
+      <c r="D193" s="4"/>
+      <c r="E193" s="3"/>
+      <c r="F193" s="4"/>
+      <c r="G193" s="3"/>
+      <c r="H193" s="4"/>
+      <c r="I193" s="3"/>
+      <c r="J193" s="4"/>
+      <c r="K193" s="4"/>
+      <c r="L193" s="4"/>
+      <c r="M193" s="4"/>
+      <c r="N193" s="4"/>
+      <c r="O193" s="4"/>
+      <c r="P193" s="4"/>
+      <c r="Q193" s="4"/>
+      <c r="R193" s="3"/>
+      <c r="S193" s="4"/>
+      <c r="T193" s="4"/>
+    </row>
+    <row r="194" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B194" s="4"/>
+      <c r="C194" s="3"/>
+      <c r="D194" s="4"/>
+      <c r="E194" s="3"/>
+      <c r="F194" s="4"/>
+      <c r="G194" s="3"/>
+      <c r="H194" s="4"/>
+      <c r="I194" s="3"/>
+      <c r="J194" s="4"/>
+      <c r="K194" s="4"/>
+      <c r="L194" s="4"/>
+      <c r="M194" s="4"/>
+      <c r="N194" s="4"/>
+      <c r="O194" s="4"/>
+      <c r="P194" s="4"/>
+      <c r="Q194" s="4"/>
+      <c r="R194" s="3"/>
+      <c r="S194" s="4"/>
+      <c r="T194" s="4"/>
+    </row>
+    <row r="195" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B195" s="4"/>
+      <c r="C195" s="3"/>
+      <c r="D195" s="4"/>
+      <c r="E195" s="3"/>
+      <c r="F195" s="4"/>
+      <c r="G195" s="3"/>
+      <c r="H195" s="4"/>
+      <c r="I195" s="3"/>
+      <c r="J195" s="4"/>
+      <c r="K195" s="4"/>
+      <c r="L195" s="4"/>
+      <c r="M195" s="4"/>
+      <c r="N195" s="4"/>
+      <c r="O195" s="4"/>
+      <c r="P195" s="4"/>
+      <c r="Q195" s="4"/>
+      <c r="R195" s="3"/>
+      <c r="S195" s="4"/>
+      <c r="T195" s="4"/>
+    </row>
+    <row r="196" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B196" s="4"/>
+      <c r="C196" s="3"/>
+      <c r="D196" s="4"/>
+      <c r="E196" s="3"/>
+      <c r="F196" s="4"/>
+      <c r="G196" s="3"/>
+      <c r="H196" s="4"/>
+      <c r="I196" s="3"/>
+      <c r="J196" s="4"/>
+      <c r="K196" s="4"/>
+      <c r="L196" s="4"/>
+      <c r="M196" s="4"/>
+      <c r="N196" s="4"/>
+      <c r="O196" s="4"/>
+      <c r="P196" s="4"/>
+      <c r="Q196" s="4"/>
+      <c r="R196" s="3"/>
+      <c r="S196" s="4"/>
+      <c r="T196" s="4"/>
+    </row>
+    <row r="197" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B197" s="4"/>
+      <c r="C197" s="3"/>
+      <c r="D197" s="4"/>
+      <c r="E197" s="3"/>
+      <c r="F197" s="4"/>
+      <c r="G197" s="3"/>
+      <c r="H197" s="4"/>
+      <c r="I197" s="3"/>
+      <c r="J197" s="4"/>
+      <c r="K197" s="4"/>
+      <c r="L197" s="4"/>
+      <c r="M197" s="4"/>
+      <c r="N197" s="4"/>
+      <c r="O197" s="4"/>
+      <c r="P197" s="4"/>
+      <c r="Q197" s="4"/>
+      <c r="R197" s="3"/>
+      <c r="S197" s="4"/>
+      <c r="T197" s="4"/>
+    </row>
+    <row r="198" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B198" s="4"/>
+      <c r="C198" s="3"/>
+      <c r="D198" s="4"/>
+      <c r="E198" s="3"/>
+      <c r="F198" s="4"/>
+      <c r="G198" s="3"/>
+      <c r="H198" s="4"/>
+      <c r="I198" s="3"/>
+      <c r="J198" s="4"/>
+      <c r="K198" s="4"/>
+      <c r="L198" s="4"/>
+      <c r="M198" s="4"/>
+      <c r="N198" s="4"/>
+      <c r="O198" s="4"/>
+      <c r="P198" s="4"/>
+      <c r="Q198" s="4"/>
+      <c r="R198" s="3"/>
+      <c r="S198" s="4"/>
+      <c r="T198" s="4"/>
+    </row>
+    <row r="199" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B199" s="4"/>
+      <c r="C199" s="3"/>
+      <c r="D199" s="4"/>
+      <c r="E199" s="3"/>
+      <c r="F199" s="4"/>
+      <c r="G199" s="3"/>
+      <c r="H199" s="4"/>
+      <c r="I199" s="3"/>
+      <c r="J199" s="4"/>
+      <c r="K199" s="4"/>
+      <c r="L199" s="4"/>
+      <c r="M199" s="4"/>
+      <c r="N199" s="4"/>
+      <c r="O199" s="4"/>
+      <c r="P199" s="4"/>
+      <c r="Q199" s="4"/>
+      <c r="R199" s="3"/>
+      <c r="S199" s="4"/>
+      <c r="T199" s="4"/>
+    </row>
+    <row r="200" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B200" s="4"/>
+      <c r="C200" s="3"/>
+      <c r="D200" s="4"/>
+      <c r="E200" s="3"/>
+      <c r="F200" s="4"/>
+      <c r="G200" s="3"/>
+      <c r="H200" s="4"/>
+      <c r="I200" s="3"/>
+      <c r="J200" s="4"/>
+      <c r="K200" s="4"/>
+      <c r="L200" s="4"/>
+      <c r="M200" s="4"/>
+      <c r="N200" s="4"/>
+      <c r="O200" s="4"/>
+      <c r="P200" s="4"/>
+      <c r="Q200" s="4"/>
+      <c r="R200" s="3"/>
+      <c r="S200" s="4"/>
+      <c r="T200" s="4"/>
+    </row>
+    <row r="201" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B201" s="4"/>
+      <c r="C201" s="3"/>
+      <c r="D201" s="4"/>
+      <c r="E201" s="3"/>
+      <c r="F201" s="4"/>
+      <c r="G201" s="3"/>
+      <c r="H201" s="4"/>
+      <c r="I201" s="3"/>
+      <c r="J201" s="4"/>
+      <c r="K201" s="4"/>
+      <c r="L201" s="4"/>
+      <c r="M201" s="4"/>
+      <c r="N201" s="4"/>
+      <c r="O201" s="4"/>
+      <c r="P201" s="4"/>
+      <c r="Q201" s="4"/>
+      <c r="R201" s="3"/>
+      <c r="S201" s="4"/>
+      <c r="T201" s="4"/>
+    </row>
+    <row r="202" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B202" s="4"/>
+      <c r="C202" s="3"/>
+      <c r="D202" s="4"/>
+      <c r="E202" s="3"/>
+      <c r="F202" s="4"/>
+      <c r="G202" s="3"/>
+      <c r="H202" s="4"/>
+      <c r="I202" s="3"/>
+      <c r="J202" s="4"/>
+      <c r="K202" s="4"/>
+      <c r="L202" s="4"/>
+      <c r="M202" s="4"/>
+      <c r="N202" s="4"/>
+      <c r="O202" s="4"/>
+      <c r="P202" s="4"/>
+      <c r="Q202" s="4"/>
+      <c r="R202" s="3"/>
+      <c r="S202" s="4"/>
+      <c r="T202" s="4"/>
+    </row>
+    <row r="203" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B203" s="4"/>
+      <c r="C203" s="3"/>
+      <c r="D203" s="4"/>
+      <c r="E203" s="3"/>
+      <c r="F203" s="4"/>
+      <c r="G203" s="3"/>
+      <c r="H203" s="4"/>
+      <c r="I203" s="3"/>
+      <c r="J203" s="4"/>
+      <c r="K203" s="4"/>
+      <c r="L203" s="4"/>
+      <c r="M203" s="4"/>
+      <c r="N203" s="4"/>
+      <c r="O203" s="4"/>
+      <c r="P203" s="4"/>
+      <c r="Q203" s="4"/>
+      <c r="R203" s="3"/>
+      <c r="S203" s="4"/>
+      <c r="T203" s="4"/>
+    </row>
+    <row r="204" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B204" s="4"/>
+      <c r="C204" s="3"/>
+      <c r="D204" s="4"/>
+      <c r="E204" s="3"/>
+      <c r="F204" s="4"/>
+      <c r="G204" s="3"/>
+      <c r="H204" s="4"/>
+      <c r="I204" s="3"/>
+      <c r="J204" s="4"/>
+      <c r="K204" s="4"/>
+      <c r="L204" s="4"/>
+      <c r="M204" s="4"/>
+      <c r="N204" s="4"/>
+      <c r="O204" s="4"/>
+      <c r="P204" s="4"/>
+      <c r="Q204" s="4"/>
+      <c r="R204" s="3"/>
+      <c r="S204" s="4"/>
+      <c r="T204" s="4"/>
+    </row>
+    <row r="205" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B205" s="4"/>
+      <c r="C205" s="3"/>
+      <c r="D205" s="4"/>
+      <c r="E205" s="3"/>
+      <c r="F205" s="4"/>
+      <c r="G205" s="3"/>
+      <c r="H205" s="4"/>
+      <c r="I205" s="3"/>
+      <c r="J205" s="4"/>
+      <c r="K205" s="4"/>
+      <c r="L205" s="4"/>
+      <c r="M205" s="4"/>
+      <c r="N205" s="4"/>
+      <c r="O205" s="4"/>
+      <c r="P205" s="4"/>
+      <c r="Q205" s="4"/>
+      <c r="R205" s="3"/>
+      <c r="S205" s="4"/>
+      <c r="T205" s="4"/>
+    </row>
+    <row r="206" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B206" s="4"/>
+      <c r="C206" s="3"/>
+      <c r="D206" s="4"/>
+      <c r="E206" s="3"/>
+      <c r="F206" s="4"/>
+      <c r="G206" s="3"/>
+      <c r="H206" s="4"/>
+      <c r="I206" s="3"/>
+      <c r="J206" s="4"/>
+      <c r="K206" s="4"/>
+      <c r="L206" s="4"/>
+      <c r="M206" s="4"/>
+      <c r="N206" s="4"/>
+      <c r="O206" s="4"/>
+      <c r="P206" s="4"/>
+      <c r="Q206" s="4"/>
+      <c r="R206" s="3"/>
+      <c r="S206" s="4"/>
+      <c r="T206" s="4"/>
+    </row>
+    <row r="207" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B207" s="4"/>
+      <c r="C207" s="3"/>
+      <c r="D207" s="4"/>
+      <c r="E207" s="3"/>
+      <c r="F207" s="4"/>
+      <c r="G207" s="3"/>
+      <c r="H207" s="4"/>
+      <c r="I207" s="3"/>
+      <c r="J207" s="4"/>
+      <c r="K207" s="4"/>
+      <c r="L207" s="4"/>
+      <c r="M207" s="4"/>
+      <c r="N207" s="4"/>
+      <c r="O207" s="4"/>
+      <c r="P207" s="4"/>
+      <c r="Q207" s="4"/>
+      <c r="R207" s="3"/>
+      <c r="S207" s="4"/>
+      <c r="T207" s="4"/>
+    </row>
+    <row r="208" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B208" s="4"/>
+      <c r="C208" s="3"/>
+      <c r="D208" s="4"/>
+      <c r="E208" s="3"/>
+      <c r="F208" s="4"/>
+      <c r="G208" s="3"/>
+      <c r="H208" s="4"/>
+      <c r="I208" s="3"/>
+      <c r="J208" s="4"/>
+      <c r="K208" s="4"/>
+      <c r="L208" s="4"/>
+      <c r="M208" s="4"/>
+      <c r="N208" s="4"/>
+      <c r="O208" s="4"/>
+      <c r="P208" s="4"/>
+      <c r="Q208" s="4"/>
+      <c r="R208" s="3"/>
+      <c r="S208" s="4"/>
+      <c r="T208" s="4"/>
+    </row>
+    <row r="209" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B209" s="4"/>
+      <c r="C209" s="3"/>
+      <c r="D209" s="4"/>
+      <c r="E209" s="3"/>
+      <c r="F209" s="4"/>
+      <c r="G209" s="3"/>
+      <c r="H209" s="4"/>
+      <c r="I209" s="3"/>
+      <c r="J209" s="4"/>
+      <c r="K209" s="4"/>
+      <c r="L209" s="4"/>
+      <c r="M209" s="4"/>
+      <c r="N209" s="4"/>
+      <c r="O209" s="4"/>
+      <c r="P209" s="4"/>
+      <c r="Q209" s="4"/>
+      <c r="R209" s="3"/>
+      <c r="S209" s="4"/>
+      <c r="T209" s="4"/>
+    </row>
+    <row r="210" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B210" s="4"/>
+      <c r="C210" s="3"/>
+      <c r="D210" s="4"/>
+      <c r="E210" s="3"/>
+      <c r="F210" s="4"/>
+      <c r="G210" s="3"/>
+      <c r="H210" s="4"/>
+      <c r="I210" s="3"/>
+      <c r="J210" s="4"/>
+      <c r="K210" s="4"/>
+      <c r="L210" s="4"/>
+      <c r="M210" s="4"/>
+      <c r="N210" s="4"/>
+      <c r="O210" s="4"/>
+      <c r="P210" s="4"/>
+      <c r="Q210" s="4"/>
+      <c r="R210" s="3"/>
+      <c r="S210" s="4"/>
+      <c r="T210" s="4"/>
+    </row>
+    <row r="211" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B211" s="4"/>
+      <c r="C211" s="3"/>
+      <c r="D211" s="4"/>
+      <c r="E211" s="3"/>
+      <c r="F211" s="4"/>
+      <c r="G211" s="3"/>
+      <c r="H211" s="4"/>
+      <c r="I211" s="3"/>
+      <c r="J211" s="4"/>
+      <c r="K211" s="4"/>
+      <c r="L211" s="4"/>
+      <c r="M211" s="4"/>
+      <c r="N211" s="4"/>
+      <c r="O211" s="4"/>
+      <c r="P211" s="4"/>
+      <c r="Q211" s="4"/>
+      <c r="R211" s="3"/>
+      <c r="S211" s="4"/>
+      <c r="T211" s="4"/>
+    </row>
+    <row r="212" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B212" s="4"/>
+      <c r="C212" s="3"/>
+      <c r="D212" s="4"/>
+      <c r="E212" s="3"/>
+      <c r="F212" s="4"/>
+      <c r="G212" s="3"/>
+      <c r="H212" s="4"/>
+      <c r="I212" s="3"/>
+      <c r="J212" s="4"/>
+      <c r="K212" s="4"/>
+      <c r="L212" s="4"/>
+      <c r="M212" s="4"/>
+      <c r="N212" s="4"/>
+      <c r="O212" s="4"/>
+      <c r="P212" s="4"/>
+      <c r="Q212" s="4"/>
+      <c r="R212" s="3"/>
+      <c r="S212" s="4"/>
+      <c r="T212" s="4"/>
+    </row>
+    <row r="213" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B213" s="4"/>
+      <c r="C213" s="3"/>
+      <c r="D213" s="4"/>
+      <c r="E213" s="3"/>
+      <c r="F213" s="4"/>
+      <c r="G213" s="3"/>
+      <c r="H213" s="4"/>
+      <c r="I213" s="3"/>
+      <c r="J213" s="4"/>
+      <c r="K213" s="4"/>
+      <c r="L213" s="4"/>
+      <c r="M213" s="4"/>
+      <c r="N213" s="4"/>
+      <c r="O213" s="4"/>
+      <c r="P213" s="4"/>
+      <c r="Q213" s="4"/>
+      <c r="R213" s="3"/>
+      <c r="S213" s="4"/>
+      <c r="T213" s="4"/>
+    </row>
+    <row r="214" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B214" s="4"/>
+      <c r="C214" s="3"/>
+      <c r="D214" s="4"/>
+      <c r="E214" s="3"/>
+      <c r="F214" s="4"/>
+      <c r="G214" s="3"/>
+      <c r="H214" s="4"/>
+      <c r="I214" s="3"/>
+      <c r="J214" s="4"/>
+      <c r="K214" s="4"/>
+      <c r="L214" s="4"/>
+      <c r="M214" s="4"/>
+      <c r="N214" s="4"/>
+      <c r="O214" s="4"/>
+      <c r="P214" s="4"/>
+      <c r="Q214" s="4"/>
+      <c r="R214" s="3"/>
+      <c r="S214" s="4"/>
+      <c r="T214" s="4"/>
+    </row>
+    <row r="215" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B215" s="4"/>
+      <c r="C215" s="3"/>
+      <c r="D215" s="4"/>
+      <c r="E215" s="3"/>
+      <c r="F215" s="4"/>
+      <c r="G215" s="3"/>
+      <c r="H215" s="4"/>
+      <c r="I215" s="3"/>
+      <c r="J215" s="4"/>
+      <c r="K215" s="4"/>
+      <c r="L215" s="4"/>
+      <c r="M215" s="4"/>
+      <c r="N215" s="4"/>
+      <c r="O215" s="4"/>
+      <c r="P215" s="4"/>
+      <c r="Q215" s="4"/>
+      <c r="R215" s="3"/>
+      <c r="S215" s="4"/>
+      <c r="T215" s="4"/>
+    </row>
+    <row r="216" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B216" s="4"/>
+      <c r="C216" s="3"/>
+      <c r="D216" s="4"/>
+      <c r="E216" s="3"/>
+      <c r="F216" s="4"/>
+      <c r="G216" s="3"/>
+      <c r="H216" s="4"/>
+      <c r="I216" s="3"/>
+      <c r="J216" s="4"/>
+      <c r="K216" s="4"/>
+      <c r="L216" s="4"/>
+      <c r="M216" s="4"/>
+      <c r="N216" s="4"/>
+      <c r="O216" s="4"/>
+      <c r="P216" s="4"/>
+      <c r="Q216" s="4"/>
+      <c r="R216" s="3"/>
+      <c r="S216" s="4"/>
+      <c r="T216" s="4"/>
+    </row>
+    <row r="217" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B217" s="4"/>
+      <c r="C217" s="3"/>
+      <c r="D217" s="4"/>
+      <c r="E217" s="3"/>
+      <c r="F217" s="4"/>
+      <c r="G217" s="3"/>
+      <c r="H217" s="4"/>
+      <c r="I217" s="3"/>
+      <c r="J217" s="4"/>
+      <c r="K217" s="4"/>
+      <c r="L217" s="4"/>
+      <c r="M217" s="4"/>
+      <c r="N217" s="4"/>
+      <c r="O217" s="4"/>
+      <c r="P217" s="4"/>
+      <c r="Q217" s="4"/>
+      <c r="R217" s="3"/>
+      <c r="S217" s="4"/>
+      <c r="T217" s="4"/>
+    </row>
+    <row r="218" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B218" s="4"/>
+      <c r="C218" s="3"/>
+      <c r="D218" s="4"/>
+      <c r="E218" s="3"/>
+      <c r="F218" s="4"/>
+      <c r="G218" s="3"/>
+      <c r="H218" s="4"/>
+      <c r="I218" s="3"/>
+      <c r="J218" s="4"/>
+      <c r="K218" s="4"/>
+      <c r="L218" s="4"/>
+      <c r="M218" s="4"/>
+      <c r="N218" s="4"/>
+      <c r="O218" s="4"/>
+      <c r="P218" s="4"/>
+      <c r="Q218" s="4"/>
+      <c r="R218" s="3"/>
+      <c r="S218" s="4"/>
+      <c r="T218" s="4"/>
+    </row>
+    <row r="219" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B219" s="4"/>
+      <c r="C219" s="3"/>
+      <c r="D219" s="4"/>
+      <c r="E219" s="3"/>
+      <c r="F219" s="4"/>
+      <c r="G219" s="3"/>
+      <c r="H219" s="4"/>
+      <c r="I219" s="3"/>
+      <c r="J219" s="4"/>
+      <c r="K219" s="4"/>
+      <c r="L219" s="4"/>
+      <c r="M219" s="4"/>
+      <c r="N219" s="4"/>
+      <c r="O219" s="4"/>
+      <c r="P219" s="4"/>
+      <c r="Q219" s="4"/>
+      <c r="R219" s="3"/>
+      <c r="S219" s="4"/>
+      <c r="T219" s="4"/>
+    </row>
+    <row r="220" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B220" s="4"/>
+      <c r="C220" s="3"/>
+      <c r="D220" s="4"/>
+      <c r="E220" s="3"/>
+      <c r="F220" s="4"/>
+      <c r="G220" s="3"/>
+      <c r="H220" s="4"/>
+      <c r="I220" s="3"/>
+      <c r="J220" s="4"/>
+      <c r="K220" s="4"/>
+      <c r="L220" s="4"/>
+      <c r="M220" s="4"/>
+      <c r="N220" s="4"/>
+      <c r="O220" s="4"/>
+      <c r="P220" s="4"/>
+      <c r="Q220" s="4"/>
+      <c r="R220" s="3"/>
+      <c r="S220" s="4"/>
+      <c r="T220" s="4"/>
+    </row>
+    <row r="221" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B221" s="4"/>
+      <c r="C221" s="3"/>
+      <c r="D221" s="4"/>
+      <c r="E221" s="3"/>
+      <c r="F221" s="4"/>
+      <c r="G221" s="3"/>
+      <c r="H221" s="4"/>
+      <c r="I221" s="3"/>
+      <c r="J221" s="4"/>
+      <c r="K221" s="4"/>
+      <c r="L221" s="4"/>
+      <c r="M221" s="4"/>
+      <c r="N221" s="4"/>
+      <c r="O221" s="4"/>
+      <c r="P221" s="4"/>
+      <c r="Q221" s="4"/>
+      <c r="R221" s="3"/>
+      <c r="S221" s="4"/>
+      <c r="T221" s="4"/>
+    </row>
+    <row r="222" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B222" s="4"/>
+      <c r="C222" s="3"/>
+      <c r="D222" s="4"/>
+      <c r="E222" s="3"/>
+      <c r="F222" s="4"/>
+      <c r="G222" s="3"/>
+      <c r="H222" s="4"/>
+      <c r="I222" s="3"/>
+      <c r="J222" s="4"/>
+      <c r="K222" s="4"/>
+      <c r="L222" s="4"/>
+      <c r="M222" s="4"/>
+      <c r="N222" s="4"/>
+      <c r="O222" s="4"/>
+      <c r="P222" s="4"/>
+      <c r="Q222" s="4"/>
+      <c r="R222" s="3"/>
+      <c r="S222" s="4"/>
+      <c r="T222" s="4"/>
+    </row>
+    <row r="223" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B223" s="4"/>
+      <c r="C223" s="3"/>
+      <c r="D223" s="4"/>
+      <c r="E223" s="3"/>
+      <c r="F223" s="4"/>
+      <c r="G223" s="3"/>
+      <c r="H223" s="4"/>
+      <c r="I223" s="3"/>
+      <c r="J223" s="4"/>
+      <c r="K223" s="4"/>
+      <c r="L223" s="4"/>
+      <c r="M223" s="4"/>
+      <c r="N223" s="4"/>
+      <c r="O223" s="4"/>
+      <c r="P223" s="4"/>
+      <c r="Q223" s="4"/>
+      <c r="R223" s="3"/>
+      <c r="S223" s="4"/>
+      <c r="T223" s="4"/>
+    </row>
+    <row r="224" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B224" s="4"/>
+      <c r="C224" s="3"/>
+      <c r="D224" s="4"/>
+      <c r="E224" s="3"/>
+      <c r="F224" s="4"/>
+      <c r="G224" s="3"/>
+      <c r="H224" s="4"/>
+      <c r="I224" s="3"/>
+      <c r="J224" s="4"/>
+      <c r="K224" s="4"/>
+      <c r="L224" s="4"/>
+      <c r="M224" s="4"/>
+      <c r="N224" s="4"/>
+      <c r="O224" s="4"/>
+      <c r="P224" s="4"/>
+      <c r="Q224" s="4"/>
+      <c r="R224" s="3"/>
+      <c r="S224" s="4"/>
+      <c r="T224" s="4"/>
+    </row>
+    <row r="225" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B225" s="4"/>
+      <c r="C225" s="3"/>
+      <c r="D225" s="4"/>
+      <c r="E225" s="3"/>
+      <c r="F225" s="4"/>
+      <c r="G225" s="3"/>
+      <c r="H225" s="4"/>
+      <c r="I225" s="3"/>
+      <c r="J225" s="4"/>
+      <c r="K225" s="4"/>
+      <c r="L225" s="4"/>
+      <c r="M225" s="4"/>
+      <c r="N225" s="4"/>
+      <c r="O225" s="4"/>
+      <c r="P225" s="4"/>
+      <c r="Q225" s="4"/>
+      <c r="R225" s="3"/>
+      <c r="S225" s="4"/>
+      <c r="T225" s="4"/>
+    </row>
+    <row r="226" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B226" s="4"/>
+      <c r="C226" s="3"/>
+      <c r="D226" s="4"/>
+      <c r="E226" s="3"/>
+      <c r="F226" s="4"/>
+      <c r="G226" s="3"/>
+      <c r="H226" s="4"/>
+      <c r="I226" s="3"/>
+      <c r="J226" s="4"/>
+      <c r="K226" s="4"/>
+      <c r="L226" s="4"/>
+      <c r="M226" s="4"/>
+      <c r="N226" s="4"/>
+      <c r="O226" s="4"/>
+      <c r="P226" s="4"/>
+      <c r="Q226" s="4"/>
+      <c r="R226" s="3"/>
+      <c r="S226" s="4"/>
+      <c r="T226" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Docs: #18 Add Documents for Mouse Cursor Manager
#18
+ Flowchart: 마우스 커서 매니저
+ Class Diagram 업데이트
+ RS 업데이트
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE277A06-2E49-4A5C-9E51-A513D772ABED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA5DCE3-9279-425E-A1E5-79DFB3687B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8625" yWindow="2730" windowWidth="17925" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="105">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -422,6 +422,13 @@
   </si>
   <si>
     <t>FR-C-E-03.05</t>
+  </si>
+  <si>
+    <t>FR-C-03</t>
+  </si>
+  <si>
+    <t>마우스 커서 조건에 따라 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -805,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U40" sqref="U40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1240,9 +1247,13 @@
       <c r="E25" s="3"/>
       <c r="F25" s="4"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="4"/>
+      <c r="H25" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="I25" s="3"/>
-      <c r="J25" s="4"/>
+      <c r="J25" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -1251,7 +1262,7 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="3"/>
-      <c r="S25" s="4"/>
+      <c r="S25" s="1"/>
       <c r="T25" s="4"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Docs: #18 Add Documents for Mouse Cursor Manager (#20)
#18
+ Flowchart: 마우스 커서 매니저
+ Class Diagram 업데이트
+ RS 업데이트
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE277A06-2E49-4A5C-9E51-A513D772ABED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA5DCE3-9279-425E-A1E5-79DFB3687B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8625" yWindow="2730" windowWidth="17925" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="105">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -422,6 +422,13 @@
   </si>
   <si>
     <t>FR-C-E-03.05</t>
+  </si>
+  <si>
+    <t>FR-C-03</t>
+  </si>
+  <si>
+    <t>마우스 커서 조건에 따라 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -805,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U40" sqref="U40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1240,9 +1247,13 @@
       <c r="E25" s="3"/>
       <c r="F25" s="4"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="4"/>
+      <c r="H25" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="I25" s="3"/>
-      <c r="J25" s="4"/>
+      <c r="J25" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -1251,7 +1262,7 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="3"/>
-      <c r="S25" s="4"/>
+      <c r="S25" s="1"/>
       <c r="T25" s="4"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Docs: Structure for Key Toggle Manager
#22

+ 전체 게임 내 키 토글을 제어하기 위한 키 ~ 함수 매핑식 키 토글 매니저 선언
+ 컨텐츠 모달 관련 문서 업데이트:: FC, RS, CD
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA5DCE3-9279-425E-A1E5-79DFB3687B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE914E86-494A-435A-98B8-D725FC0A4AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8625" yWindow="2730" windowWidth="17925" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="136">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -428,6 +428,119 @@
   </si>
   <si>
     <t>마우스 커서 조건에 따라 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-04</t>
+  </si>
+  <si>
+    <t>FR-U-M-04.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-04.02</t>
+  </si>
+  <si>
+    <t>FR-U-M-04.03</t>
+  </si>
+  <si>
+    <t>FR-U-M-04.04</t>
+  </si>
+  <si>
+    <t>토글 함수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내부 컨텐츠 초기화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트래킹 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-04.05</t>
+  </si>
+  <si>
+    <t>FR-U-M-04.06</t>
+  </si>
+  <si>
+    <t>FR-U-M-04.07</t>
+  </si>
+  <si>
+    <t>토글 키 트래킹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 트래킹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 함수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-04.04.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-04.04.02</t>
+  </si>
+  <si>
+    <t>FR-U-M-05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-05.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨텐츠 초기화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-05.02</t>
+  </si>
+  <si>
+    <t>FR-U-M-05.03</t>
+  </si>
+  <si>
+    <t>FR-S-03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단축키 시스템</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨텐츠 모달 추상 클래스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[SerializeField] 기반 사이즈 초기화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내부 컨텐츠 적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초기 오브젝트 연결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-04.08</t>
+  </si>
+  <si>
+    <t>컨텐츠 모달용 VO 선언</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트용 컨텐츠 모달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임 오브젝트 연결</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -812,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1048,9 +1161,13 @@
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="4"/>
+      <c r="J16" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -1059,7 +1176,7 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="4"/>
+      <c r="S16" s="1"/>
       <c r="T16" s="4"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.3">
@@ -1410,7 +1527,7 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="1"/>
+      <c r="S31" s="2"/>
       <c r="T31" s="4"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
@@ -1460,7 +1577,7 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="3"/>
-      <c r="S33" s="1"/>
+      <c r="S33" s="2"/>
       <c r="T33" s="4"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.3">
@@ -1535,7 +1652,7 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="3"/>
-      <c r="S36" s="1"/>
+      <c r="S36" s="2"/>
       <c r="T36" s="4"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.3">
@@ -2620,9 +2737,13 @@
       <c r="E84" s="3"/>
       <c r="F84" s="4"/>
       <c r="G84" s="3"/>
-      <c r="H84" s="4"/>
+      <c r="H84" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="I84" s="3"/>
-      <c r="J84" s="4"/>
+      <c r="J84" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="K84" s="4"/>
       <c r="L84" s="4"/>
       <c r="M84" s="4"/>
@@ -2631,7 +2752,7 @@
       <c r="P84" s="4"/>
       <c r="Q84" s="4"/>
       <c r="R84" s="3"/>
-      <c r="S84" s="4"/>
+      <c r="S84" s="1"/>
       <c r="T84" s="4"/>
     </row>
     <row r="85" spans="2:20" x14ac:dyDescent="0.3">
@@ -2641,10 +2762,14 @@
       <c r="E85" s="3"/>
       <c r="F85" s="4"/>
       <c r="G85" s="3"/>
-      <c r="H85" s="4"/>
+      <c r="H85" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="I85" s="3"/>
       <c r="J85" s="4"/>
-      <c r="K85" s="4"/>
+      <c r="K85" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
       <c r="N85" s="4"/>
@@ -2652,7 +2777,7 @@
       <c r="P85" s="4"/>
       <c r="Q85" s="4"/>
       <c r="R85" s="3"/>
-      <c r="S85" s="4"/>
+      <c r="S85" s="1"/>
       <c r="T85" s="4"/>
     </row>
     <row r="86" spans="2:20" x14ac:dyDescent="0.3">
@@ -2662,10 +2787,14 @@
       <c r="E86" s="3"/>
       <c r="F86" s="4"/>
       <c r="G86" s="3"/>
-      <c r="H86" s="4"/>
+      <c r="H86" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="I86" s="3"/>
       <c r="J86" s="4"/>
-      <c r="K86" s="4"/>
+      <c r="K86" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
       <c r="N86" s="4"/>
@@ -2673,7 +2802,7 @@
       <c r="P86" s="4"/>
       <c r="Q86" s="4"/>
       <c r="R86" s="3"/>
-      <c r="S86" s="4"/>
+      <c r="S86" s="1"/>
       <c r="T86" s="4"/>
     </row>
     <row r="87" spans="2:20" x14ac:dyDescent="0.3">
@@ -2683,10 +2812,14 @@
       <c r="E87" s="3"/>
       <c r="F87" s="4"/>
       <c r="G87" s="3"/>
-      <c r="H87" s="4"/>
+      <c r="H87" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="I87" s="3"/>
       <c r="J87" s="4"/>
-      <c r="K87" s="4"/>
+      <c r="K87" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="L87" s="4"/>
       <c r="M87" s="4"/>
       <c r="N87" s="4"/>
@@ -2694,7 +2827,7 @@
       <c r="P87" s="4"/>
       <c r="Q87" s="4"/>
       <c r="R87" s="3"/>
-      <c r="S87" s="4"/>
+      <c r="S87" s="1"/>
       <c r="T87" s="4"/>
     </row>
     <row r="88" spans="2:20" x14ac:dyDescent="0.3">
@@ -2704,10 +2837,14 @@
       <c r="E88" s="3"/>
       <c r="F88" s="4"/>
       <c r="G88" s="3"/>
-      <c r="H88" s="4"/>
+      <c r="H88" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="I88" s="3"/>
       <c r="J88" s="4"/>
-      <c r="K88" s="4"/>
+      <c r="K88" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
       <c r="N88" s="4"/>
@@ -2715,7 +2852,7 @@
       <c r="P88" s="4"/>
       <c r="Q88" s="4"/>
       <c r="R88" s="3"/>
-      <c r="S88" s="4"/>
+      <c r="S88" s="1"/>
       <c r="T88" s="4"/>
     </row>
     <row r="89" spans="2:20" x14ac:dyDescent="0.3">
@@ -2725,18 +2862,22 @@
       <c r="E89" s="3"/>
       <c r="F89" s="4"/>
       <c r="G89" s="3"/>
-      <c r="H89" s="4"/>
+      <c r="H89" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="I89" s="3"/>
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
-      <c r="L89" s="4"/>
+      <c r="L89" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="M89" s="4"/>
       <c r="N89" s="4"/>
       <c r="O89" s="4"/>
       <c r="P89" s="4"/>
       <c r="Q89" s="4"/>
       <c r="R89" s="3"/>
-      <c r="S89" s="4"/>
+      <c r="S89" s="1"/>
       <c r="T89" s="4"/>
     </row>
     <row r="90" spans="2:20" x14ac:dyDescent="0.3">
@@ -2746,18 +2887,22 @@
       <c r="E90" s="3"/>
       <c r="F90" s="4"/>
       <c r="G90" s="3"/>
-      <c r="H90" s="4"/>
+      <c r="H90" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="I90" s="3"/>
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
-      <c r="L90" s="4"/>
+      <c r="L90" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="M90" s="4"/>
       <c r="N90" s="4"/>
       <c r="O90" s="4"/>
       <c r="P90" s="4"/>
       <c r="Q90" s="4"/>
       <c r="R90" s="3"/>
-      <c r="S90" s="4"/>
+      <c r="S90" s="1"/>
       <c r="T90" s="4"/>
     </row>
     <row r="91" spans="2:20" x14ac:dyDescent="0.3">
@@ -2769,18 +2914,16 @@
         <v>7</v>
       </c>
       <c r="E91" s="3"/>
-      <c r="F91" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="F91" s="4"/>
       <c r="G91" s="3"/>
       <c r="H91" s="4" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="I91" s="3"/>
-      <c r="J91" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="K91" s="4"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="L91" s="4"/>
       <c r="M91" s="4"/>
       <c r="N91" s="4"/>
@@ -2788,7 +2931,7 @@
       <c r="P91" s="4"/>
       <c r="Q91" s="4"/>
       <c r="R91" s="3"/>
-      <c r="S91" s="1"/>
+      <c r="S91" s="2"/>
       <c r="T91" s="4"/>
     </row>
     <row r="92" spans="2:20" x14ac:dyDescent="0.3">
@@ -2799,13 +2942,13 @@
       <c r="F92" s="4"/>
       <c r="G92" s="3"/>
       <c r="H92" s="4" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="I92" s="3"/>
-      <c r="J92" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="K92" s="4"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
       <c r="N92" s="4"/>
@@ -2823,10 +2966,14 @@
       <c r="E93" s="3"/>
       <c r="F93" s="4"/>
       <c r="G93" s="3"/>
-      <c r="H93" s="4"/>
+      <c r="H93" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="I93" s="3"/>
       <c r="J93" s="4"/>
-      <c r="K93" s="4"/>
+      <c r="K93" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
       <c r="N93" s="4"/>
@@ -2834,7 +2981,7 @@
       <c r="P93" s="4"/>
       <c r="Q93" s="4"/>
       <c r="R93" s="3"/>
-      <c r="S93" s="4"/>
+      <c r="S93" s="1"/>
       <c r="T93" s="4"/>
     </row>
     <row r="94" spans="2:20" x14ac:dyDescent="0.3">
@@ -2844,10 +2991,14 @@
       <c r="E94" s="3"/>
       <c r="F94" s="4"/>
       <c r="G94" s="3"/>
-      <c r="H94" s="4"/>
+      <c r="H94" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="I94" s="3"/>
       <c r="J94" s="4"/>
-      <c r="K94" s="4"/>
+      <c r="K94" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="L94" s="4"/>
       <c r="M94" s="4"/>
       <c r="N94" s="4"/>
@@ -2855,7 +3006,7 @@
       <c r="P94" s="4"/>
       <c r="Q94" s="4"/>
       <c r="R94" s="3"/>
-      <c r="S94" s="4"/>
+      <c r="S94" s="1"/>
       <c r="T94" s="4"/>
     </row>
     <row r="95" spans="2:20" x14ac:dyDescent="0.3">
@@ -2865,9 +3016,13 @@
       <c r="E95" s="3"/>
       <c r="F95" s="4"/>
       <c r="G95" s="3"/>
-      <c r="H95" s="4"/>
+      <c r="H95" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I95" s="3"/>
-      <c r="J95" s="4"/>
+      <c r="J95" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
       <c r="M95" s="4"/>
@@ -2876,7 +3031,7 @@
       <c r="P95" s="4"/>
       <c r="Q95" s="4"/>
       <c r="R95" s="3"/>
-      <c r="S95" s="4"/>
+      <c r="S95" s="1"/>
       <c r="T95" s="4"/>
     </row>
     <row r="96" spans="2:20" x14ac:dyDescent="0.3">
@@ -2886,10 +3041,14 @@
       <c r="E96" s="3"/>
       <c r="F96" s="4"/>
       <c r="G96" s="3"/>
-      <c r="H96" s="4"/>
+      <c r="H96" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="I96" s="3"/>
       <c r="J96" s="4"/>
-      <c r="K96" s="4"/>
+      <c r="K96" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="L96" s="4"/>
       <c r="M96" s="4"/>
       <c r="N96" s="4"/>
@@ -2897,7 +3056,7 @@
       <c r="P96" s="4"/>
       <c r="Q96" s="4"/>
       <c r="R96" s="3"/>
-      <c r="S96" s="4"/>
+      <c r="S96" s="1"/>
       <c r="T96" s="4"/>
     </row>
     <row r="97" spans="2:20" x14ac:dyDescent="0.3">
@@ -2907,10 +3066,14 @@
       <c r="E97" s="3"/>
       <c r="F97" s="4"/>
       <c r="G97" s="3"/>
-      <c r="H97" s="4"/>
+      <c r="H97" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="I97" s="3"/>
       <c r="J97" s="4"/>
-      <c r="K97" s="4"/>
+      <c r="K97" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="L97" s="4"/>
       <c r="M97" s="4"/>
       <c r="N97" s="4"/>
@@ -2918,7 +3081,7 @@
       <c r="P97" s="4"/>
       <c r="Q97" s="4"/>
       <c r="R97" s="3"/>
-      <c r="S97" s="4"/>
+      <c r="S97" s="1"/>
       <c r="T97" s="4"/>
     </row>
     <row r="98" spans="2:20" x14ac:dyDescent="0.3">
@@ -2928,10 +3091,14 @@
       <c r="E98" s="3"/>
       <c r="F98" s="4"/>
       <c r="G98" s="3"/>
-      <c r="H98" s="4"/>
+      <c r="H98" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="I98" s="3"/>
       <c r="J98" s="4"/>
-      <c r="K98" s="4"/>
+      <c r="K98" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="L98" s="4"/>
       <c r="M98" s="4"/>
       <c r="N98" s="4"/>
@@ -2939,7 +3106,7 @@
       <c r="P98" s="4"/>
       <c r="Q98" s="4"/>
       <c r="R98" s="3"/>
-      <c r="S98" s="4"/>
+      <c r="S98" s="1"/>
       <c r="T98" s="4"/>
     </row>
     <row r="99" spans="2:20" x14ac:dyDescent="0.3">
@@ -3094,11 +3261,17 @@
       <c r="C106" s="3"/>
       <c r="D106" s="4"/>
       <c r="E106" s="3"/>
-      <c r="F106" s="4"/>
+      <c r="F106" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="G106" s="3"/>
-      <c r="H106" s="4"/>
+      <c r="H106" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="I106" s="3"/>
-      <c r="J106" s="4"/>
+      <c r="J106" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="K106" s="4"/>
       <c r="L106" s="4"/>
       <c r="M106" s="4"/>
@@ -3107,7 +3280,7 @@
       <c r="P106" s="4"/>
       <c r="Q106" s="4"/>
       <c r="R106" s="3"/>
-      <c r="S106" s="4"/>
+      <c r="S106" s="1"/>
       <c r="T106" s="4"/>
     </row>
     <row r="107" spans="2:20" x14ac:dyDescent="0.3">
@@ -3117,9 +3290,13 @@
       <c r="E107" s="3"/>
       <c r="F107" s="4"/>
       <c r="G107" s="3"/>
-      <c r="H107" s="4"/>
+      <c r="H107" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="I107" s="3"/>
-      <c r="J107" s="4"/>
+      <c r="J107" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="K107" s="4"/>
       <c r="L107" s="4"/>
       <c r="M107" s="4"/>
@@ -3128,7 +3305,7 @@
       <c r="P107" s="4"/>
       <c r="Q107" s="4"/>
       <c r="R107" s="3"/>
-      <c r="S107" s="4"/>
+      <c r="S107" s="1"/>
       <c r="T107" s="4"/>
     </row>
     <row r="108" spans="2:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Docs: ContentModal for Grid
#22

+ 그리드 형식의 컨텐츠 모달 구상중: 6 * 8 기준
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE914E86-494A-435A-98B8-D725FC0A4AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104A9263-6956-4325-8D27-BD2C98AB76A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="143">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -513,6 +513,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>FR-U-M-06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-06.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>컨텐츠 모달 추상 클래스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -542,6 +550,24 @@
   <si>
     <t>게임 오브젝트 연결</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리드용 컨텐츠 모달 추상 클래스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리드용 컨텐츠 클래스: 단일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-06.01.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-06.01.02</t>
+  </si>
+  <si>
+    <t>FR-U-M-06.01.03</t>
   </si>
 </sst>
 </file>
@@ -925,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K77" sqref="K77"/>
+    <sheetView tabSelected="1" topLeftCell="D57" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U92" sqref="U92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2742,7 +2768,7 @@
       </c>
       <c r="I84" s="3"/>
       <c r="J84" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K84" s="4"/>
       <c r="L84" s="4"/>
@@ -2768,7 +2794,7 @@
       <c r="I85" s="3"/>
       <c r="J85" s="4"/>
       <c r="K85" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
@@ -2947,7 +2973,7 @@
       <c r="I92" s="3"/>
       <c r="J92" s="4"/>
       <c r="K92" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
@@ -2972,7 +2998,7 @@
       <c r="I93" s="3"/>
       <c r="J93" s="4"/>
       <c r="K93" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
@@ -2992,12 +3018,12 @@
       <c r="F94" s="4"/>
       <c r="G94" s="3"/>
       <c r="H94" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I94" s="3"/>
       <c r="J94" s="4"/>
       <c r="K94" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L94" s="4"/>
       <c r="M94" s="4"/>
@@ -3021,7 +3047,7 @@
       </c>
       <c r="I95" s="3"/>
       <c r="J95" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
@@ -3072,7 +3098,7 @@
       <c r="I97" s="3"/>
       <c r="J97" s="4"/>
       <c r="K97" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L97" s="4"/>
       <c r="M97" s="4"/>
@@ -3097,7 +3123,7 @@
       <c r="I98" s="3"/>
       <c r="J98" s="4"/>
       <c r="K98" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L98" s="4"/>
       <c r="M98" s="4"/>
@@ -3116,9 +3142,13 @@
       <c r="E99" s="3"/>
       <c r="F99" s="4"/>
       <c r="G99" s="3"/>
-      <c r="H99" s="4"/>
+      <c r="H99" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="I99" s="3"/>
-      <c r="J99" s="4"/>
+      <c r="J99" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="K99" s="4"/>
       <c r="L99" s="4"/>
       <c r="M99" s="4"/>
@@ -3127,7 +3157,7 @@
       <c r="P99" s="4"/>
       <c r="Q99" s="4"/>
       <c r="R99" s="3"/>
-      <c r="S99" s="4"/>
+      <c r="S99" s="2"/>
       <c r="T99" s="4"/>
     </row>
     <row r="100" spans="2:20" x14ac:dyDescent="0.3">
@@ -3137,10 +3167,14 @@
       <c r="E100" s="3"/>
       <c r="F100" s="4"/>
       <c r="G100" s="3"/>
-      <c r="H100" s="4"/>
+      <c r="H100" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="I100" s="3"/>
       <c r="J100" s="4"/>
-      <c r="K100" s="4"/>
+      <c r="K100" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="L100" s="4"/>
       <c r="M100" s="4"/>
       <c r="N100" s="4"/>
@@ -3148,7 +3182,7 @@
       <c r="P100" s="4"/>
       <c r="Q100" s="4"/>
       <c r="R100" s="3"/>
-      <c r="S100" s="4"/>
+      <c r="S100" s="2"/>
       <c r="T100" s="4"/>
     </row>
     <row r="101" spans="2:20" x14ac:dyDescent="0.3">
@@ -3158,18 +3192,22 @@
       <c r="E101" s="3"/>
       <c r="F101" s="4"/>
       <c r="G101" s="3"/>
-      <c r="H101" s="4"/>
+      <c r="H101" s="4" t="s">
+        <v>140</v>
+      </c>
       <c r="I101" s="3"/>
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
-      <c r="L101" s="4"/>
+      <c r="L101" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="M101" s="4"/>
       <c r="N101" s="4"/>
       <c r="O101" s="4"/>
       <c r="P101" s="4"/>
       <c r="Q101" s="4"/>
       <c r="R101" s="3"/>
-      <c r="S101" s="4"/>
+      <c r="S101" s="2"/>
       <c r="T101" s="4"/>
     </row>
     <row r="102" spans="2:20" x14ac:dyDescent="0.3">
@@ -3179,18 +3217,22 @@
       <c r="E102" s="3"/>
       <c r="F102" s="4"/>
       <c r="G102" s="3"/>
-      <c r="H102" s="4"/>
+      <c r="H102" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="I102" s="3"/>
       <c r="J102" s="4"/>
       <c r="K102" s="4"/>
-      <c r="L102" s="4"/>
+      <c r="L102" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="M102" s="4"/>
       <c r="N102" s="4"/>
       <c r="O102" s="4"/>
       <c r="P102" s="4"/>
       <c r="Q102" s="4"/>
       <c r="R102" s="3"/>
-      <c r="S102" s="4"/>
+      <c r="S102" s="2"/>
       <c r="T102" s="4"/>
     </row>
     <row r="103" spans="2:20" x14ac:dyDescent="0.3">
@@ -3200,18 +3242,22 @@
       <c r="E103" s="3"/>
       <c r="F103" s="4"/>
       <c r="G103" s="3"/>
-      <c r="H103" s="4"/>
+      <c r="H103" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="I103" s="3"/>
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
-      <c r="L103" s="4"/>
+      <c r="L103" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="M103" s="4"/>
       <c r="N103" s="4"/>
       <c r="O103" s="4"/>
       <c r="P103" s="4"/>
       <c r="Q103" s="4"/>
       <c r="R103" s="3"/>
-      <c r="S103" s="4"/>
+      <c r="S103" s="2"/>
       <c r="T103" s="4"/>
     </row>
     <row r="104" spans="2:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Docs: Drag to Move Controller
#22

+ 드래그 이동 컨트롤러 관련 문서 업데이트: CD, RS
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104A9263-6956-4325-8D27-BD2C98AB76A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD79749-08FC-4E96-8F3D-C2B200F04E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="145">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -568,13 +568,21 @@
   </si>
   <si>
     <t>FR-U-M-06.01.03</t>
+  </si>
+  <si>
+    <t>FR-C-A-03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임 오브젝트 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -589,8 +597,23 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,6 +635,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -661,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -669,6 +698,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -951,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D57" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U92" sqref="U92"/>
+    <sheetView tabSelected="1" topLeftCell="D61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q97" sqref="Q97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2058,9 +2090,13 @@
       <c r="E53" s="3"/>
       <c r="F53" s="4"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="4"/>
+      <c r="H53" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="I53" s="3"/>
-      <c r="J53" s="4"/>
+      <c r="J53" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
@@ -2069,7 +2105,7 @@
       <c r="P53" s="4"/>
       <c r="Q53" s="4"/>
       <c r="R53" s="3"/>
-      <c r="S53" s="4"/>
+      <c r="S53" s="1"/>
       <c r="T53" s="4"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.3">
@@ -2942,22 +2978,22 @@
       <c r="E91" s="3"/>
       <c r="F91" s="4"/>
       <c r="G91" s="3"/>
-      <c r="H91" s="4" t="s">
+      <c r="H91" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="I91" s="3"/>
-      <c r="J91" s="4"/>
-      <c r="K91" s="4" t="s">
+      <c r="I91" s="8"/>
+      <c r="J91" s="9"/>
+      <c r="K91" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="L91" s="4"/>
-      <c r="M91" s="4"/>
-      <c r="N91" s="4"/>
-      <c r="O91" s="4"/>
-      <c r="P91" s="4"/>
-      <c r="Q91" s="4"/>
-      <c r="R91" s="3"/>
-      <c r="S91" s="2"/>
+      <c r="L91" s="9"/>
+      <c r="M91" s="9"/>
+      <c r="N91" s="9"/>
+      <c r="O91" s="9"/>
+      <c r="P91" s="9"/>
+      <c r="Q91" s="9"/>
+      <c r="R91" s="8"/>
+      <c r="S91" s="9"/>
       <c r="T91" s="4"/>
     </row>
     <row r="92" spans="2:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Closes #22 Document/19 basic screen drawer (#24)
* Docs: Structure for Key Toggle Manager

#22

+ 전체 게임 내 키 토글을 제어하기 위한 키 ~ 함수 매핑식 키 토글 매니저 선언
+ 컨텐츠 모달 관련 문서 업데이트:: FC, RS, CD

* Docs: ContentModal for Grid

#22

+ 그리드 형식의 컨텐츠 모달 구상중: 6 * 8 기준

* Docs: Drag to Move Controller

#22

+ 드래그 이동 컨트롤러 관련 문서 업데이트: CD, RS

* Docs: Update DragToMoveController

#22

~ 문서 업데이트: CD
~ 박스 콜라이더의 크기 버그로 움직이지 않음
~ 박스 콜라이더 크기 반응형으로 전환

* Docs: Update CD for Modal Module

#22 #2

~ 문서 업데이트: CD
~ 그리드 모달 관련 클래스 다이어그램 계층 지향적 정리

* Docs: Update CD for Modal Module

#22 #2

~ 문서 업데이트: CD
~ 그리드 컨텐츠 콜백 함수 전달 로직 반영

* Docs: Update CD for Modal Module

#22 #2

+ 키토글 매니저를 위한 추상 클래스 반영

* Docs: Update CD

#22 #2

+ 토글 단축키 및 컨텐츠 모달 에디터에 귀속화
</commit_message>
<xml_diff>
--- a/documents/Requirement Specification.xlsx
+++ b/documents/Requirement Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\To-the-North-documents\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA5DCE3-9279-425E-A1E5-79DFB3687B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD79749-08FC-4E96-8F3D-C2B200F04E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8625" yWindow="2730" windowWidth="17925" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="145">
   <si>
     <t>Requirement Specification</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -428,6 +428,153 @@
   </si>
   <si>
     <t>마우스 커서 조건에 따라 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-04</t>
+  </si>
+  <si>
+    <t>FR-U-M-04.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-04.02</t>
+  </si>
+  <si>
+    <t>FR-U-M-04.03</t>
+  </si>
+  <si>
+    <t>FR-U-M-04.04</t>
+  </si>
+  <si>
+    <t>토글 함수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내부 컨텐츠 초기화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트래킹 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-04.05</t>
+  </si>
+  <si>
+    <t>FR-U-M-04.06</t>
+  </si>
+  <si>
+    <t>FR-U-M-04.07</t>
+  </si>
+  <si>
+    <t>토글 키 트래킹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 트래킹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 함수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-04.04.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-04.04.02</t>
+  </si>
+  <si>
+    <t>FR-U-M-05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-05.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨텐츠 초기화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-05.02</t>
+  </si>
+  <si>
+    <t>FR-U-M-05.03</t>
+  </si>
+  <si>
+    <t>FR-S-03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단축키 시스템</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-06.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨텐츠 모달 추상 클래스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[SerializeField] 기반 사이즈 초기화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내부 컨텐츠 적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초기 오브젝트 연결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-04.08</t>
+  </si>
+  <si>
+    <t>컨텐츠 모달용 VO 선언</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트용 컨텐츠 모달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임 오브젝트 연결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리드용 컨텐츠 모달 추상 클래스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리드용 컨텐츠 클래스: 단일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-06.01.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-U-M-06.01.02</t>
+  </si>
+  <si>
+    <t>FR-U-M-06.01.03</t>
+  </si>
+  <si>
+    <t>FR-C-A-03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임 오브젝트 이동</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -435,7 +582,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,8 +597,23 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,6 +635,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -522,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -530,6 +698,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -812,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32"/>
+    <sheetView tabSelected="1" topLeftCell="D61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q97" sqref="Q97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1048,9 +1219,13 @@
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="4"/>
+      <c r="J16" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -1059,7 +1234,7 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="4"/>
+      <c r="S16" s="1"/>
       <c r="T16" s="4"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.3">
@@ -1410,7 +1585,7 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="1"/>
+      <c r="S31" s="2"/>
       <c r="T31" s="4"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
@@ -1460,7 +1635,7 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="3"/>
-      <c r="S33" s="1"/>
+      <c r="S33" s="2"/>
       <c r="T33" s="4"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.3">
@@ -1535,7 +1710,7 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="3"/>
-      <c r="S36" s="1"/>
+      <c r="S36" s="2"/>
       <c r="T36" s="4"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.3">
@@ -1915,9 +2090,13 @@
       <c r="E53" s="3"/>
       <c r="F53" s="4"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="4"/>
+      <c r="H53" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="I53" s="3"/>
-      <c r="J53" s="4"/>
+      <c r="J53" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
@@ -1926,7 +2105,7 @@
       <c r="P53" s="4"/>
       <c r="Q53" s="4"/>
       <c r="R53" s="3"/>
-      <c r="S53" s="4"/>
+      <c r="S53" s="1"/>
       <c r="T53" s="4"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.3">
@@ -2620,9 +2799,13 @@
       <c r="E84" s="3"/>
       <c r="F84" s="4"/>
       <c r="G84" s="3"/>
-      <c r="H84" s="4"/>
+      <c r="H84" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="I84" s="3"/>
-      <c r="J84" s="4"/>
+      <c r="J84" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="K84" s="4"/>
       <c r="L84" s="4"/>
       <c r="M84" s="4"/>
@@ -2631,7 +2814,7 @@
       <c r="P84" s="4"/>
       <c r="Q84" s="4"/>
       <c r="R84" s="3"/>
-      <c r="S84" s="4"/>
+      <c r="S84" s="1"/>
       <c r="T84" s="4"/>
     </row>
     <row r="85" spans="2:20" x14ac:dyDescent="0.3">
@@ -2641,10 +2824,14 @@
       <c r="E85" s="3"/>
       <c r="F85" s="4"/>
       <c r="G85" s="3"/>
-      <c r="H85" s="4"/>
+      <c r="H85" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="I85" s="3"/>
       <c r="J85" s="4"/>
-      <c r="K85" s="4"/>
+      <c r="K85" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
       <c r="N85" s="4"/>
@@ -2652,7 +2839,7 @@
       <c r="P85" s="4"/>
       <c r="Q85" s="4"/>
       <c r="R85" s="3"/>
-      <c r="S85" s="4"/>
+      <c r="S85" s="1"/>
       <c r="T85" s="4"/>
     </row>
     <row r="86" spans="2:20" x14ac:dyDescent="0.3">
@@ -2662,10 +2849,14 @@
       <c r="E86" s="3"/>
       <c r="F86" s="4"/>
       <c r="G86" s="3"/>
-      <c r="H86" s="4"/>
+      <c r="H86" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="I86" s="3"/>
       <c r="J86" s="4"/>
-      <c r="K86" s="4"/>
+      <c r="K86" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
       <c r="N86" s="4"/>
@@ -2673,7 +2864,7 @@
       <c r="P86" s="4"/>
       <c r="Q86" s="4"/>
       <c r="R86" s="3"/>
-      <c r="S86" s="4"/>
+      <c r="S86" s="1"/>
       <c r="T86" s="4"/>
     </row>
     <row r="87" spans="2:20" x14ac:dyDescent="0.3">
@@ -2683,10 +2874,14 @@
       <c r="E87" s="3"/>
       <c r="F87" s="4"/>
       <c r="G87" s="3"/>
-      <c r="H87" s="4"/>
+      <c r="H87" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="I87" s="3"/>
       <c r="J87" s="4"/>
-      <c r="K87" s="4"/>
+      <c r="K87" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="L87" s="4"/>
       <c r="M87" s="4"/>
       <c r="N87" s="4"/>
@@ -2694,7 +2889,7 @@
       <c r="P87" s="4"/>
       <c r="Q87" s="4"/>
       <c r="R87" s="3"/>
-      <c r="S87" s="4"/>
+      <c r="S87" s="1"/>
       <c r="T87" s="4"/>
     </row>
     <row r="88" spans="2:20" x14ac:dyDescent="0.3">
@@ -2704,10 +2899,14 @@
       <c r="E88" s="3"/>
       <c r="F88" s="4"/>
       <c r="G88" s="3"/>
-      <c r="H88" s="4"/>
+      <c r="H88" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="I88" s="3"/>
       <c r="J88" s="4"/>
-      <c r="K88" s="4"/>
+      <c r="K88" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
       <c r="N88" s="4"/>
@@ -2715,7 +2914,7 @@
       <c r="P88" s="4"/>
       <c r="Q88" s="4"/>
       <c r="R88" s="3"/>
-      <c r="S88" s="4"/>
+      <c r="S88" s="1"/>
       <c r="T88" s="4"/>
     </row>
     <row r="89" spans="2:20" x14ac:dyDescent="0.3">
@@ -2725,18 +2924,22 @@
       <c r="E89" s="3"/>
       <c r="F89" s="4"/>
       <c r="G89" s="3"/>
-      <c r="H89" s="4"/>
+      <c r="H89" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="I89" s="3"/>
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
-      <c r="L89" s="4"/>
+      <c r="L89" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="M89" s="4"/>
       <c r="N89" s="4"/>
       <c r="O89" s="4"/>
       <c r="P89" s="4"/>
       <c r="Q89" s="4"/>
       <c r="R89" s="3"/>
-      <c r="S89" s="4"/>
+      <c r="S89" s="1"/>
       <c r="T89" s="4"/>
     </row>
     <row r="90" spans="2:20" x14ac:dyDescent="0.3">
@@ -2746,18 +2949,22 @@
       <c r="E90" s="3"/>
       <c r="F90" s="4"/>
       <c r="G90" s="3"/>
-      <c r="H90" s="4"/>
+      <c r="H90" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="I90" s="3"/>
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
-      <c r="L90" s="4"/>
+      <c r="L90" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="M90" s="4"/>
       <c r="N90" s="4"/>
       <c r="O90" s="4"/>
       <c r="P90" s="4"/>
       <c r="Q90" s="4"/>
       <c r="R90" s="3"/>
-      <c r="S90" s="4"/>
+      <c r="S90" s="1"/>
       <c r="T90" s="4"/>
     </row>
     <row r="91" spans="2:20" x14ac:dyDescent="0.3">
@@ -2769,26 +2976,24 @@
         <v>7</v>
       </c>
       <c r="E91" s="3"/>
-      <c r="F91" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="F91" s="4"/>
       <c r="G91" s="3"/>
-      <c r="H91" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I91" s="3"/>
-      <c r="J91" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="K91" s="4"/>
-      <c r="L91" s="4"/>
-      <c r="M91" s="4"/>
-      <c r="N91" s="4"/>
-      <c r="O91" s="4"/>
-      <c r="P91" s="4"/>
-      <c r="Q91" s="4"/>
-      <c r="R91" s="3"/>
-      <c r="S91" s="1"/>
+      <c r="H91" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I91" s="8"/>
+      <c r="J91" s="9"/>
+      <c r="K91" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="L91" s="9"/>
+      <c r="M91" s="9"/>
+      <c r="N91" s="9"/>
+      <c r="O91" s="9"/>
+      <c r="P91" s="9"/>
+      <c r="Q91" s="9"/>
+      <c r="R91" s="8"/>
+      <c r="S91" s="9"/>
       <c r="T91" s="4"/>
     </row>
     <row r="92" spans="2:20" x14ac:dyDescent="0.3">
@@ -2799,13 +3004,13 @@
       <c r="F92" s="4"/>
       <c r="G92" s="3"/>
       <c r="H92" s="4" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="I92" s="3"/>
-      <c r="J92" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="K92" s="4"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
       <c r="N92" s="4"/>
@@ -2823,10 +3028,14 @@
       <c r="E93" s="3"/>
       <c r="F93" s="4"/>
       <c r="G93" s="3"/>
-      <c r="H93" s="4"/>
+      <c r="H93" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="I93" s="3"/>
       <c r="J93" s="4"/>
-      <c r="K93" s="4"/>
+      <c r="K93" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
       <c r="N93" s="4"/>
@@ -2834,7 +3043,7 @@
       <c r="P93" s="4"/>
       <c r="Q93" s="4"/>
       <c r="R93" s="3"/>
-      <c r="S93" s="4"/>
+      <c r="S93" s="1"/>
       <c r="T93" s="4"/>
     </row>
     <row r="94" spans="2:20" x14ac:dyDescent="0.3">
@@ -2844,10 +3053,14 @@
       <c r="E94" s="3"/>
       <c r="F94" s="4"/>
       <c r="G94" s="3"/>
-      <c r="H94" s="4"/>
+      <c r="H94" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="I94" s="3"/>
       <c r="J94" s="4"/>
-      <c r="K94" s="4"/>
+      <c r="K94" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="L94" s="4"/>
       <c r="M94" s="4"/>
       <c r="N94" s="4"/>
@@ -2855,7 +3068,7 @@
       <c r="P94" s="4"/>
       <c r="Q94" s="4"/>
       <c r="R94" s="3"/>
-      <c r="S94" s="4"/>
+      <c r="S94" s="1"/>
       <c r="T94" s="4"/>
     </row>
     <row r="95" spans="2:20" x14ac:dyDescent="0.3">
@@ -2865,9 +3078,13 @@
       <c r="E95" s="3"/>
       <c r="F95" s="4"/>
       <c r="G95" s="3"/>
-      <c r="H95" s="4"/>
+      <c r="H95" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I95" s="3"/>
-      <c r="J95" s="4"/>
+      <c r="J95" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
       <c r="M95" s="4"/>
@@ -2876,7 +3093,7 @@
       <c r="P95" s="4"/>
       <c r="Q95" s="4"/>
       <c r="R95" s="3"/>
-      <c r="S95" s="4"/>
+      <c r="S95" s="1"/>
       <c r="T95" s="4"/>
     </row>
     <row r="96" spans="2:20" x14ac:dyDescent="0.3">
@@ -2886,10 +3103,14 @@
       <c r="E96" s="3"/>
       <c r="F96" s="4"/>
       <c r="G96" s="3"/>
-      <c r="H96" s="4"/>
+      <c r="H96" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="I96" s="3"/>
       <c r="J96" s="4"/>
-      <c r="K96" s="4"/>
+      <c r="K96" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="L96" s="4"/>
       <c r="M96" s="4"/>
       <c r="N96" s="4"/>
@@ -2897,7 +3118,7 @@
       <c r="P96" s="4"/>
       <c r="Q96" s="4"/>
       <c r="R96" s="3"/>
-      <c r="S96" s="4"/>
+      <c r="S96" s="1"/>
       <c r="T96" s="4"/>
     </row>
     <row r="97" spans="2:20" x14ac:dyDescent="0.3">
@@ -2907,10 +3128,14 @@
       <c r="E97" s="3"/>
       <c r="F97" s="4"/>
       <c r="G97" s="3"/>
-      <c r="H97" s="4"/>
+      <c r="H97" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="I97" s="3"/>
       <c r="J97" s="4"/>
-      <c r="K97" s="4"/>
+      <c r="K97" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="L97" s="4"/>
       <c r="M97" s="4"/>
       <c r="N97" s="4"/>
@@ -2918,7 +3143,7 @@
       <c r="P97" s="4"/>
       <c r="Q97" s="4"/>
       <c r="R97" s="3"/>
-      <c r="S97" s="4"/>
+      <c r="S97" s="1"/>
       <c r="T97" s="4"/>
     </row>
     <row r="98" spans="2:20" x14ac:dyDescent="0.3">
@@ -2928,10 +3153,14 @@
       <c r="E98" s="3"/>
       <c r="F98" s="4"/>
       <c r="G98" s="3"/>
-      <c r="H98" s="4"/>
+      <c r="H98" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="I98" s="3"/>
       <c r="J98" s="4"/>
-      <c r="K98" s="4"/>
+      <c r="K98" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="L98" s="4"/>
       <c r="M98" s="4"/>
       <c r="N98" s="4"/>
@@ -2939,7 +3168,7 @@
       <c r="P98" s="4"/>
       <c r="Q98" s="4"/>
       <c r="R98" s="3"/>
-      <c r="S98" s="4"/>
+      <c r="S98" s="1"/>
       <c r="T98" s="4"/>
     </row>
     <row r="99" spans="2:20" x14ac:dyDescent="0.3">
@@ -2949,9 +3178,13 @@
       <c r="E99" s="3"/>
       <c r="F99" s="4"/>
       <c r="G99" s="3"/>
-      <c r="H99" s="4"/>
+      <c r="H99" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="I99" s="3"/>
-      <c r="J99" s="4"/>
+      <c r="J99" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="K99" s="4"/>
       <c r="L99" s="4"/>
       <c r="M99" s="4"/>
@@ -2960,7 +3193,7 @@
       <c r="P99" s="4"/>
       <c r="Q99" s="4"/>
       <c r="R99" s="3"/>
-      <c r="S99" s="4"/>
+      <c r="S99" s="2"/>
       <c r="T99" s="4"/>
     </row>
     <row r="100" spans="2:20" x14ac:dyDescent="0.3">
@@ -2970,10 +3203,14 @@
       <c r="E100" s="3"/>
       <c r="F100" s="4"/>
       <c r="G100" s="3"/>
-      <c r="H100" s="4"/>
+      <c r="H100" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="I100" s="3"/>
       <c r="J100" s="4"/>
-      <c r="K100" s="4"/>
+      <c r="K100" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="L100" s="4"/>
       <c r="M100" s="4"/>
       <c r="N100" s="4"/>
@@ -2981,7 +3218,7 @@
       <c r="P100" s="4"/>
       <c r="Q100" s="4"/>
       <c r="R100" s="3"/>
-      <c r="S100" s="4"/>
+      <c r="S100" s="2"/>
       <c r="T100" s="4"/>
     </row>
     <row r="101" spans="2:20" x14ac:dyDescent="0.3">
@@ -2991,18 +3228,22 @@
       <c r="E101" s="3"/>
       <c r="F101" s="4"/>
       <c r="G101" s="3"/>
-      <c r="H101" s="4"/>
+      <c r="H101" s="4" t="s">
+        <v>140</v>
+      </c>
       <c r="I101" s="3"/>
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
-      <c r="L101" s="4"/>
+      <c r="L101" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="M101" s="4"/>
       <c r="N101" s="4"/>
       <c r="O101" s="4"/>
       <c r="P101" s="4"/>
       <c r="Q101" s="4"/>
       <c r="R101" s="3"/>
-      <c r="S101" s="4"/>
+      <c r="S101" s="2"/>
       <c r="T101" s="4"/>
     </row>
     <row r="102" spans="2:20" x14ac:dyDescent="0.3">
@@ -3012,18 +3253,22 @@
       <c r="E102" s="3"/>
       <c r="F102" s="4"/>
       <c r="G102" s="3"/>
-      <c r="H102" s="4"/>
+      <c r="H102" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="I102" s="3"/>
       <c r="J102" s="4"/>
       <c r="K102" s="4"/>
-      <c r="L102" s="4"/>
+      <c r="L102" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="M102" s="4"/>
       <c r="N102" s="4"/>
       <c r="O102" s="4"/>
       <c r="P102" s="4"/>
       <c r="Q102" s="4"/>
       <c r="R102" s="3"/>
-      <c r="S102" s="4"/>
+      <c r="S102" s="2"/>
       <c r="T102" s="4"/>
     </row>
     <row r="103" spans="2:20" x14ac:dyDescent="0.3">
@@ -3033,18 +3278,22 @@
       <c r="E103" s="3"/>
       <c r="F103" s="4"/>
       <c r="G103" s="3"/>
-      <c r="H103" s="4"/>
+      <c r="H103" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="I103" s="3"/>
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
-      <c r="L103" s="4"/>
+      <c r="L103" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="M103" s="4"/>
       <c r="N103" s="4"/>
       <c r="O103" s="4"/>
       <c r="P103" s="4"/>
       <c r="Q103" s="4"/>
       <c r="R103" s="3"/>
-      <c r="S103" s="4"/>
+      <c r="S103" s="2"/>
       <c r="T103" s="4"/>
     </row>
     <row r="104" spans="2:20" x14ac:dyDescent="0.3">
@@ -3094,11 +3343,17 @@
       <c r="C106" s="3"/>
       <c r="D106" s="4"/>
       <c r="E106" s="3"/>
-      <c r="F106" s="4"/>
+      <c r="F106" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="G106" s="3"/>
-      <c r="H106" s="4"/>
+      <c r="H106" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="I106" s="3"/>
-      <c r="J106" s="4"/>
+      <c r="J106" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="K106" s="4"/>
       <c r="L106" s="4"/>
       <c r="M106" s="4"/>
@@ -3107,7 +3362,7 @@
       <c r="P106" s="4"/>
       <c r="Q106" s="4"/>
       <c r="R106" s="3"/>
-      <c r="S106" s="4"/>
+      <c r="S106" s="1"/>
       <c r="T106" s="4"/>
     </row>
     <row r="107" spans="2:20" x14ac:dyDescent="0.3">
@@ -3117,9 +3372,13 @@
       <c r="E107" s="3"/>
       <c r="F107" s="4"/>
       <c r="G107" s="3"/>
-      <c r="H107" s="4"/>
+      <c r="H107" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="I107" s="3"/>
-      <c r="J107" s="4"/>
+      <c r="J107" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="K107" s="4"/>
       <c r="L107" s="4"/>
       <c r="M107" s="4"/>
@@ -3128,7 +3387,7 @@
       <c r="P107" s="4"/>
       <c r="Q107" s="4"/>
       <c r="R107" s="3"/>
-      <c r="S107" s="4"/>
+      <c r="S107" s="1"/>
       <c r="T107" s="4"/>
     </row>
     <row r="108" spans="2:20" x14ac:dyDescent="0.3">

</xml_diff>